<commit_message>
Incorporated separate ss for spouse
</commit_message>
<xml_diff>
--- a/test/TestCalculations.xlsx
+++ b/test/TestCalculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Year</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>IRA Savings</t>
+  </si>
+  <si>
+    <t>Spouse SS</t>
   </si>
 </sst>
 </file>
@@ -453,14 +456,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2595" ySplit="735" topLeftCell="B4" activePane="bottomLeft"/>
+      <pane xSplit="2595" ySplit="735" topLeftCell="F3" activePane="bottomLeft"/>
       <selection activeCell="A19" sqref="A19"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,1054 +784,1083 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K5">
-        <f>2900*12</f>
-        <v>34800</v>
-      </c>
-      <c r="L5">
-        <f>ROUND(K5*1.02,0)</f>
-        <v>35496</v>
-      </c>
-      <c r="M5">
-        <f t="shared" ref="M5:T5" si="12">ROUND(L5*1.02,0)</f>
-        <v>36206</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="12"/>
-        <v>36930</v>
-      </c>
       <c r="O5">
-        <f t="shared" si="12"/>
-        <v>37669</v>
+        <f>2400*12</f>
+        <v>28800</v>
       </c>
       <c r="P5">
-        <f t="shared" si="12"/>
-        <v>38422</v>
+        <f t="shared" ref="L5:T6" si="12">ROUND(O5*1.02,0)</f>
+        <v>29376</v>
       </c>
       <c r="Q5">
         <f t="shared" si="12"/>
-        <v>39190</v>
+        <v>29964</v>
       </c>
       <c r="R5">
         <f t="shared" si="12"/>
-        <v>39974</v>
+        <v>30563</v>
       </c>
       <c r="S5">
         <f t="shared" si="12"/>
-        <v>40773</v>
+        <v>31174</v>
       </c>
       <c r="T5">
         <f t="shared" si="12"/>
-        <v>41588</v>
+        <v>31797</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6">
+        <f>1300*12</f>
+        <v>15600</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="12"/>
+        <v>15912</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6" si="13">ROUND(L6*1.02,0)</f>
+        <v>16230</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6" si="14">ROUND(M6*1.02,0)</f>
+        <v>16555</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6" si="15">ROUND(N6*1.02,0)</f>
+        <v>16886</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6" si="16">ROUND(O6*1.02,0)</f>
+        <v>17224</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6" si="17">ROUND(P6*1.02,0)</f>
+        <v>17568</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6" si="18">ROUND(Q6*1.02,0)</f>
+        <v>17919</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6" si="19">ROUND(R6*1.02,0)</f>
+        <v>18277</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ref="T6" si="20">ROUND(S6*1.02,0)</f>
+        <v>18643</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <f>250*12</f>
         <v>3000</v>
       </c>
-      <c r="H6">
-        <f>ROUND(G6*1.015,0)</f>
+      <c r="H7">
+        <f>ROUND(G7*1.015,0)</f>
         <v>3045</v>
       </c>
-      <c r="I6">
-        <f t="shared" ref="I6:S6" si="13">ROUND(H6*1.015,0)</f>
+      <c r="I7">
+        <f t="shared" ref="I7:S7" si="21">ROUND(H7*1.015,0)</f>
         <v>3091</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="13"/>
+      <c r="J7">
+        <f t="shared" si="21"/>
         <v>3137</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="13"/>
+      <c r="K7">
+        <f t="shared" si="21"/>
         <v>3184</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="13"/>
+      <c r="L7">
+        <f t="shared" si="21"/>
         <v>3232</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="13"/>
+      <c r="M7">
+        <f t="shared" si="21"/>
         <v>3280</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="13"/>
+      <c r="N7">
+        <f t="shared" si="21"/>
         <v>3329</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="13"/>
+      <c r="O7">
+        <f t="shared" si="21"/>
         <v>3379</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="13"/>
+      <c r="P7">
+        <f t="shared" si="21"/>
         <v>3430</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="13"/>
+      <c r="Q7">
+        <f t="shared" si="21"/>
         <v>3481</v>
       </c>
-      <c r="R6">
-        <f t="shared" si="13"/>
+      <c r="R7">
+        <f t="shared" si="21"/>
         <v>3533</v>
       </c>
-      <c r="S6">
-        <f t="shared" si="13"/>
+      <c r="S7">
+        <f t="shared" si="21"/>
         <v>3586</v>
       </c>
-      <c r="T6">
-        <f>ROUND(S6*1.015,0)</f>
+      <c r="T7">
+        <f>ROUND(S7*1.015,0)</f>
         <v>3640</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <f>400*12</f>
         <v>4800</v>
       </c>
-      <c r="I7">
-        <f t="shared" ref="I7:T7" si="14">ROUND(H7*1.01,0)</f>
+      <c r="I8">
+        <f t="shared" ref="I8:T8" si="22">ROUND(H8*1.01,0)</f>
         <v>4848</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="14"/>
+      <c r="J8">
+        <f t="shared" si="22"/>
         <v>4896</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="14"/>
+      <c r="K8">
+        <f t="shared" si="22"/>
         <v>4945</v>
       </c>
-      <c r="L7">
-        <f t="shared" si="14"/>
+      <c r="L8">
+        <f t="shared" si="22"/>
         <v>4994</v>
       </c>
-      <c r="M7">
-        <f t="shared" si="14"/>
+      <c r="M8">
+        <f t="shared" si="22"/>
         <v>5044</v>
       </c>
-      <c r="N7">
-        <f t="shared" si="14"/>
+      <c r="N8">
+        <f t="shared" si="22"/>
         <v>5094</v>
       </c>
-      <c r="O7">
-        <f t="shared" si="14"/>
+      <c r="O8">
+        <f t="shared" si="22"/>
         <v>5145</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="14"/>
+      <c r="P8">
+        <f t="shared" si="22"/>
         <v>5196</v>
       </c>
-      <c r="Q7">
-        <f t="shared" si="14"/>
+      <c r="Q8">
+        <f t="shared" si="22"/>
         <v>5248</v>
       </c>
-      <c r="R7">
-        <f t="shared" si="14"/>
+      <c r="R8">
+        <f t="shared" si="22"/>
         <v>5300</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="14"/>
+      <c r="S8">
+        <f t="shared" si="22"/>
         <v>5353</v>
       </c>
-      <c r="T7">
-        <f t="shared" si="14"/>
+      <c r="T8">
+        <f t="shared" si="22"/>
         <v>5407</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8">
-        <v>9000</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <f>SUM(B3:B7)</f>
+      <c r="B10">
+        <f>SUM(B3:B8)</f>
         <v>105000</v>
       </c>
-      <c r="C9">
-        <f t="shared" ref="C9:S9" si="15">SUM(C3:C7)</f>
+      <c r="C10">
+        <f t="shared" ref="C10:S10" si="23">SUM(C3:C8)</f>
         <v>105000</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="15"/>
+      <c r="D10">
+        <f t="shared" si="23"/>
         <v>105000</v>
       </c>
-      <c r="E9">
-        <f>SUM(E3:E8)</f>
+      <c r="E10">
+        <f>SUM(E3:E9)</f>
         <v>153600</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="15"/>
+      <c r="F10">
+        <f t="shared" si="23"/>
         <v>110392</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="15"/>
+      <c r="G10">
+        <f t="shared" si="23"/>
         <v>114200</v>
       </c>
-      <c r="H9">
-        <f>SUM(H3:H7)</f>
+      <c r="H10">
+        <f>SUM(H3:H8)</f>
         <v>49869</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="15"/>
+      <c r="I10">
+        <f t="shared" si="23"/>
         <v>50803</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="15"/>
+      <c r="J10">
+        <f t="shared" si="23"/>
         <v>51754</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="15"/>
-        <v>87524</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="15"/>
-        <v>89209</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="15"/>
-        <v>90927</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="15"/>
-        <v>92678</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="15"/>
-        <v>94465</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="15"/>
-        <v>96285</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="15"/>
-        <v>98141</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="15"/>
-        <v>100033</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="15"/>
-        <v>101963</v>
-      </c>
-      <c r="T9">
-        <f>SUM(T3:T7)</f>
-        <v>103931</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="K10">
+        <f t="shared" si="23"/>
+        <v>68324</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="23"/>
+        <v>69625</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="23"/>
+        <v>70951</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="23"/>
+        <v>72303</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="23"/>
+        <v>102482</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="23"/>
+        <v>104463</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="23"/>
+        <v>106483</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="23"/>
+        <v>108541</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="23"/>
+        <v>110641</v>
+      </c>
+      <c r="T10">
+        <f>SUM(T3:T8)</f>
+        <v>112783</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <f t="shared" ref="B11:C11" si="16">B9-B19</f>
-        <v>105000</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="16"/>
-        <v>105000</v>
-      </c>
-      <c r="D11">
-        <f>D9-D19</f>
-        <v>105000</v>
-      </c>
-      <c r="E11">
-        <f t="shared" ref="E11:T11" si="17">E9-E19</f>
-        <v>153600</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="17"/>
-        <v>110392</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="17"/>
-        <v>114200</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="17"/>
-        <v>106010</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="17"/>
-        <v>110180</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="17"/>
-        <v>113355</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="17"/>
-        <v>117911</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="17"/>
-        <v>122695</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="17"/>
-        <v>127723</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="17"/>
-        <v>133009</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="17"/>
-        <v>138571</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="17"/>
-        <v>130025</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="17"/>
-        <v>135758</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="17"/>
-        <v>141809</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="17"/>
-        <v>148201</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="17"/>
-        <v>154955</v>
-      </c>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:C12" si="24">B10-B20</f>
+        <v>105000</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="24"/>
+        <v>105000</v>
+      </c>
+      <c r="D12">
+        <f>D10-D20</f>
+        <v>105000</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:T12" si="25">E10-E20</f>
+        <v>153600</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="25"/>
+        <v>110392</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="25"/>
+        <v>114200</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="25"/>
+        <v>106010</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="25"/>
+        <v>110180</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="25"/>
+        <v>113355</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="25"/>
+        <v>117911</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="25"/>
+        <v>122695</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="25"/>
+        <v>127723</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="25"/>
+        <v>133009</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="25"/>
+        <v>138571</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="25"/>
+        <v>130025</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="25"/>
+        <v>135758</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="25"/>
+        <v>141809</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="25"/>
+        <v>148201</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="25"/>
+        <v>154955</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
-        <f>ROUND((9500 + 0.25*(B11- 88000) + B3 * 0.0765),0)</f>
+      <c r="B13">
+        <f>ROUND((9500 + 0.25*(B12- 88000) + B3 * 0.0765),0)</f>
         <v>21783</v>
       </c>
-      <c r="C12">
-        <f>ROUND((9500 + 0.25*(C11 - 88000) + C3 * 0.0765),0)</f>
+      <c r="C13">
+        <f>ROUND((9500 + 0.25*(C12 - 88000) + C3 * 0.0765),0)</f>
         <v>21783</v>
       </c>
-      <c r="D12">
-        <f>ROUND((9500 + 0.25*(D11- 88000) + D3 * 0.0765),0)</f>
+      <c r="D13">
+        <f>ROUND((9500 + 0.25*(D12- 88000) + D3 * 0.0765),0)</f>
         <v>21783</v>
       </c>
-      <c r="E12">
-        <f>ROUND((9500 + 0.25*(E11-E8+$B$25-88000) + E3 * 0.0765),0)</f>
+      <c r="E13">
+        <f>ROUND((9500 + 0.25*(E12-E9+$B$26-88000) + E3 * 0.0765),0)</f>
         <v>35433</v>
       </c>
-      <c r="F12">
-        <f t="shared" ref="F12:T12" si="18">ROUND((9500 + 0.25*(F11+$B$25- 88000) + F3 * 0.0765),0)</f>
+      <c r="F13">
+        <f t="shared" ref="F13:T13" si="26">ROUND((9500 + 0.25*(F12+$B$26- 88000) + F3 * 0.0765),0)</f>
         <v>24203</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="18"/>
+      <c r="G13">
+        <f t="shared" si="26"/>
         <v>25155</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="18"/>
+      <c r="H13">
+        <f t="shared" si="26"/>
         <v>17753</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="18"/>
+      <c r="I13">
+        <f t="shared" si="26"/>
         <v>18795</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="18"/>
+      <c r="J13">
+        <f t="shared" si="26"/>
         <v>19589</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="18"/>
+      <c r="K13">
+        <f t="shared" si="26"/>
         <v>20728</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="18"/>
+      <c r="L13">
+        <f t="shared" si="26"/>
         <v>21924</v>
       </c>
-      <c r="M12">
-        <f t="shared" si="18"/>
+      <c r="M13">
+        <f t="shared" si="26"/>
         <v>23181</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="18"/>
+      <c r="N13">
+        <f t="shared" si="26"/>
         <v>24502</v>
       </c>
-      <c r="O12">
-        <f t="shared" si="18"/>
+      <c r="O13">
+        <f t="shared" si="26"/>
         <v>25893</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="18"/>
+      <c r="P13">
+        <f t="shared" si="26"/>
         <v>23756</v>
       </c>
-      <c r="Q12">
-        <f t="shared" si="18"/>
+      <c r="Q13">
+        <f t="shared" si="26"/>
         <v>25190</v>
       </c>
-      <c r="R12">
-        <f t="shared" si="18"/>
+      <c r="R13">
+        <f t="shared" si="26"/>
         <v>26702</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="18"/>
+      <c r="S13">
+        <f t="shared" si="26"/>
         <v>28300</v>
       </c>
-      <c r="T12">
-        <f t="shared" si="18"/>
+      <c r="T13">
+        <f t="shared" si="26"/>
         <v>29989</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>72200</v>
-      </c>
-      <c r="C14">
-        <f>ROUND(B14*1.03,0)</f>
-        <v>74366</v>
-      </c>
-      <c r="D14">
-        <f>ROUND(C14*1.03,0)</f>
-        <v>76597</v>
-      </c>
-      <c r="E14">
-        <f>ROUND(D14*1.03,0)</f>
-        <v>78895</v>
-      </c>
-      <c r="F14">
-        <f t="shared" ref="F14:L14" si="19">ROUND(E14*1.03,0)</f>
-        <v>81262</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="19"/>
-        <v>83700</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="19"/>
-        <v>86211</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="19"/>
-        <v>88797</v>
-      </c>
-      <c r="J14">
-        <f>ROUND(I14*1.03,0)-1200</f>
-        <v>90261</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="19"/>
-        <v>92969</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="19"/>
-        <v>95758</v>
-      </c>
-      <c r="M14">
-        <f t="shared" ref="M14" si="20">ROUND(L14*1.03,0)</f>
-        <v>98631</v>
-      </c>
-      <c r="N14">
-        <f t="shared" ref="N14" si="21">ROUND(M14*1.03,0)</f>
-        <v>101590</v>
-      </c>
-      <c r="O14">
-        <f t="shared" ref="O14" si="22">ROUND(N14*1.03,0)</f>
-        <v>104638</v>
-      </c>
-      <c r="P14">
-        <f>ROUND(O14*1.03,0)-(1200*12)</f>
-        <v>93377</v>
-      </c>
-      <c r="Q14">
-        <f>ROUND(P14*1.03,0)</f>
-        <v>96178</v>
-      </c>
-      <c r="R14">
-        <f>ROUND(Q14*1.03,0)</f>
-        <v>99063</v>
-      </c>
-      <c r="S14">
-        <f>ROUND(R14*1.03,0)</f>
-        <v>102035</v>
-      </c>
-      <c r="T14">
-        <f>ROUND(S14*1.03,0)</f>
-        <v>105096</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>12000</v>
+        <v>72200</v>
       </c>
       <c r="C15">
-        <f>ROUND(B15*1.08,0)</f>
-        <v>12960</v>
+        <f>ROUND(B15*1.03,0)</f>
+        <v>74366</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:L15" si="23">ROUND(C15*1.08,0)</f>
-        <v>13997</v>
+        <f>ROUND(C15*1.03,0)</f>
+        <v>76597</v>
       </c>
       <c r="E15">
-        <f>ROUND(D15*1.08,0) + 600</f>
-        <v>15717</v>
+        <f>ROUND(D15*1.03,0)</f>
+        <v>78895</v>
       </c>
       <c r="F15">
-        <f t="shared" si="23"/>
-        <v>16974</v>
+        <f t="shared" ref="F15:L15" si="27">ROUND(E15*1.03,0)</f>
+        <v>81262</v>
       </c>
       <c r="G15">
-        <f t="shared" si="23"/>
-        <v>18332</v>
+        <f t="shared" si="27"/>
+        <v>83700</v>
       </c>
       <c r="H15">
-        <f t="shared" si="23"/>
-        <v>19799</v>
+        <f t="shared" si="27"/>
+        <v>86211</v>
       </c>
       <c r="I15">
-        <f t="shared" si="23"/>
-        <v>21383</v>
+        <f t="shared" si="27"/>
+        <v>88797</v>
       </c>
       <c r="J15">
-        <f t="shared" si="23"/>
-        <v>23094</v>
+        <f>ROUND(I15*1.03,0)-1200</f>
+        <v>90261</v>
       </c>
       <c r="K15">
-        <f t="shared" si="23"/>
-        <v>24942</v>
+        <f t="shared" si="27"/>
+        <v>92969</v>
       </c>
       <c r="L15">
-        <f t="shared" si="23"/>
-        <v>26937</v>
+        <f t="shared" si="27"/>
+        <v>95758</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15" si="24">ROUND(L15*1.08,0)</f>
-        <v>29092</v>
+        <f t="shared" ref="M15" si="28">ROUND(L15*1.03,0)</f>
+        <v>98631</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15" si="25">ROUND(M15*1.08,0)</f>
-        <v>31419</v>
+        <f t="shared" ref="N15" si="29">ROUND(M15*1.03,0)</f>
+        <v>101590</v>
       </c>
       <c r="O15">
-        <f t="shared" ref="O15" si="26">ROUND(N15*1.08,0)</f>
-        <v>33933</v>
+        <f t="shared" ref="O15" si="30">ROUND(N15*1.03,0)</f>
+        <v>104638</v>
       </c>
       <c r="P15">
-        <f t="shared" ref="P15" si="27">ROUND(O15*1.08,0)</f>
-        <v>36648</v>
+        <f>ROUND(O15*1.03,0)-(1200*12)</f>
+        <v>93377</v>
       </c>
       <c r="Q15">
-        <f t="shared" ref="Q15" si="28">ROUND(P15*1.08,0)</f>
-        <v>39580</v>
+        <f>ROUND(P15*1.03,0)</f>
+        <v>96178</v>
       </c>
       <c r="R15">
-        <f t="shared" ref="R15" si="29">ROUND(Q15*1.08,0)</f>
-        <v>42746</v>
+        <f>ROUND(Q15*1.03,0)</f>
+        <v>99063</v>
       </c>
       <c r="S15">
-        <f t="shared" ref="S15:T15" si="30">ROUND(R15*1.08,0)</f>
-        <v>46166</v>
+        <f>ROUND(R15*1.03,0)</f>
+        <v>102035</v>
       </c>
       <c r="T15">
-        <f t="shared" si="30"/>
-        <v>49859</v>
+        <f>ROUND(S15*1.03,0)</f>
+        <v>105096</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>12000</v>
+      </c>
+      <c r="C16">
+        <f>ROUND(B16*1.08,0)</f>
+        <v>12960</v>
       </c>
       <c r="D16">
-        <v>8000</v>
+        <f t="shared" ref="D16:L16" si="31">ROUND(C16*1.08,0)</f>
+        <v>13997</v>
+      </c>
+      <c r="E16">
+        <f>ROUND(D16*1.08,0) + 600</f>
+        <v>15717</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="31"/>
+        <v>16974</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="31"/>
+        <v>18332</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="31"/>
+        <v>19799</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="31"/>
+        <v>21383</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="31"/>
+        <v>23094</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="31"/>
+        <v>24942</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="31"/>
+        <v>26937</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16" si="32">ROUND(L16*1.08,0)</f>
+        <v>29092</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ref="N16" si="33">ROUND(M16*1.08,0)</f>
+        <v>31419</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ref="O16" si="34">ROUND(N16*1.08,0)</f>
+        <v>33933</v>
+      </c>
+      <c r="P16">
+        <f t="shared" ref="P16" si="35">ROUND(O16*1.08,0)</f>
+        <v>36648</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ref="Q16" si="36">ROUND(P16*1.08,0)</f>
+        <v>39580</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ref="R16" si="37">ROUND(Q16*1.08,0)</f>
+        <v>42746</v>
+      </c>
+      <c r="S16">
+        <f t="shared" ref="S16:T16" si="38">ROUND(R16*1.08,0)</f>
+        <v>46166</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="38"/>
+        <v>49859</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17">
-        <f>(B14+B15)</f>
+      <c r="B18">
+        <f>(B15+B16)</f>
         <v>84200</v>
       </c>
-      <c r="C17">
-        <f t="shared" ref="C17:S17" si="31">(C14+C15)</f>
+      <c r="C18">
+        <f t="shared" ref="C18:S18" si="39">(C15+C16)</f>
         <v>87326</v>
       </c>
-      <c r="D17">
-        <f>(D14+D15+D16)</f>
+      <c r="D18">
+        <f>(D15+D16+D17)</f>
         <v>98594</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="31"/>
+      <c r="E18">
+        <f t="shared" si="39"/>
         <v>94612</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="31"/>
+      <c r="F18">
+        <f t="shared" si="39"/>
         <v>98236</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="31"/>
+      <c r="G18">
+        <f t="shared" si="39"/>
         <v>102032</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="31"/>
+      <c r="H18">
+        <f t="shared" si="39"/>
         <v>106010</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="31"/>
+      <c r="I18">
+        <f t="shared" si="39"/>
         <v>110180</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="31"/>
+      <c r="J18">
+        <f t="shared" si="39"/>
         <v>113355</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="31"/>
+      <c r="K18">
+        <f t="shared" si="39"/>
         <v>117911</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="31"/>
+      <c r="L18">
+        <f t="shared" si="39"/>
         <v>122695</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="31"/>
+      <c r="M18">
+        <f t="shared" si="39"/>
         <v>127723</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="31"/>
+      <c r="N18">
+        <f t="shared" si="39"/>
         <v>133009</v>
       </c>
-      <c r="O17">
-        <f t="shared" si="31"/>
+      <c r="O18">
+        <f t="shared" si="39"/>
         <v>138571</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="31"/>
+      <c r="P18">
+        <f t="shared" si="39"/>
         <v>130025</v>
       </c>
-      <c r="Q17">
-        <f t="shared" si="31"/>
+      <c r="Q18">
+        <f t="shared" si="39"/>
         <v>135758</v>
       </c>
-      <c r="R17">
-        <f t="shared" si="31"/>
+      <c r="R18">
+        <f t="shared" si="39"/>
         <v>141809</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="31"/>
+      <c r="S18">
+        <f t="shared" si="39"/>
         <v>148201</v>
       </c>
-      <c r="T17">
-        <f t="shared" ref="T17" si="32">(T14+T15)</f>
+      <c r="T18">
+        <f t="shared" ref="T18" si="40">(T15+T16)</f>
         <v>154955</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-    </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ref="H19:T19" si="33">H9-H17</f>
-        <v>-56141</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="33"/>
-        <v>-59377</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="33"/>
-        <v>-61601</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="33"/>
-        <v>-30387</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="33"/>
-        <v>-33486</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="33"/>
-        <v>-36796</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="33"/>
-        <v>-40331</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="33"/>
-        <v>-44106</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="33"/>
-        <v>-33740</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="33"/>
-        <v>-37617</v>
-      </c>
-      <c r="R19">
-        <f t="shared" si="33"/>
-        <v>-41776</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="33"/>
-        <v>-46238</v>
-      </c>
-      <c r="T19">
-        <f t="shared" si="33"/>
-        <v>-51024</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:T20" si="41">H10-H18</f>
+        <v>-56141</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="41"/>
+        <v>-59377</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="41"/>
+        <v>-61601</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="41"/>
+        <v>-49587</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="41"/>
+        <v>-53070</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="41"/>
+        <v>-56772</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="41"/>
+        <v>-60706</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="41"/>
+        <v>-36089</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="41"/>
+        <v>-25562</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="41"/>
+        <v>-29275</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="41"/>
+        <v>-33268</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="41"/>
+        <v>-37560</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="41"/>
+        <v>-42172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B20">
-        <f>B9-B12-B17</f>
+      <c r="B21">
+        <f>B10-B13-B18</f>
         <v>-983</v>
       </c>
-      <c r="C20">
-        <f>C9-C12-C17</f>
+      <c r="C21">
+        <f>C10-C13-C18</f>
         <v>-4109</v>
       </c>
-      <c r="D20">
-        <f>D9-D12-D17</f>
+      <c r="D21">
+        <f>D10-D13-D18</f>
         <v>-15377</v>
       </c>
-      <c r="E20">
-        <f>E9-E12-E17</f>
+      <c r="E21">
+        <f>E10-E13-E18</f>
         <v>23555</v>
       </c>
-      <c r="F20">
-        <f t="shared" ref="F20:G20" si="34">F9-F12-F17</f>
+      <c r="F21">
+        <f t="shared" ref="F21:G21" si="42">F10-F13-F18</f>
         <v>-12047</v>
       </c>
-      <c r="G20">
-        <f t="shared" si="34"/>
+      <c r="G21">
+        <f t="shared" si="42"/>
         <v>-12987</v>
       </c>
-      <c r="H20">
-        <f>-H12</f>
+      <c r="H21">
+        <f>-H13</f>
         <v>-17753</v>
       </c>
-      <c r="I20">
-        <f t="shared" ref="I20:T20" si="35">-I12</f>
+      <c r="I21">
+        <f t="shared" ref="I21:T21" si="43">-I13</f>
         <v>-18795</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="35"/>
+      <c r="J21">
+        <f t="shared" si="43"/>
         <v>-19589</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="35"/>
+      <c r="K21">
+        <f t="shared" si="43"/>
         <v>-20728</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="35"/>
+      <c r="L21">
+        <f t="shared" si="43"/>
         <v>-21924</v>
       </c>
-      <c r="M20">
-        <f t="shared" si="35"/>
+      <c r="M21">
+        <f t="shared" si="43"/>
         <v>-23181</v>
       </c>
-      <c r="N20">
-        <f t="shared" si="35"/>
+      <c r="N21">
+        <f t="shared" si="43"/>
         <v>-24502</v>
       </c>
-      <c r="O20">
-        <f t="shared" si="35"/>
+      <c r="O21">
+        <f t="shared" si="43"/>
         <v>-25893</v>
       </c>
-      <c r="P20">
-        <f t="shared" si="35"/>
+      <c r="P21">
+        <f t="shared" si="43"/>
         <v>-23756</v>
       </c>
-      <c r="Q20">
-        <f t="shared" si="35"/>
+      <c r="Q21">
+        <f t="shared" si="43"/>
         <v>-25190</v>
       </c>
-      <c r="R20">
-        <f t="shared" si="35"/>
+      <c r="R21">
+        <f t="shared" si="43"/>
         <v>-26702</v>
       </c>
-      <c r="S20">
-        <f t="shared" si="35"/>
+      <c r="S21">
+        <f t="shared" si="43"/>
         <v>-28300</v>
       </c>
-      <c r="T20">
-        <f t="shared" si="35"/>
+      <c r="T21">
+        <f t="shared" si="43"/>
         <v>-29989</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22">
-        <f>ROUND((600000+B19)*1.025,0)</f>
-        <v>615000</v>
-      </c>
-      <c r="C22">
-        <f>ROUND((B22+C19)*1.025,0)</f>
-        <v>630375</v>
-      </c>
-      <c r="D22">
-        <f>ROUND((C22+D19)*1.025,0)</f>
-        <v>646134</v>
-      </c>
-      <c r="E22">
-        <f t="shared" ref="E22:T22" si="36">ROUND((D22-$B$25+E19)*1.025,0)</f>
-        <v>646912</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="36"/>
-        <v>647710</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="36"/>
-        <v>648528</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="36"/>
-        <v>591822</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="36"/>
-        <v>530381</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="36"/>
-        <v>465125</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="36"/>
-        <v>430231</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="36"/>
-        <v>391289</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="36"/>
-        <v>347980</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="36"/>
-        <v>299965</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="36"/>
-        <v>246880</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="36"/>
-        <v>203094</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="36"/>
-        <v>154239</v>
-      </c>
-      <c r="R22">
-        <f t="shared" si="36"/>
-        <v>99900</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="36"/>
-        <v>39629</v>
-      </c>
-      <c r="T22">
-        <f t="shared" si="36"/>
-        <v>-27055</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B23">
-        <f>ROUND((60000+B20)*1.025,0)</f>
-        <v>60492</v>
+        <f>ROUND((600000+B20)*1.025,0)</f>
+        <v>615000</v>
       </c>
       <c r="C23">
         <f>ROUND((B23+C20)*1.025,0)</f>
-        <v>57793</v>
+        <v>630375</v>
       </c>
       <c r="D23">
         <f>ROUND((C23+D20)*1.025,0)</f>
+        <v>646134</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:T23" si="44">ROUND((D23-$B$26+E20)*1.025,0)</f>
+        <v>646912</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="44"/>
+        <v>647710</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="44"/>
+        <v>648528</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="44"/>
+        <v>591822</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="44"/>
+        <v>530381</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="44"/>
+        <v>465125</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="44"/>
+        <v>410551</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="44"/>
+        <v>351043</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="44"/>
+        <v>286253</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="44"/>
+        <v>215811</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="44"/>
+        <v>168840</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="44"/>
+        <v>131485</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="44"/>
+        <v>89390</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="44"/>
+        <v>42150</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="44"/>
+        <v>-10670</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="44"/>
+        <v>-69538</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <f>ROUND((60000+B21)*1.025,0)</f>
+        <v>60492</v>
+      </c>
+      <c r="C24">
+        <f>ROUND((B24+C21)*1.025,0)</f>
+        <v>57793</v>
+      </c>
+      <c r="D24">
+        <f>ROUND((C24+D21)*1.025,0)</f>
         <v>43476</v>
       </c>
-      <c r="E23">
-        <f t="shared" ref="E23:T23" si="37">ROUND((D23+E20 + $B$25)*1.025,0)</f>
+      <c r="E24">
+        <f t="shared" ref="E24:T24" si="45">ROUND((D24+E21 + $B$26)*1.025,0)</f>
         <v>84082</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="37"/>
+      <c r="F24">
+        <f t="shared" si="45"/>
         <v>89211</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="37"/>
+      <c r="G24">
+        <f t="shared" si="45"/>
         <v>93505</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="37"/>
+      <c r="H24">
+        <f t="shared" si="45"/>
         <v>93021</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="37"/>
+      <c r="I24">
+        <f t="shared" si="45"/>
         <v>91457</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="37"/>
+      <c r="J24">
+        <f t="shared" si="45"/>
         <v>89040</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="37"/>
+      <c r="K24">
+        <f t="shared" si="45"/>
         <v>85395</v>
       </c>
-      <c r="L23">
-        <f t="shared" si="37"/>
+      <c r="L24">
+        <f t="shared" si="45"/>
         <v>80433</v>
       </c>
-      <c r="M23">
-        <f t="shared" si="37"/>
+      <c r="M24">
+        <f t="shared" si="45"/>
         <v>74058</v>
       </c>
-      <c r="N23">
-        <f t="shared" si="37"/>
+      <c r="N24">
+        <f t="shared" si="45"/>
         <v>66170</v>
       </c>
-      <c r="O23">
-        <f t="shared" si="37"/>
+      <c r="O24">
+        <f t="shared" si="45"/>
         <v>56659</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="37"/>
+      <c r="P24">
+        <f t="shared" si="45"/>
         <v>49101</v>
       </c>
-      <c r="Q23">
-        <f t="shared" si="37"/>
+      <c r="Q24">
+        <f t="shared" si="45"/>
         <v>39884</v>
       </c>
-      <c r="R23">
-        <f t="shared" si="37"/>
+      <c r="R24">
+        <f t="shared" si="45"/>
         <v>28887</v>
       </c>
-      <c r="S23">
-        <f t="shared" si="37"/>
+      <c r="S24">
+        <f t="shared" si="45"/>
         <v>15977</v>
       </c>
-      <c r="T23">
-        <f t="shared" si="37"/>
+      <c r="T24">
+        <f t="shared" si="45"/>
         <v>1013</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-    </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>15000</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
partial_first_year: Modified spread sheet and tests to fail
</commit_message>
<xml_diff>
--- a/test/TestCalculations.xlsx
+++ b/test/TestCalculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Year</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Spouse SS</t>
+  </si>
+  <si>
+    <t>Starting month</t>
+  </si>
+  <si>
+    <t>April</t>
   </si>
 </sst>
 </file>
@@ -456,14 +462,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2595" ySplit="735" topLeftCell="F3" activePane="bottomLeft"/>
+      <pane xSplit="2595" ySplit="735" activePane="bottomRight"/>
       <selection activeCell="A19" sqref="A19"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD28"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,11 +642,11 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <f>70*1500</f>
-        <v>105000</v>
+        <f>70*1500*C27</f>
+        <v>78750</v>
       </c>
       <c r="C3">
-        <f>B3</f>
+        <f>B3/C27</f>
         <v>105000</v>
       </c>
       <c r="D3">
@@ -986,7 +992,7 @@
       </c>
       <c r="B10">
         <f>SUM(B3:B8)</f>
-        <v>105000</v>
+        <v>78750</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:S10" si="23">SUM(C3:C8)</f>
@@ -1070,7 +1076,7 @@
       </c>
       <c r="B12">
         <f t="shared" ref="B12:C12" si="24">B10-B20</f>
-        <v>105000</v>
+        <v>78750</v>
       </c>
       <c r="C12">
         <f t="shared" si="24"/>
@@ -1094,55 +1100,55 @@
       </c>
       <c r="H12">
         <f t="shared" si="25"/>
-        <v>106010</v>
+        <v>105771</v>
       </c>
       <c r="I12">
         <f t="shared" si="25"/>
-        <v>110180</v>
+        <v>109934</v>
       </c>
       <c r="J12">
         <f t="shared" si="25"/>
-        <v>113355</v>
+        <v>113102</v>
       </c>
       <c r="K12">
         <f t="shared" si="25"/>
-        <v>117911</v>
+        <v>117650</v>
       </c>
       <c r="L12">
         <f t="shared" si="25"/>
-        <v>122695</v>
+        <v>122426</v>
       </c>
       <c r="M12">
         <f t="shared" si="25"/>
-        <v>127723</v>
+        <v>127446</v>
       </c>
       <c r="N12">
         <f t="shared" si="25"/>
-        <v>133009</v>
+        <v>132724</v>
       </c>
       <c r="O12">
         <f t="shared" si="25"/>
-        <v>138571</v>
+        <v>138277</v>
       </c>
       <c r="P12">
         <f t="shared" si="25"/>
-        <v>130025</v>
+        <v>129722</v>
       </c>
       <c r="Q12">
         <f t="shared" si="25"/>
-        <v>135758</v>
+        <v>135446</v>
       </c>
       <c r="R12">
         <f t="shared" si="25"/>
-        <v>141809</v>
+        <v>141488</v>
       </c>
       <c r="S12">
         <f t="shared" si="25"/>
-        <v>148201</v>
+        <v>147870</v>
       </c>
       <c r="T12">
         <f t="shared" si="25"/>
-        <v>154955</v>
+        <v>154614</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1150,8 +1156,8 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <f>ROUND((9500 + 0.25*(B12- 88000) + B3 * 0.0765),0)</f>
-        <v>21783</v>
+        <f>ROUND((9500 + 0.25*((B12/C27)- 88000) + B3 * 0.0765),0)</f>
+        <v>19774</v>
       </c>
       <c r="C13">
         <f>ROUND((9500 + 0.25*(C12 - 88000) + C3 * 0.0765),0)</f>
@@ -1175,55 +1181,55 @@
       </c>
       <c r="H13">
         <f t="shared" si="26"/>
-        <v>17753</v>
+        <v>17693</v>
       </c>
       <c r="I13">
         <f t="shared" si="26"/>
-        <v>18795</v>
+        <v>18734</v>
       </c>
       <c r="J13">
         <f t="shared" si="26"/>
-        <v>19589</v>
+        <v>19526</v>
       </c>
       <c r="K13">
         <f t="shared" si="26"/>
-        <v>20728</v>
+        <v>20663</v>
       </c>
       <c r="L13">
         <f t="shared" si="26"/>
-        <v>21924</v>
+        <v>21857</v>
       </c>
       <c r="M13">
         <f t="shared" si="26"/>
-        <v>23181</v>
+        <v>23112</v>
       </c>
       <c r="N13">
         <f t="shared" si="26"/>
-        <v>24502</v>
+        <v>24431</v>
       </c>
       <c r="O13">
         <f t="shared" si="26"/>
-        <v>25893</v>
+        <v>25819</v>
       </c>
       <c r="P13">
         <f t="shared" si="26"/>
-        <v>23756</v>
+        <v>23681</v>
       </c>
       <c r="Q13">
         <f t="shared" si="26"/>
-        <v>25190</v>
+        <v>25112</v>
       </c>
       <c r="R13">
         <f t="shared" si="26"/>
-        <v>26702</v>
+        <v>26622</v>
       </c>
       <c r="S13">
         <f t="shared" si="26"/>
-        <v>28300</v>
+        <v>28218</v>
       </c>
       <c r="T13">
         <f t="shared" si="26"/>
-        <v>29989</v>
+        <v>29904</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1234,79 +1240,80 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>72200</v>
+        <f>72000*C27</f>
+        <v>54000</v>
       </c>
       <c r="C15">
-        <f>ROUND(B15*1.03,0)</f>
-        <v>74366</v>
+        <f>ROUND((B15/C27)*1.03,0)</f>
+        <v>74160</v>
       </c>
       <c r="D15">
         <f>ROUND(C15*1.03,0)</f>
-        <v>76597</v>
+        <v>76385</v>
       </c>
       <c r="E15">
         <f>ROUND(D15*1.03,0)</f>
-        <v>78895</v>
+        <v>78677</v>
       </c>
       <c r="F15">
         <f t="shared" ref="F15:L15" si="27">ROUND(E15*1.03,0)</f>
-        <v>81262</v>
+        <v>81037</v>
       </c>
       <c r="G15">
         <f t="shared" si="27"/>
-        <v>83700</v>
+        <v>83468</v>
       </c>
       <c r="H15">
         <f t="shared" si="27"/>
-        <v>86211</v>
+        <v>85972</v>
       </c>
       <c r="I15">
         <f t="shared" si="27"/>
-        <v>88797</v>
+        <v>88551</v>
       </c>
       <c r="J15">
         <f>ROUND(I15*1.03,0)-1200</f>
-        <v>90261</v>
+        <v>90008</v>
       </c>
       <c r="K15">
         <f t="shared" si="27"/>
-        <v>92969</v>
+        <v>92708</v>
       </c>
       <c r="L15">
         <f t="shared" si="27"/>
-        <v>95758</v>
+        <v>95489</v>
       </c>
       <c r="M15">
         <f t="shared" ref="M15" si="28">ROUND(L15*1.03,0)</f>
-        <v>98631</v>
+        <v>98354</v>
       </c>
       <c r="N15">
         <f t="shared" ref="N15" si="29">ROUND(M15*1.03,0)</f>
-        <v>101590</v>
+        <v>101305</v>
       </c>
       <c r="O15">
         <f t="shared" ref="O15" si="30">ROUND(N15*1.03,0)</f>
-        <v>104638</v>
+        <v>104344</v>
       </c>
       <c r="P15">
         <f>ROUND(O15*1.03,0)-(1200*12)</f>
-        <v>93377</v>
+        <v>93074</v>
       </c>
       <c r="Q15">
         <f>ROUND(P15*1.03,0)</f>
-        <v>96178</v>
+        <v>95866</v>
       </c>
       <c r="R15">
         <f>ROUND(Q15*1.03,0)</f>
-        <v>99063</v>
+        <v>98742</v>
       </c>
       <c r="S15">
         <f>ROUND(R15*1.03,0)</f>
-        <v>102035</v>
+        <v>101704</v>
       </c>
       <c r="T15">
         <f>ROUND(S15*1.03,0)</f>
-        <v>105096</v>
+        <v>104755</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1314,10 +1321,11 @@
         <v>2</v>
       </c>
       <c r="B16">
-        <v>12000</v>
+        <f>12000*C27</f>
+        <v>9000</v>
       </c>
       <c r="C16">
-        <f>ROUND(B16*1.08,0)</f>
+        <f>ROUND((B16/C27)*1.08,0)</f>
         <v>12960</v>
       </c>
       <c r="D16">
@@ -1403,79 +1411,79 @@
       </c>
       <c r="B18">
         <f>(B15+B16)</f>
-        <v>84200</v>
+        <v>63000</v>
       </c>
       <c r="C18">
         <f t="shared" ref="C18:S18" si="39">(C15+C16)</f>
-        <v>87326</v>
+        <v>87120</v>
       </c>
       <c r="D18">
         <f>(D15+D16+D17)</f>
-        <v>98594</v>
+        <v>98382</v>
       </c>
       <c r="E18">
         <f t="shared" si="39"/>
-        <v>94612</v>
+        <v>94394</v>
       </c>
       <c r="F18">
         <f t="shared" si="39"/>
-        <v>98236</v>
+        <v>98011</v>
       </c>
       <c r="G18">
         <f t="shared" si="39"/>
-        <v>102032</v>
+        <v>101800</v>
       </c>
       <c r="H18">
         <f t="shared" si="39"/>
-        <v>106010</v>
+        <v>105771</v>
       </c>
       <c r="I18">
         <f t="shared" si="39"/>
-        <v>110180</v>
+        <v>109934</v>
       </c>
       <c r="J18">
         <f t="shared" si="39"/>
-        <v>113355</v>
+        <v>113102</v>
       </c>
       <c r="K18">
         <f t="shared" si="39"/>
-        <v>117911</v>
+        <v>117650</v>
       </c>
       <c r="L18">
         <f t="shared" si="39"/>
-        <v>122695</v>
+        <v>122426</v>
       </c>
       <c r="M18">
         <f t="shared" si="39"/>
-        <v>127723</v>
+        <v>127446</v>
       </c>
       <c r="N18">
         <f t="shared" si="39"/>
-        <v>133009</v>
+        <v>132724</v>
       </c>
       <c r="O18">
         <f t="shared" si="39"/>
-        <v>138571</v>
+        <v>138277</v>
       </c>
       <c r="P18">
         <f t="shared" si="39"/>
-        <v>130025</v>
+        <v>129722</v>
       </c>
       <c r="Q18">
         <f t="shared" si="39"/>
-        <v>135758</v>
+        <v>135446</v>
       </c>
       <c r="R18">
         <f t="shared" si="39"/>
-        <v>141809</v>
+        <v>141488</v>
       </c>
       <c r="S18">
         <f t="shared" si="39"/>
-        <v>148201</v>
+        <v>147870</v>
       </c>
       <c r="T18">
         <f t="shared" ref="T18" si="40">(T15+T16)</f>
-        <v>154955</v>
+        <v>154614</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -1505,55 +1513,55 @@
       </c>
       <c r="H20">
         <f t="shared" ref="H20:T20" si="41">H10-H18</f>
-        <v>-56141</v>
+        <v>-55902</v>
       </c>
       <c r="I20">
         <f t="shared" si="41"/>
-        <v>-59377</v>
+        <v>-59131</v>
       </c>
       <c r="J20">
         <f t="shared" si="41"/>
-        <v>-61601</v>
+        <v>-61348</v>
       </c>
       <c r="K20">
         <f t="shared" si="41"/>
-        <v>-49587</v>
+        <v>-49326</v>
       </c>
       <c r="L20">
         <f t="shared" si="41"/>
-        <v>-53070</v>
+        <v>-52801</v>
       </c>
       <c r="M20">
         <f t="shared" si="41"/>
-        <v>-56772</v>
+        <v>-56495</v>
       </c>
       <c r="N20">
         <f t="shared" si="41"/>
-        <v>-60706</v>
+        <v>-60421</v>
       </c>
       <c r="O20">
         <f t="shared" si="41"/>
-        <v>-36089</v>
+        <v>-35795</v>
       </c>
       <c r="P20">
         <f t="shared" si="41"/>
-        <v>-25562</v>
+        <v>-25259</v>
       </c>
       <c r="Q20">
         <f t="shared" si="41"/>
-        <v>-29275</v>
+        <v>-28963</v>
       </c>
       <c r="R20">
         <f t="shared" si="41"/>
-        <v>-33268</v>
+        <v>-32947</v>
       </c>
       <c r="S20">
         <f t="shared" si="41"/>
-        <v>-37560</v>
+        <v>-37229</v>
       </c>
       <c r="T20">
         <f t="shared" si="41"/>
-        <v>-42172</v>
+        <v>-41831</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -1562,79 +1570,79 @@
       </c>
       <c r="B21">
         <f>B10-B13-B18</f>
-        <v>-983</v>
+        <v>-4024</v>
       </c>
       <c r="C21">
         <f>C10-C13-C18</f>
-        <v>-4109</v>
+        <v>-3903</v>
       </c>
       <c r="D21">
         <f>D10-D13-D18</f>
-        <v>-15377</v>
+        <v>-15165</v>
       </c>
       <c r="E21">
         <f>E10-E13-E18</f>
-        <v>23555</v>
+        <v>23773</v>
       </c>
       <c r="F21">
         <f t="shared" ref="F21:G21" si="42">F10-F13-F18</f>
-        <v>-12047</v>
+        <v>-11822</v>
       </c>
       <c r="G21">
         <f t="shared" si="42"/>
-        <v>-12987</v>
+        <v>-12755</v>
       </c>
       <c r="H21">
         <f>-H13</f>
-        <v>-17753</v>
+        <v>-17693</v>
       </c>
       <c r="I21">
         <f t="shared" ref="I21:T21" si="43">-I13</f>
-        <v>-18795</v>
+        <v>-18734</v>
       </c>
       <c r="J21">
         <f t="shared" si="43"/>
-        <v>-19589</v>
+        <v>-19526</v>
       </c>
       <c r="K21">
         <f t="shared" si="43"/>
-        <v>-20728</v>
+        <v>-20663</v>
       </c>
       <c r="L21">
         <f t="shared" si="43"/>
-        <v>-21924</v>
+        <v>-21857</v>
       </c>
       <c r="M21">
         <f t="shared" si="43"/>
-        <v>-23181</v>
+        <v>-23112</v>
       </c>
       <c r="N21">
         <f t="shared" si="43"/>
-        <v>-24502</v>
+        <v>-24431</v>
       </c>
       <c r="O21">
         <f t="shared" si="43"/>
-        <v>-25893</v>
+        <v>-25819</v>
       </c>
       <c r="P21">
         <f t="shared" si="43"/>
-        <v>-23756</v>
+        <v>-23681</v>
       </c>
       <c r="Q21">
         <f t="shared" si="43"/>
-        <v>-25190</v>
+        <v>-25112</v>
       </c>
       <c r="R21">
         <f t="shared" si="43"/>
-        <v>-26702</v>
+        <v>-26622</v>
       </c>
       <c r="S21">
         <f t="shared" si="43"/>
-        <v>-28300</v>
+        <v>-28218</v>
       </c>
       <c r="T21">
         <f t="shared" si="43"/>
-        <v>-29989</v>
+        <v>-29904</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -1670,55 +1678,55 @@
       </c>
       <c r="H23">
         <f t="shared" si="44"/>
-        <v>591822</v>
+        <v>592067</v>
       </c>
       <c r="I23">
         <f t="shared" si="44"/>
-        <v>530381</v>
+        <v>530884</v>
       </c>
       <c r="J23">
         <f t="shared" si="44"/>
-        <v>465125</v>
+        <v>465899</v>
       </c>
       <c r="K23">
         <f t="shared" si="44"/>
-        <v>410551</v>
+        <v>411612</v>
       </c>
       <c r="L23">
         <f t="shared" si="44"/>
-        <v>351043</v>
+        <v>352406</v>
       </c>
       <c r="M23">
         <f t="shared" si="44"/>
-        <v>286253</v>
+        <v>287934</v>
       </c>
       <c r="N23">
         <f t="shared" si="44"/>
-        <v>215811</v>
+        <v>217826</v>
       </c>
       <c r="O23">
         <f t="shared" si="44"/>
-        <v>168840</v>
+        <v>171207</v>
       </c>
       <c r="P23">
         <f t="shared" si="44"/>
-        <v>131485</v>
+        <v>134222</v>
       </c>
       <c r="Q23">
         <f t="shared" si="44"/>
-        <v>89390</v>
+        <v>92515</v>
       </c>
       <c r="R23">
         <f t="shared" si="44"/>
-        <v>42150</v>
+        <v>45682</v>
       </c>
       <c r="S23">
         <f t="shared" si="44"/>
-        <v>-10670</v>
+        <v>-6711</v>
       </c>
       <c r="T23">
         <f t="shared" si="44"/>
-        <v>-69538</v>
+        <v>-65131</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -1727,79 +1735,79 @@
       </c>
       <c r="B24">
         <f>ROUND((60000+B21)*1.025,0)</f>
-        <v>60492</v>
+        <v>57375</v>
       </c>
       <c r="C24">
         <f>ROUND((B24+C21)*1.025,0)</f>
-        <v>57793</v>
+        <v>54809</v>
       </c>
       <c r="D24">
         <f>ROUND((C24+D21)*1.025,0)</f>
-        <v>43476</v>
+        <v>40635</v>
       </c>
       <c r="E24">
         <f t="shared" ref="E24:T24" si="45">ROUND((D24+E21 + $B$26)*1.025,0)</f>
-        <v>84082</v>
+        <v>81393</v>
       </c>
       <c r="F24">
         <f t="shared" si="45"/>
-        <v>89211</v>
+        <v>86685</v>
       </c>
       <c r="G24">
         <f t="shared" si="45"/>
-        <v>93505</v>
+        <v>91153</v>
       </c>
       <c r="H24">
         <f t="shared" si="45"/>
-        <v>93021</v>
+        <v>90672</v>
       </c>
       <c r="I24">
         <f t="shared" si="45"/>
-        <v>91457</v>
+        <v>89111</v>
       </c>
       <c r="J24">
         <f t="shared" si="45"/>
-        <v>89040</v>
+        <v>86700</v>
       </c>
       <c r="K24">
         <f t="shared" si="45"/>
-        <v>85395</v>
+        <v>83063</v>
       </c>
       <c r="L24">
         <f t="shared" si="45"/>
-        <v>80433</v>
+        <v>78111</v>
       </c>
       <c r="M24">
         <f t="shared" si="45"/>
-        <v>74058</v>
+        <v>71749</v>
       </c>
       <c r="N24">
         <f t="shared" si="45"/>
-        <v>66170</v>
+        <v>63876</v>
       </c>
       <c r="O24">
         <f t="shared" si="45"/>
-        <v>56659</v>
+        <v>54383</v>
       </c>
       <c r="P24">
         <f t="shared" si="45"/>
-        <v>49101</v>
+        <v>46845</v>
       </c>
       <c r="Q24">
         <f t="shared" si="45"/>
-        <v>39884</v>
+        <v>37651</v>
       </c>
       <c r="R24">
         <f t="shared" si="45"/>
-        <v>28887</v>
+        <v>26680</v>
       </c>
       <c r="S24">
         <f t="shared" si="45"/>
-        <v>15977</v>
+        <v>13799</v>
       </c>
       <c r="T24">
         <f t="shared" si="45"/>
-        <v>1013</v>
+        <v>-1133</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -1814,53 +1822,64 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refractored partial year into separate method
</commit_message>
<xml_diff>
--- a/test/TestCalculations.xlsx
+++ b/test/TestCalculations.xlsx
@@ -21,15 +21,9 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Expenses</t>
-  </si>
-  <si>
     <t>Med Exp</t>
   </si>
   <si>
-    <t>Gross Exp</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -115,6 +109,12 @@
   </si>
   <si>
     <t>April</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Exp </t>
+  </si>
+  <si>
+    <t>Expenses (final_annual_expenses)</t>
   </si>
 </sst>
 </file>
@@ -465,11 +465,11 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2595" ySplit="735" activePane="bottomRight"/>
+      <pane xSplit="2595" ySplit="735" topLeftCell="B1" activePane="bottomRight"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD28"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +560,7 @@
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>57</v>
@@ -639,14 +639,14 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <f>70*1500*C27</f>
-        <v>78750</v>
+        <f>70*1500</f>
+        <v>105000</v>
       </c>
       <c r="C3">
-        <f>B3/C27</f>
+        <f>B3</f>
         <v>105000</v>
       </c>
       <c r="D3">
@@ -719,7 +719,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <f>3300*12</f>
@@ -788,7 +788,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O5">
         <f>2400*12</f>
@@ -817,7 +817,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K6">
         <f>1300*12</f>
@@ -862,7 +862,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <f>250*12</f>
@@ -923,7 +923,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H8">
         <f>400*12</f>
@@ -980,7 +980,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>9000</v>
@@ -988,11 +988,11 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <f>SUM(B3:B8)</f>
-        <v>78750</v>
+        <v>105000</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:S10" si="23">SUM(C3:C8)</f>
@@ -1072,14 +1072,14 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12:C12" si="24">B10-B20</f>
+        <f>(B10-B20) *C27</f>
         <v>78750</v>
       </c>
       <c r="C12">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="B12:C12" si="24">C10-C20</f>
         <v>105000</v>
       </c>
       <c r="D12">
@@ -1153,11 +1153,11 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <f>ROUND((9500 + 0.25*((B12/C27)- 88000) + B3 * 0.0765),0)</f>
-        <v>19774</v>
+        <f>ROUND((1700 + 0.15*(B12- 36000) + B3 * 0.0765),0)</f>
+        <v>16145</v>
       </c>
       <c r="C13">
         <f>ROUND((9500 + 0.25*(C12 - 88000) + C3 * 0.0765),0)</f>
@@ -1169,67 +1169,67 @@
       </c>
       <c r="E13">
         <f>ROUND((9500 + 0.25*(E12-E9+$B$26-88000) + E3 * 0.0765),0)</f>
-        <v>35433</v>
+        <v>35308</v>
       </c>
       <c r="F13">
         <f t="shared" ref="F13:T13" si="26">ROUND((9500 + 0.25*(F12+$B$26- 88000) + F3 * 0.0765),0)</f>
-        <v>24203</v>
+        <v>24078</v>
       </c>
       <c r="G13">
         <f t="shared" si="26"/>
-        <v>25155</v>
+        <v>25030</v>
       </c>
       <c r="H13">
         <f t="shared" si="26"/>
-        <v>17693</v>
+        <v>17568</v>
       </c>
       <c r="I13">
         <f t="shared" si="26"/>
-        <v>18734</v>
+        <v>18609</v>
       </c>
       <c r="J13">
         <f t="shared" si="26"/>
-        <v>19526</v>
+        <v>19401</v>
       </c>
       <c r="K13">
         <f t="shared" si="26"/>
-        <v>20663</v>
+        <v>20538</v>
       </c>
       <c r="L13">
         <f t="shared" si="26"/>
-        <v>21857</v>
+        <v>21732</v>
       </c>
       <c r="M13">
         <f t="shared" si="26"/>
-        <v>23112</v>
+        <v>22987</v>
       </c>
       <c r="N13">
         <f t="shared" si="26"/>
-        <v>24431</v>
+        <v>24306</v>
       </c>
       <c r="O13">
         <f t="shared" si="26"/>
-        <v>25819</v>
+        <v>25694</v>
       </c>
       <c r="P13">
         <f t="shared" si="26"/>
-        <v>23681</v>
+        <v>23556</v>
       </c>
       <c r="Q13">
         <f t="shared" si="26"/>
-        <v>25112</v>
+        <v>24987</v>
       </c>
       <c r="R13">
         <f t="shared" si="26"/>
-        <v>26622</v>
+        <v>26497</v>
       </c>
       <c r="S13">
         <f t="shared" si="26"/>
-        <v>28218</v>
+        <v>28093</v>
       </c>
       <c r="T13">
         <f t="shared" si="26"/>
-        <v>29904</v>
+        <v>29779</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <f>72000*C27</f>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16">
         <f>12000*C27</f>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D17">
         <v>8000</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <f>(B15+B16)</f>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1566,11 +1566,11 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <f>B10-B13-B18</f>
-        <v>-4024</v>
+        <f>B10*C27-B13-B18</f>
+        <v>-395</v>
       </c>
       <c r="C21">
         <f>C10-C13-C18</f>
@@ -1582,67 +1582,67 @@
       </c>
       <c r="E21">
         <f>E10-E13-E18</f>
-        <v>23773</v>
+        <v>23898</v>
       </c>
       <c r="F21">
         <f t="shared" ref="F21:G21" si="42">F10-F13-F18</f>
-        <v>-11822</v>
+        <v>-11697</v>
       </c>
       <c r="G21">
         <f t="shared" si="42"/>
-        <v>-12755</v>
+        <v>-12630</v>
       </c>
       <c r="H21">
         <f>-H13</f>
-        <v>-17693</v>
+        <v>-17568</v>
       </c>
       <c r="I21">
         <f t="shared" ref="I21:T21" si="43">-I13</f>
-        <v>-18734</v>
+        <v>-18609</v>
       </c>
       <c r="J21">
         <f t="shared" si="43"/>
-        <v>-19526</v>
+        <v>-19401</v>
       </c>
       <c r="K21">
         <f t="shared" si="43"/>
-        <v>-20663</v>
+        <v>-20538</v>
       </c>
       <c r="L21">
         <f t="shared" si="43"/>
-        <v>-21857</v>
+        <v>-21732</v>
       </c>
       <c r="M21">
         <f t="shared" si="43"/>
-        <v>-23112</v>
+        <v>-22987</v>
       </c>
       <c r="N21">
         <f t="shared" si="43"/>
-        <v>-24431</v>
+        <v>-24306</v>
       </c>
       <c r="O21">
         <f t="shared" si="43"/>
-        <v>-25819</v>
+        <v>-25694</v>
       </c>
       <c r="P21">
         <f t="shared" si="43"/>
-        <v>-23681</v>
+        <v>-23556</v>
       </c>
       <c r="Q21">
         <f t="shared" si="43"/>
-        <v>-25112</v>
+        <v>-24987</v>
       </c>
       <c r="R21">
         <f t="shared" si="43"/>
-        <v>-26622</v>
+        <v>-26497</v>
       </c>
       <c r="S21">
         <f t="shared" si="43"/>
-        <v>-28218</v>
+        <v>-28093</v>
       </c>
       <c r="T21">
         <f t="shared" si="43"/>
-        <v>-29904</v>
+        <v>-29779</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -1650,7 +1650,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <f>ROUND((600000+B20)*1.025,0)</f>
@@ -1666,148 +1666,148 @@
       </c>
       <c r="E23">
         <f t="shared" ref="E23:T23" si="44">ROUND((D23-$B$26+E20)*1.025,0)</f>
-        <v>646912</v>
+        <v>647425</v>
       </c>
       <c r="F23">
         <f t="shared" si="44"/>
-        <v>647710</v>
+        <v>648748</v>
       </c>
       <c r="G23">
         <f t="shared" si="44"/>
-        <v>648528</v>
+        <v>650104</v>
       </c>
       <c r="H23">
         <f t="shared" si="44"/>
-        <v>592067</v>
+        <v>594195</v>
       </c>
       <c r="I23">
         <f t="shared" si="44"/>
-        <v>530884</v>
+        <v>533578</v>
       </c>
       <c r="J23">
         <f t="shared" si="44"/>
-        <v>465899</v>
+        <v>469173</v>
       </c>
       <c r="K23">
         <f t="shared" si="44"/>
-        <v>411612</v>
+        <v>415481</v>
       </c>
       <c r="L23">
         <f t="shared" si="44"/>
-        <v>352406</v>
+        <v>356885</v>
       </c>
       <c r="M23">
         <f t="shared" si="44"/>
-        <v>287934</v>
+        <v>293037</v>
       </c>
       <c r="N23">
         <f t="shared" si="44"/>
-        <v>217826</v>
+        <v>223569</v>
       </c>
       <c r="O23">
         <f t="shared" si="44"/>
-        <v>171207</v>
+        <v>177606</v>
       </c>
       <c r="P23">
         <f t="shared" si="44"/>
-        <v>134222</v>
+        <v>141293</v>
       </c>
       <c r="Q23">
         <f t="shared" si="44"/>
-        <v>92515</v>
+        <v>100276</v>
       </c>
       <c r="R23">
         <f t="shared" si="44"/>
-        <v>45682</v>
+        <v>54150</v>
       </c>
       <c r="S23">
         <f t="shared" si="44"/>
-        <v>-6711</v>
+        <v>2482</v>
       </c>
       <c r="T23">
         <f t="shared" si="44"/>
-        <v>-65131</v>
+        <v>-55195</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <f>ROUND((60000+B21)*1.025,0)</f>
-        <v>57375</v>
+        <v>61095</v>
       </c>
       <c r="C24">
         <f>ROUND((B24+C21)*1.025,0)</f>
-        <v>54809</v>
+        <v>58622</v>
       </c>
       <c r="D24">
         <f>ROUND((C24+D21)*1.025,0)</f>
-        <v>40635</v>
+        <v>44543</v>
       </c>
       <c r="E24">
         <f t="shared" ref="E24:T24" si="45">ROUND((D24+E21 + $B$26)*1.025,0)</f>
-        <v>81393</v>
+        <v>85015</v>
       </c>
       <c r="F24">
         <f t="shared" si="45"/>
-        <v>86685</v>
+        <v>90013</v>
       </c>
       <c r="G24">
         <f t="shared" si="45"/>
-        <v>91153</v>
+        <v>94180</v>
       </c>
       <c r="H24">
         <f t="shared" si="45"/>
-        <v>90672</v>
+        <v>93390</v>
       </c>
       <c r="I24">
         <f t="shared" si="45"/>
-        <v>89111</v>
+        <v>91513</v>
       </c>
       <c r="J24">
         <f t="shared" si="45"/>
-        <v>86700</v>
+        <v>88777</v>
       </c>
       <c r="K24">
         <f t="shared" si="45"/>
-        <v>83063</v>
+        <v>84807</v>
       </c>
       <c r="L24">
         <f t="shared" si="45"/>
-        <v>78111</v>
+        <v>79514</v>
       </c>
       <c r="M24">
         <f t="shared" si="45"/>
-        <v>71749</v>
+        <v>72803</v>
       </c>
       <c r="N24">
         <f t="shared" si="45"/>
-        <v>63876</v>
+        <v>64572</v>
       </c>
       <c r="O24">
         <f t="shared" si="45"/>
-        <v>54383</v>
+        <v>54712</v>
       </c>
       <c r="P24">
         <f t="shared" si="45"/>
-        <v>46845</v>
+        <v>46797</v>
       </c>
       <c r="Q24">
         <f t="shared" si="45"/>
-        <v>37651</v>
+        <v>37218</v>
       </c>
       <c r="R24">
         <f t="shared" si="45"/>
-        <v>26680</v>
+        <v>25852</v>
       </c>
       <c r="S24">
         <f t="shared" si="45"/>
-        <v>13799</v>
+        <v>12565</v>
       </c>
       <c r="T24">
         <f t="shared" si="45"/>
-        <v>-1133</v>
+        <v>-2782</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -1815,18 +1815,18 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>15000</v>
+        <v>14500</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27">
         <v>0.75</v>
@@ -1837,50 +1837,50 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ss reduction year and percent Income.rb
</commit_message>
<xml_diff>
--- a/test/TestCalculations.xlsx
+++ b/test/TestCalculations.xlsx
@@ -469,7 +469,7 @@
       <selection activeCell="A19" sqref="A19"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
+      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,15 +791,15 @@
         <v>4</v>
       </c>
       <c r="O5">
-        <f>2400*12</f>
-        <v>28800</v>
+        <f>3000*12</f>
+        <v>36000</v>
       </c>
       <c r="P5">
         <f t="shared" ref="L5:T6" si="12">ROUND(O5*1.02,0)</f>
-        <v>29376</v>
+        <v>36720</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="12"/>
+        <f>ROUND(P5*1.02*0.8,0)</f>
         <v>29964</v>
       </c>
       <c r="R5">
@@ -844,20 +844,20 @@
         <v>17224</v>
       </c>
       <c r="Q6">
-        <f t="shared" ref="Q6" si="17">ROUND(P6*1.02,0)</f>
-        <v>17568</v>
+        <f>ROUND(P6*1.02*0.8,0)</f>
+        <v>14055</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6" si="18">ROUND(Q6*1.02,0)</f>
-        <v>17919</v>
+        <f t="shared" ref="R6" si="17">ROUND(Q6*1.02,0)</f>
+        <v>14336</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6" si="19">ROUND(R6*1.02,0)</f>
-        <v>18277</v>
+        <f t="shared" ref="S6" si="18">ROUND(R6*1.02,0)</f>
+        <v>14623</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6" si="20">ROUND(S6*1.02,0)</f>
-        <v>18643</v>
+        <f t="shared" ref="T6" si="19">ROUND(S6*1.02,0)</f>
+        <v>14915</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -873,47 +873,47 @@
         <v>3045</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:S7" si="21">ROUND(H7*1.015,0)</f>
+        <f t="shared" ref="I7:S7" si="20">ROUND(H7*1.015,0)</f>
         <v>3091</v>
       </c>
       <c r="J7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3137</v>
       </c>
       <c r="K7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3184</v>
       </c>
       <c r="L7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3232</v>
       </c>
       <c r="M7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3280</v>
       </c>
       <c r="N7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3329</v>
       </c>
       <c r="O7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3379</v>
       </c>
       <c r="P7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3430</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3481</v>
       </c>
       <c r="R7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3533</v>
       </c>
       <c r="S7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3586</v>
       </c>
       <c r="T7">
@@ -930,51 +930,51 @@
         <v>4800</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:T8" si="22">ROUND(H8*1.01,0)</f>
+        <f t="shared" ref="I8:T8" si="21">ROUND(H8*1.01,0)</f>
         <v>4848</v>
       </c>
       <c r="J8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4896</v>
       </c>
       <c r="K8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4945</v>
       </c>
       <c r="L8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4994</v>
       </c>
       <c r="M8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5044</v>
       </c>
       <c r="N8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5094</v>
       </c>
       <c r="O8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5145</v>
       </c>
       <c r="P8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5196</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5248</v>
       </c>
       <c r="R8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5300</v>
       </c>
       <c r="S8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5353</v>
       </c>
       <c r="T8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>5407</v>
       </c>
     </row>
@@ -995,11 +995,11 @@
         <v>105000</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:S10" si="23">SUM(C3:C8)</f>
+        <f t="shared" ref="C10:S10" si="22">SUM(C3:C8)</f>
         <v>105000</v>
       </c>
       <c r="D10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>105000</v>
       </c>
       <c r="E10">
@@ -1007,11 +1007,11 @@
         <v>153600</v>
       </c>
       <c r="F10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>110392</v>
       </c>
       <c r="G10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>114200</v>
       </c>
       <c r="H10">
@@ -1019,52 +1019,52 @@
         <v>49869</v>
       </c>
       <c r="I10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>50803</v>
       </c>
       <c r="J10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>51754</v>
       </c>
       <c r="K10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>68324</v>
       </c>
       <c r="L10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>69625</v>
       </c>
       <c r="M10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>70951</v>
       </c>
       <c r="N10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>72303</v>
       </c>
       <c r="O10">
-        <f t="shared" si="23"/>
-        <v>102482</v>
+        <f t="shared" si="22"/>
+        <v>109682</v>
       </c>
       <c r="P10">
-        <f t="shared" si="23"/>
-        <v>104463</v>
+        <f t="shared" si="22"/>
+        <v>111807</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="23"/>
-        <v>106483</v>
+        <f t="shared" si="22"/>
+        <v>102970</v>
       </c>
       <c r="R10">
-        <f t="shared" si="23"/>
-        <v>108541</v>
+        <f t="shared" si="22"/>
+        <v>104958</v>
       </c>
       <c r="S10">
-        <f t="shared" si="23"/>
-        <v>110641</v>
+        <f t="shared" si="22"/>
+        <v>106987</v>
       </c>
       <c r="T10">
         <f>SUM(T3:T8)</f>
-        <v>112783</v>
+        <v>109055</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1079,7 +1079,7 @@
         <v>78750</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="B12:C12" si="24">C10-C20</f>
+        <f t="shared" ref="C12" si="23">C10-C20</f>
         <v>105000</v>
       </c>
       <c r="D12">
@@ -1087,67 +1087,67 @@
         <v>105000</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:T12" si="25">E10-E20</f>
+        <f t="shared" ref="E12:T12" si="24">E10-E20</f>
         <v>153600</v>
       </c>
       <c r="F12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>110392</v>
       </c>
       <c r="G12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>114200</v>
       </c>
       <c r="H12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>105771</v>
       </c>
       <c r="I12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>109934</v>
       </c>
       <c r="J12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>113102</v>
       </c>
       <c r="K12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>117650</v>
       </c>
       <c r="L12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>122426</v>
       </c>
       <c r="M12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>127446</v>
       </c>
       <c r="N12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>132724</v>
       </c>
       <c r="O12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>138277</v>
       </c>
       <c r="P12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>129722</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>135446</v>
       </c>
       <c r="R12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>141488</v>
       </c>
       <c r="S12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>147870</v>
       </c>
       <c r="T12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>154614</v>
       </c>
     </row>
@@ -1172,63 +1172,63 @@
         <v>35308</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:T13" si="26">ROUND((9500 + 0.25*(F12+$B$26- 88000) + F3 * 0.0765),0)</f>
+        <f t="shared" ref="F13:T13" si="25">ROUND((9500 + 0.25*(F12+$B$26- 88000) + F3 * 0.0765),0)</f>
         <v>24078</v>
       </c>
       <c r="G13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>25030</v>
       </c>
       <c r="H13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>17568</v>
       </c>
       <c r="I13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>18609</v>
       </c>
       <c r="J13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>19401</v>
       </c>
       <c r="K13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>20538</v>
       </c>
       <c r="L13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>21732</v>
       </c>
       <c r="M13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>22987</v>
       </c>
       <c r="N13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>24306</v>
       </c>
       <c r="O13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>25694</v>
       </c>
       <c r="P13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>23556</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>24987</v>
       </c>
       <c r="R13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>26497</v>
       </c>
       <c r="S13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>28093</v>
       </c>
       <c r="T13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>29779</v>
       </c>
     </row>
@@ -1256,19 +1256,19 @@
         <v>78677</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:L15" si="27">ROUND(E15*1.03,0)</f>
+        <f t="shared" ref="F15:L15" si="26">ROUND(E15*1.03,0)</f>
         <v>81037</v>
       </c>
       <c r="G15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>83468</v>
       </c>
       <c r="H15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>85972</v>
       </c>
       <c r="I15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>88551</v>
       </c>
       <c r="J15">
@@ -1276,23 +1276,23 @@
         <v>90008</v>
       </c>
       <c r="K15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>92708</v>
       </c>
       <c r="L15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>95489</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15" si="28">ROUND(L15*1.03,0)</f>
+        <f t="shared" ref="M15" si="27">ROUND(L15*1.03,0)</f>
         <v>98354</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15" si="29">ROUND(M15*1.03,0)</f>
+        <f t="shared" ref="N15" si="28">ROUND(M15*1.03,0)</f>
         <v>101305</v>
       </c>
       <c r="O15">
-        <f t="shared" ref="O15" si="30">ROUND(N15*1.03,0)</f>
+        <f t="shared" ref="O15" si="29">ROUND(N15*1.03,0)</f>
         <v>104344</v>
       </c>
       <c r="P15">
@@ -1329,7 +1329,7 @@
         <v>12960</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:L16" si="31">ROUND(C16*1.08,0)</f>
+        <f t="shared" ref="D16:L16" si="30">ROUND(C16*1.08,0)</f>
         <v>13997</v>
       </c>
       <c r="E16">
@@ -1337,63 +1337,63 @@
         <v>15717</v>
       </c>
       <c r="F16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>16974</v>
       </c>
       <c r="G16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>18332</v>
       </c>
       <c r="H16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>19799</v>
       </c>
       <c r="I16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>21383</v>
       </c>
       <c r="J16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>23094</v>
       </c>
       <c r="K16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>24942</v>
       </c>
       <c r="L16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>26937</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16" si="32">ROUND(L16*1.08,0)</f>
+        <f t="shared" ref="M16" si="31">ROUND(L16*1.08,0)</f>
         <v>29092</v>
       </c>
       <c r="N16">
-        <f t="shared" ref="N16" si="33">ROUND(M16*1.08,0)</f>
+        <f t="shared" ref="N16" si="32">ROUND(M16*1.08,0)</f>
         <v>31419</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16" si="34">ROUND(N16*1.08,0)</f>
+        <f t="shared" ref="O16" si="33">ROUND(N16*1.08,0)</f>
         <v>33933</v>
       </c>
       <c r="P16">
-        <f t="shared" ref="P16" si="35">ROUND(O16*1.08,0)</f>
+        <f t="shared" ref="P16" si="34">ROUND(O16*1.08,0)</f>
         <v>36648</v>
       </c>
       <c r="Q16">
-        <f t="shared" ref="Q16" si="36">ROUND(P16*1.08,0)</f>
+        <f t="shared" ref="Q16" si="35">ROUND(P16*1.08,0)</f>
         <v>39580</v>
       </c>
       <c r="R16">
-        <f t="shared" ref="R16" si="37">ROUND(Q16*1.08,0)</f>
+        <f t="shared" ref="R16" si="36">ROUND(Q16*1.08,0)</f>
         <v>42746</v>
       </c>
       <c r="S16">
-        <f t="shared" ref="S16:T16" si="38">ROUND(R16*1.08,0)</f>
+        <f t="shared" ref="S16:T16" si="37">ROUND(R16*1.08,0)</f>
         <v>46166</v>
       </c>
       <c r="T16">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>49859</v>
       </c>
     </row>
@@ -1414,7 +1414,7 @@
         <v>63000</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:S18" si="39">(C15+C16)</f>
+        <f t="shared" ref="C18:S18" si="38">(C15+C16)</f>
         <v>87120</v>
       </c>
       <c r="D18">
@@ -1422,67 +1422,67 @@
         <v>98382</v>
       </c>
       <c r="E18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>94394</v>
       </c>
       <c r="F18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>98011</v>
       </c>
       <c r="G18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>101800</v>
       </c>
       <c r="H18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>105771</v>
       </c>
       <c r="I18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>109934</v>
       </c>
       <c r="J18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>113102</v>
       </c>
       <c r="K18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>117650</v>
       </c>
       <c r="L18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>122426</v>
       </c>
       <c r="M18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>127446</v>
       </c>
       <c r="N18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>132724</v>
       </c>
       <c r="O18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>138277</v>
       </c>
       <c r="P18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>129722</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>135446</v>
       </c>
       <c r="R18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>141488</v>
       </c>
       <c r="S18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>147870</v>
       </c>
       <c r="T18">
-        <f t="shared" ref="T18" si="40">(T15+T16)</f>
+        <f t="shared" ref="T18" si="39">(T15+T16)</f>
         <v>154614</v>
       </c>
     </row>
@@ -1512,56 +1512,56 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:T20" si="41">H10-H18</f>
+        <f t="shared" ref="H20:T20" si="40">H10-H18</f>
         <v>-55902</v>
       </c>
       <c r="I20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>-59131</v>
       </c>
       <c r="J20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>-61348</v>
       </c>
       <c r="K20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>-49326</v>
       </c>
       <c r="L20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>-52801</v>
       </c>
       <c r="M20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>-56495</v>
       </c>
       <c r="N20">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>-60421</v>
       </c>
       <c r="O20">
-        <f t="shared" si="41"/>
-        <v>-35795</v>
+        <f t="shared" si="40"/>
+        <v>-28595</v>
       </c>
       <c r="P20">
-        <f t="shared" si="41"/>
-        <v>-25259</v>
+        <f t="shared" si="40"/>
+        <v>-17915</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="41"/>
-        <v>-28963</v>
+        <f t="shared" si="40"/>
+        <v>-32476</v>
       </c>
       <c r="R20">
-        <f t="shared" si="41"/>
-        <v>-32947</v>
+        <f t="shared" si="40"/>
+        <v>-36530</v>
       </c>
       <c r="S20">
-        <f t="shared" si="41"/>
-        <v>-37229</v>
+        <f t="shared" si="40"/>
+        <v>-40883</v>
       </c>
       <c r="T20">
-        <f t="shared" si="41"/>
-        <v>-41831</v>
+        <f t="shared" si="40"/>
+        <v>-45559</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -1585,11 +1585,11 @@
         <v>23898</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:G21" si="42">F10-F13-F18</f>
+        <f t="shared" ref="F21:G21" si="41">F10-F13-F18</f>
         <v>-11697</v>
       </c>
       <c r="G21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>-12630</v>
       </c>
       <c r="H21">
@@ -1597,51 +1597,51 @@
         <v>-17568</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:T21" si="43">-I13</f>
+        <f t="shared" ref="I21:T21" si="42">-I13</f>
         <v>-18609</v>
       </c>
       <c r="J21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-19401</v>
       </c>
       <c r="K21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-20538</v>
       </c>
       <c r="L21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-21732</v>
       </c>
       <c r="M21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-22987</v>
       </c>
       <c r="N21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-24306</v>
       </c>
       <c r="O21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-25694</v>
       </c>
       <c r="P21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-23556</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-24987</v>
       </c>
       <c r="R21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-26497</v>
       </c>
       <c r="S21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-28093</v>
       </c>
       <c r="T21">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-29779</v>
       </c>
     </row>
@@ -1665,68 +1665,68 @@
         <v>646134</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:T23" si="44">ROUND((D23-$B$26+E20)*1.025,0)</f>
+        <f t="shared" ref="E23:T23" si="43">ROUND((D23-$B$26+E20)*1.025,0)</f>
         <v>647425</v>
       </c>
       <c r="F23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>648748</v>
       </c>
       <c r="G23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>650104</v>
       </c>
       <c r="H23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>594195</v>
       </c>
       <c r="I23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>533578</v>
       </c>
       <c r="J23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>469173</v>
       </c>
       <c r="K23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>415481</v>
       </c>
       <c r="L23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>356885</v>
       </c>
       <c r="M23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>293037</v>
       </c>
       <c r="N23">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>223569</v>
       </c>
       <c r="O23">
-        <f t="shared" si="44"/>
-        <v>177606</v>
+        <f t="shared" si="43"/>
+        <v>184986</v>
       </c>
       <c r="P23">
-        <f t="shared" si="44"/>
-        <v>141293</v>
+        <f t="shared" si="43"/>
+        <v>156385</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="44"/>
-        <v>100276</v>
+        <f t="shared" si="43"/>
+        <v>112144</v>
       </c>
       <c r="R23">
-        <f t="shared" si="44"/>
-        <v>54150</v>
+        <f t="shared" si="43"/>
+        <v>62642</v>
       </c>
       <c r="S23">
-        <f t="shared" si="44"/>
-        <v>2482</v>
+        <f t="shared" si="43"/>
+        <v>7440</v>
       </c>
       <c r="T23">
-        <f t="shared" si="44"/>
-        <v>-55195</v>
+        <f t="shared" si="43"/>
+        <v>-53934</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -1746,67 +1746,67 @@
         <v>44543</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:T24" si="45">ROUND((D24+E21 + $B$26)*1.025,0)</f>
+        <f t="shared" ref="E24:T24" si="44">ROUND((D24+E21 + $B$26)*1.025,0)</f>
         <v>85015</v>
       </c>
       <c r="F24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>90013</v>
       </c>
       <c r="G24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>94180</v>
       </c>
       <c r="H24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>93390</v>
       </c>
       <c r="I24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>91513</v>
       </c>
       <c r="J24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>88777</v>
       </c>
       <c r="K24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>84807</v>
       </c>
       <c r="L24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>79514</v>
       </c>
       <c r="M24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>72803</v>
       </c>
       <c r="N24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>64572</v>
       </c>
       <c r="O24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>54712</v>
       </c>
       <c r="P24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>46797</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>37218</v>
       </c>
       <c r="R24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>25852</v>
       </c>
       <c r="S24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>12565</v>
       </c>
       <c r="T24">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>-2782</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ability to reduce SS income at a specified year
</commit_message>
<xml_diff>
--- a/test/TestCalculations.xlsx
+++ b/test/TestCalculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Year</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Expenses (final_annual_expenses)</t>
+  </si>
+  <si>
+    <t>Calculated IRA Savings</t>
+  </si>
+  <si>
+    <t>Calculated non-IRA Savings</t>
+  </si>
+  <si>
+    <t>IRA Sav - Cal IRA Sav</t>
+  </si>
+  <si>
+    <t>non-IRA Sav - Calc non-IRA Sav</t>
   </si>
 </sst>
 </file>
@@ -462,14 +474,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:AL42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2595" ySplit="735" topLeftCell="B1" activePane="bottomRight"/>
+      <pane xSplit="2595" ySplit="735" topLeftCell="L1" activePane="bottomRight"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="O5" sqref="O5"/>
+      <selection pane="topRight" activeCell="AA2" sqref="AA2"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="AK30" sqref="AK30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +493,7 @@
     <col min="12" max="12" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,8 +569,26 @@
       <c r="T1" s="1">
         <v>2029</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -636,8 +666,62 @@
       <c r="T2" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" s="1">
+        <v>76</v>
+      </c>
+      <c r="V2" s="1">
+        <v>77</v>
+      </c>
+      <c r="W2" s="1">
+        <v>78</v>
+      </c>
+      <c r="X2" s="1">
+        <v>79</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>80</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>81</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>82</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>83</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>84</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>95</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>86</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>87</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>88</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>89</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>90</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>91</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>92</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -716,8 +800,76 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <f t="shared" ref="U3" si="11">ROUND(T3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3" si="12">ROUND(U3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3" si="13">ROUND(V3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3" si="14">ROUND(W3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3" si="15">ROUND(X3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3" si="16">ROUND(Y3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" ref="AA3" si="17">ROUND(Z3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3" si="18">ROUND(AA3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <f t="shared" ref="AC3" si="19">ROUND(AB3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <f t="shared" ref="AD3" si="20">ROUND(AC3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" ref="AE3" si="21">ROUND(AD3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" ref="AF3" si="22">ROUND(AE3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" ref="AG3" si="23">ROUND(AF3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <f t="shared" ref="AH3" si="24">ROUND(AG3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <f t="shared" ref="AI3" si="25">ROUND(AH3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" ref="AJ3" si="26">ROUND(AI3*1.03,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" ref="AK3" si="27">ROUND(AJ3*1.03,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -730,63 +882,131 @@
         <v>40392</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:T4" si="11">ROUND(F4*1.02,0)</f>
+        <f t="shared" ref="G4:T4" si="28">ROUND(F4*1.02,0)</f>
         <v>41200</v>
       </c>
       <c r="H4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>42024</v>
       </c>
       <c r="I4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>42864</v>
       </c>
       <c r="J4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>43721</v>
       </c>
       <c r="K4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>44595</v>
       </c>
       <c r="L4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>45487</v>
       </c>
       <c r="M4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>46397</v>
       </c>
       <c r="N4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>47325</v>
       </c>
       <c r="O4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>48272</v>
       </c>
       <c r="P4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>49237</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>50222</v>
       </c>
       <c r="R4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>51226</v>
       </c>
       <c r="S4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>52251</v>
       </c>
       <c r="T4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="28"/>
         <v>53296</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <f t="shared" ref="U4:U6" si="29">ROUND(T4*1.02,0)</f>
+        <v>54362</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V6" si="30">ROUND(U4*1.02,0)</f>
+        <v>55449</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4:W6" si="31">ROUND(V4*1.02,0)</f>
+        <v>56558</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X6" si="32">ROUND(W4*1.02,0)</f>
+        <v>57689</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y6" si="33">ROUND(X4*1.02,0)</f>
+        <v>58843</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z6" si="34">ROUND(Y4*1.02,0)</f>
+        <v>60020</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA6" si="35">ROUND(Z4*1.02,0)</f>
+        <v>61220</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" ref="AB4:AB6" si="36">ROUND(AA4*1.02,0)</f>
+        <v>62444</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" ref="AC4:AC6" si="37">ROUND(AB4*1.02,0)</f>
+        <v>63693</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD6" si="38">ROUND(AC4*1.02,0)</f>
+        <v>64967</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" ref="AE4:AE6" si="39">ROUND(AD4*1.02,0)</f>
+        <v>66266</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" ref="AF4:AF6" si="40">ROUND(AE4*1.02,0)</f>
+        <v>67591</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" ref="AG4:AG6" si="41">ROUND(AF4*1.02,0)</f>
+        <v>68943</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" ref="AH4:AH6" si="42">ROUND(AG4*1.02,0)</f>
+        <v>70322</v>
+      </c>
+      <c r="AI4">
+        <f t="shared" ref="AI4:AI6" si="43">ROUND(AH4*1.02,0)</f>
+        <v>71728</v>
+      </c>
+      <c r="AJ4">
+        <f t="shared" ref="AJ4:AJ6" si="44">ROUND(AI4*1.02,0)</f>
+        <v>73163</v>
+      </c>
+      <c r="AK4">
+        <f t="shared" ref="AK4:AK6" si="45">ROUND(AJ4*1.02,0)</f>
+        <v>74626</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -795,7 +1015,7 @@
         <v>36000</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="L5:T6" si="12">ROUND(O5*1.02,0)</f>
+        <f t="shared" ref="L5:T6" si="46">ROUND(O5*1.02,0)</f>
         <v>36720</v>
       </c>
       <c r="Q5">
@@ -803,19 +1023,87 @@
         <v>29964</v>
       </c>
       <c r="R5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="46"/>
         <v>30563</v>
       </c>
       <c r="S5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="46"/>
         <v>31174</v>
       </c>
       <c r="T5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="46"/>
         <v>31797</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <f t="shared" si="29"/>
+        <v>32433</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="30"/>
+        <v>33082</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="31"/>
+        <v>33744</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="32"/>
+        <v>34419</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="33"/>
+        <v>35107</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="34"/>
+        <v>35809</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="35"/>
+        <v>36525</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="36"/>
+        <v>37256</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="37"/>
+        <v>38001</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="38"/>
+        <v>38761</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="39"/>
+        <v>39536</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="40"/>
+        <v>40327</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="41"/>
+        <v>41134</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="42"/>
+        <v>41957</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="43"/>
+        <v>42796</v>
+      </c>
+      <c r="AJ5">
+        <f t="shared" si="44"/>
+        <v>43652</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" si="45"/>
+        <v>44525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -824,23 +1112,23 @@
         <v>15600</v>
       </c>
       <c r="L6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="46"/>
         <v>15912</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6" si="13">ROUND(L6*1.02,0)</f>
+        <f t="shared" ref="M6" si="47">ROUND(L6*1.02,0)</f>
         <v>16230</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6" si="14">ROUND(M6*1.02,0)</f>
+        <f t="shared" ref="N6" si="48">ROUND(M6*1.02,0)</f>
         <v>16555</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6" si="15">ROUND(N6*1.02,0)</f>
+        <f t="shared" ref="O6" si="49">ROUND(N6*1.02,0)</f>
         <v>16886</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6" si="16">ROUND(O6*1.02,0)</f>
+        <f t="shared" ref="P6" si="50">ROUND(O6*1.02,0)</f>
         <v>17224</v>
       </c>
       <c r="Q6">
@@ -848,19 +1136,87 @@
         <v>14055</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6" si="17">ROUND(Q6*1.02,0)</f>
+        <f t="shared" ref="R6" si="51">ROUND(Q6*1.02,0)</f>
         <v>14336</v>
       </c>
       <c r="S6">
-        <f t="shared" ref="S6" si="18">ROUND(R6*1.02,0)</f>
+        <f t="shared" ref="S6" si="52">ROUND(R6*1.02,0)</f>
         <v>14623</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6" si="19">ROUND(S6*1.02,0)</f>
+        <f t="shared" ref="T6" si="53">ROUND(S6*1.02,0)</f>
         <v>14915</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <f t="shared" si="29"/>
+        <v>15213</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="30"/>
+        <v>15517</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="31"/>
+        <v>15827</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="32"/>
+        <v>16144</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="33"/>
+        <v>16467</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="34"/>
+        <v>16796</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="35"/>
+        <v>17132</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="36"/>
+        <v>17475</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="37"/>
+        <v>17825</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="38"/>
+        <v>18182</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="39"/>
+        <v>18546</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="40"/>
+        <v>18917</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="41"/>
+        <v>19295</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="42"/>
+        <v>19681</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" si="43"/>
+        <v>20075</v>
+      </c>
+      <c r="AJ6">
+        <f t="shared" si="44"/>
+        <v>20477</v>
+      </c>
+      <c r="AK6">
+        <f t="shared" si="45"/>
+        <v>20887</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -873,55 +1229,123 @@
         <v>3045</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:S7" si="20">ROUND(H7*1.015,0)</f>
+        <f t="shared" ref="I7:S7" si="54">ROUND(H7*1.015,0)</f>
         <v>3091</v>
       </c>
       <c r="J7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3137</v>
       </c>
       <c r="K7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3184</v>
       </c>
       <c r="L7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3232</v>
       </c>
       <c r="M7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3280</v>
       </c>
       <c r="N7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3329</v>
       </c>
       <c r="O7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3379</v>
       </c>
       <c r="P7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3430</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3481</v>
       </c>
       <c r="R7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3533</v>
       </c>
       <c r="S7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="54"/>
         <v>3586</v>
       </c>
       <c r="T7">
         <f>ROUND(S7*1.015,0)</f>
         <v>3640</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <f t="shared" ref="U7:Z7" si="55">ROUND(T7*1.015,0)</f>
+        <v>3695</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="55"/>
+        <v>3750</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="55"/>
+        <v>3806</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="55"/>
+        <v>3863</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="55"/>
+        <v>3921</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="55"/>
+        <v>3980</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" ref="AA7" si="56">ROUND(Z7*1.015,0)</f>
+        <v>4040</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" ref="AB7" si="57">ROUND(AA7*1.015,0)</f>
+        <v>4101</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" ref="AC7" si="58">ROUND(AB7*1.015,0)</f>
+        <v>4163</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" ref="AD7" si="59">ROUND(AC7*1.015,0)</f>
+        <v>4225</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" ref="AE7" si="60">ROUND(AD7*1.015,0)</f>
+        <v>4288</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" ref="AF7" si="61">ROUND(AE7*1.015,0)</f>
+        <v>4352</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" ref="AG7" si="62">ROUND(AF7*1.015,0)</f>
+        <v>4417</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" ref="AH7" si="63">ROUND(AG7*1.015,0)</f>
+        <v>4483</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" ref="AI7" si="64">ROUND(AH7*1.015,0)</f>
+        <v>4550</v>
+      </c>
+      <c r="AJ7">
+        <f t="shared" ref="AJ7" si="65">ROUND(AI7*1.015,0)</f>
+        <v>4618</v>
+      </c>
+      <c r="AK7">
+        <f t="shared" ref="AK7" si="66">ROUND(AJ7*1.015,0)</f>
+        <v>4687</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -930,55 +1354,123 @@
         <v>4800</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:T8" si="21">ROUND(H8*1.01,0)</f>
+        <f t="shared" ref="I8:T8" si="67">ROUND(H8*1.01,0)</f>
         <v>4848</v>
       </c>
       <c r="J8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>4896</v>
       </c>
       <c r="K8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>4945</v>
       </c>
       <c r="L8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>4994</v>
       </c>
       <c r="M8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>5044</v>
       </c>
       <c r="N8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>5094</v>
       </c>
       <c r="O8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>5145</v>
       </c>
       <c r="P8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>5196</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>5248</v>
       </c>
       <c r="R8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>5300</v>
       </c>
       <c r="S8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>5353</v>
       </c>
       <c r="T8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="67"/>
         <v>5407</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <f t="shared" ref="U8" si="68">ROUND(T8*1.01,0)</f>
+        <v>5461</v>
+      </c>
+      <c r="V8">
+        <f t="shared" ref="V8" si="69">ROUND(U8*1.01,0)</f>
+        <v>5516</v>
+      </c>
+      <c r="W8">
+        <f t="shared" ref="W8" si="70">ROUND(V8*1.01,0)</f>
+        <v>5571</v>
+      </c>
+      <c r="X8">
+        <f t="shared" ref="X8" si="71">ROUND(W8*1.01,0)</f>
+        <v>5627</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ref="Y8" si="72">ROUND(X8*1.01,0)</f>
+        <v>5683</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" ref="Z8" si="73">ROUND(Y8*1.01,0)</f>
+        <v>5740</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" ref="AA8" si="74">ROUND(Z8*1.01,0)</f>
+        <v>5797</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" ref="AB8" si="75">ROUND(AA8*1.01,0)</f>
+        <v>5855</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" ref="AC8" si="76">ROUND(AB8*1.01,0)</f>
+        <v>5914</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" ref="AD8" si="77">ROUND(AC8*1.01,0)</f>
+        <v>5973</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" ref="AE8" si="78">ROUND(AD8*1.01,0)</f>
+        <v>6033</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" ref="AF8" si="79">ROUND(AE8*1.01,0)</f>
+        <v>6093</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" ref="AG8" si="80">ROUND(AF8*1.01,0)</f>
+        <v>6154</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" ref="AH8" si="81">ROUND(AG8*1.01,0)</f>
+        <v>6216</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" ref="AI8" si="82">ROUND(AH8*1.01,0)</f>
+        <v>6278</v>
+      </c>
+      <c r="AJ8">
+        <f t="shared" ref="AJ8" si="83">ROUND(AI8*1.01,0)</f>
+        <v>6341</v>
+      </c>
+      <c r="AK8">
+        <f t="shared" ref="AK8" si="84">ROUND(AJ8*1.01,0)</f>
+        <v>6404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -986,7 +1478,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -995,11 +1487,11 @@
         <v>105000</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:S10" si="22">SUM(C3:C8)</f>
+        <f t="shared" ref="C10:S10" si="85">SUM(C3:C8)</f>
         <v>105000</v>
       </c>
       <c r="D10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>105000</v>
       </c>
       <c r="E10">
@@ -1007,11 +1499,11 @@
         <v>153600</v>
       </c>
       <c r="F10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>110392</v>
       </c>
       <c r="G10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>114200</v>
       </c>
       <c r="H10">
@@ -1019,67 +1511,135 @@
         <v>49869</v>
       </c>
       <c r="I10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>50803</v>
       </c>
       <c r="J10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>51754</v>
       </c>
       <c r="K10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>68324</v>
       </c>
       <c r="L10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>69625</v>
       </c>
       <c r="M10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>70951</v>
       </c>
       <c r="N10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>72303</v>
       </c>
       <c r="O10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>109682</v>
       </c>
       <c r="P10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>111807</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>102970</v>
       </c>
       <c r="R10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>104958</v>
       </c>
       <c r="S10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="85"/>
         <v>106987</v>
       </c>
       <c r="T10">
         <f>SUM(T3:T8)</f>
         <v>109055</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <f t="shared" ref="U10:Z10" si="86">SUM(U3:U8)</f>
+        <v>111164</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="86"/>
+        <v>113314</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="86"/>
+        <v>115506</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="86"/>
+        <v>117742</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="86"/>
+        <v>120021</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="86"/>
+        <v>122345</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" ref="AA10:AK10" si="87">SUM(AA3:AA8)</f>
+        <v>124714</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="87"/>
+        <v>127131</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="87"/>
+        <v>129596</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="87"/>
+        <v>132108</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="87"/>
+        <v>134669</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="87"/>
+        <v>137280</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="87"/>
+        <v>139943</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="87"/>
+        <v>142659</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="87"/>
+        <v>145427</v>
+      </c>
+      <c r="AJ10">
+        <f t="shared" si="87"/>
+        <v>148251</v>
+      </c>
+      <c r="AK10">
+        <f t="shared" si="87"/>
+        <v>151129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12">
-        <f>(B10-B20) *C27</f>
+        <f>(B10-B20) *C32</f>
         <v>78750</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12" si="23">C10-C20</f>
+        <f t="shared" ref="C12" si="88">C10-C20</f>
         <v>105000</v>
       </c>
       <c r="D12">
@@ -1087,71 +1647,139 @@
         <v>105000</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:T12" si="24">E10-E20</f>
+        <f t="shared" ref="E12:T12" si="89">E10-E20</f>
         <v>153600</v>
       </c>
       <c r="F12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>110392</v>
       </c>
       <c r="G12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>114200</v>
       </c>
       <c r="H12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>105771</v>
       </c>
       <c r="I12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>109934</v>
       </c>
       <c r="J12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>113102</v>
       </c>
       <c r="K12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>117650</v>
       </c>
       <c r="L12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>122426</v>
       </c>
       <c r="M12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>127446</v>
       </c>
       <c r="N12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>132724</v>
       </c>
       <c r="O12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>138277</v>
       </c>
       <c r="P12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>129722</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>135446</v>
       </c>
       <c r="R12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>141488</v>
       </c>
       <c r="S12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>147870</v>
       </c>
       <c r="T12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="89"/>
         <v>154614</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <f t="shared" ref="U12:Z12" si="90">U10-U20</f>
+        <v>161746</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="90"/>
+        <v>169291</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="90"/>
+        <v>177277</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="90"/>
+        <v>185736</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="90"/>
+        <v>194700</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="90"/>
+        <v>204204</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" ref="AA12:AK12" si="91">AA10-AA20</f>
+        <v>214286</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="91"/>
+        <v>224987</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="91"/>
+        <v>236351</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="91"/>
+        <v>248425</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="91"/>
+        <v>261260</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="91"/>
+        <v>274910</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="91"/>
+        <v>289435</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="91"/>
+        <v>304898</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="91"/>
+        <v>321368</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" si="91"/>
+        <v>338917</v>
+      </c>
+      <c r="AK12">
+        <f t="shared" si="91"/>
+        <v>357625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1168,83 +1796,151 @@
         <v>21783</v>
       </c>
       <c r="E13">
-        <f>ROUND((9500 + 0.25*(E12-E9+$B$26-88000) + E3 * 0.0765),0)</f>
+        <f>ROUND((9500 + 0.25*(E12-E9+$B$31-88000) + E3 * 0.0765),0)</f>
         <v>35308</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:T13" si="25">ROUND((9500 + 0.25*(F12+$B$26- 88000) + F3 * 0.0765),0)</f>
+        <f t="shared" ref="F13:T13" si="92">ROUND((9500 + 0.25*(F12+$B$31- 88000) + F3 * 0.0765),0)</f>
         <v>24078</v>
       </c>
       <c r="G13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>25030</v>
       </c>
       <c r="H13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>17568</v>
       </c>
       <c r="I13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>18609</v>
       </c>
       <c r="J13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>19401</v>
       </c>
       <c r="K13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>20538</v>
       </c>
       <c r="L13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>21732</v>
       </c>
       <c r="M13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>22987</v>
       </c>
       <c r="N13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>24306</v>
       </c>
       <c r="O13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>25694</v>
       </c>
       <c r="P13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>23556</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>24987</v>
       </c>
       <c r="R13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>26497</v>
       </c>
       <c r="S13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>28093</v>
       </c>
       <c r="T13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="92"/>
         <v>29779</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <f t="shared" ref="U13:Z13" si="93">ROUND((9500 + 0.25*(U12+$B$31- 88000) + U3 * 0.0765),0)</f>
+        <v>31562</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="93"/>
+        <v>33448</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="93"/>
+        <v>35444</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="93"/>
+        <v>37559</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="93"/>
+        <v>39800</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="93"/>
+        <v>42176</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" ref="AA13:AK13" si="94">ROUND((9500 + 0.25*(AA12+$B$31- 88000) + AA3 * 0.0765),0)</f>
+        <v>44697</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="94"/>
+        <v>47372</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="94"/>
+        <v>50213</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="94"/>
+        <v>53231</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="94"/>
+        <v>56440</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="94"/>
+        <v>59853</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="94"/>
+        <v>63484</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="94"/>
+        <v>67350</v>
+      </c>
+      <c r="AI13">
+        <f t="shared" si="94"/>
+        <v>71467</v>
+      </c>
+      <c r="AJ13">
+        <f t="shared" si="94"/>
+        <v>75854</v>
+      </c>
+      <c r="AK13">
+        <f t="shared" si="94"/>
+        <v>80531</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B15">
-        <f>72000*C27</f>
+        <f>72000*C32</f>
         <v>54000</v>
       </c>
       <c r="C15">
-        <f>ROUND((B15/C27)*1.03,0)</f>
+        <f>ROUND((B15/C32)*1.03,0)</f>
         <v>74160</v>
       </c>
       <c r="D15">
@@ -1256,19 +1952,19 @@
         <v>78677</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:L15" si="26">ROUND(E15*1.03,0)</f>
+        <f t="shared" ref="F15:L15" si="95">ROUND(E15*1.03,0)</f>
         <v>81037</v>
       </c>
       <c r="G15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="95"/>
         <v>83468</v>
       </c>
       <c r="H15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="95"/>
         <v>85972</v>
       </c>
       <c r="I15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="95"/>
         <v>88551</v>
       </c>
       <c r="J15">
@@ -1276,23 +1972,23 @@
         <v>90008</v>
       </c>
       <c r="K15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="95"/>
         <v>92708</v>
       </c>
       <c r="L15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="95"/>
         <v>95489</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15" si="27">ROUND(L15*1.03,0)</f>
+        <f t="shared" ref="M15" si="96">ROUND(L15*1.03,0)</f>
         <v>98354</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15" si="28">ROUND(M15*1.03,0)</f>
+        <f t="shared" ref="N15" si="97">ROUND(M15*1.03,0)</f>
         <v>101305</v>
       </c>
       <c r="O15">
-        <f t="shared" ref="O15" si="29">ROUND(N15*1.03,0)</f>
+        <f t="shared" ref="O15" si="98">ROUND(N15*1.03,0)</f>
         <v>104344</v>
       </c>
       <c r="P15">
@@ -1315,21 +2011,89 @@
         <f>ROUND(S15*1.03,0)</f>
         <v>104755</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <f t="shared" ref="U15:Z15" si="99">ROUND(T15*1.03,0)</f>
+        <v>107898</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="99"/>
+        <v>111135</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="99"/>
+        <v>114469</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="99"/>
+        <v>117903</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="99"/>
+        <v>121440</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="99"/>
+        <v>125083</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" ref="AA15" si="100">ROUND(Z15*1.03,0)</f>
+        <v>128835</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" ref="AB15" si="101">ROUND(AA15*1.03,0)</f>
+        <v>132700</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" ref="AC15" si="102">ROUND(AB15*1.03,0)</f>
+        <v>136681</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" ref="AD15" si="103">ROUND(AC15*1.03,0)</f>
+        <v>140781</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" ref="AE15" si="104">ROUND(AD15*1.03,0)</f>
+        <v>145004</v>
+      </c>
+      <c r="AF15">
+        <f t="shared" ref="AF15" si="105">ROUND(AE15*1.03,0)</f>
+        <v>149354</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" ref="AG15" si="106">ROUND(AF15*1.03,0)</f>
+        <v>153835</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" ref="AH15" si="107">ROUND(AG15*1.03,0)</f>
+        <v>158450</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" ref="AI15" si="108">ROUND(AH15*1.03,0)</f>
+        <v>163204</v>
+      </c>
+      <c r="AJ15">
+        <f t="shared" ref="AJ15" si="109">ROUND(AI15*1.03,0)</f>
+        <v>168100</v>
+      </c>
+      <c r="AK15">
+        <f t="shared" ref="AK15" si="110">ROUND(AJ15*1.03,0)</f>
+        <v>173143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B16">
-        <f>12000*C27</f>
+        <f>12000*C32</f>
         <v>9000</v>
       </c>
       <c r="C16">
-        <f>ROUND((B16/C27)*1.08,0)</f>
+        <f>ROUND((B16/C32)*1.08,0)</f>
         <v>12960</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:L16" si="30">ROUND(C16*1.08,0)</f>
+        <f t="shared" ref="D16:L16" si="111">ROUND(C16*1.08,0)</f>
         <v>13997</v>
       </c>
       <c r="E16">
@@ -1337,67 +2101,135 @@
         <v>15717</v>
       </c>
       <c r="F16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="111"/>
         <v>16974</v>
       </c>
       <c r="G16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="111"/>
         <v>18332</v>
       </c>
       <c r="H16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="111"/>
         <v>19799</v>
       </c>
       <c r="I16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="111"/>
         <v>21383</v>
       </c>
       <c r="J16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="111"/>
         <v>23094</v>
       </c>
       <c r="K16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="111"/>
         <v>24942</v>
       </c>
       <c r="L16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="111"/>
         <v>26937</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16" si="31">ROUND(L16*1.08,0)</f>
+        <f t="shared" ref="M16" si="112">ROUND(L16*1.08,0)</f>
         <v>29092</v>
       </c>
       <c r="N16">
-        <f t="shared" ref="N16" si="32">ROUND(M16*1.08,0)</f>
+        <f t="shared" ref="N16" si="113">ROUND(M16*1.08,0)</f>
         <v>31419</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16" si="33">ROUND(N16*1.08,0)</f>
+        <f t="shared" ref="O16" si="114">ROUND(N16*1.08,0)</f>
         <v>33933</v>
       </c>
       <c r="P16">
-        <f t="shared" ref="P16" si="34">ROUND(O16*1.08,0)</f>
+        <f t="shared" ref="P16" si="115">ROUND(O16*1.08,0)</f>
         <v>36648</v>
       </c>
       <c r="Q16">
-        <f t="shared" ref="Q16" si="35">ROUND(P16*1.08,0)</f>
+        <f t="shared" ref="Q16" si="116">ROUND(P16*1.08,0)</f>
         <v>39580</v>
       </c>
       <c r="R16">
-        <f t="shared" ref="R16" si="36">ROUND(Q16*1.08,0)</f>
+        <f t="shared" ref="R16" si="117">ROUND(Q16*1.08,0)</f>
         <v>42746</v>
       </c>
       <c r="S16">
-        <f t="shared" ref="S16:T16" si="37">ROUND(R16*1.08,0)</f>
+        <f t="shared" ref="S16:T16" si="118">ROUND(R16*1.08,0)</f>
         <v>46166</v>
       </c>
       <c r="T16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="118"/>
         <v>49859</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <f t="shared" ref="U16" si="119">ROUND(T16*1.08,0)</f>
+        <v>53848</v>
+      </c>
+      <c r="V16">
+        <f t="shared" ref="V16" si="120">ROUND(U16*1.08,0)</f>
+        <v>58156</v>
+      </c>
+      <c r="W16">
+        <f t="shared" ref="W16" si="121">ROUND(V16*1.08,0)</f>
+        <v>62808</v>
+      </c>
+      <c r="X16">
+        <f t="shared" ref="X16" si="122">ROUND(W16*1.08,0)</f>
+        <v>67833</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" ref="Y16" si="123">ROUND(X16*1.08,0)</f>
+        <v>73260</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" ref="Z16" si="124">ROUND(Y16*1.08,0)</f>
+        <v>79121</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" ref="AA16" si="125">ROUND(Z16*1.08,0)</f>
+        <v>85451</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" ref="AB16" si="126">ROUND(AA16*1.08,0)</f>
+        <v>92287</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" ref="AC16" si="127">ROUND(AB16*1.08,0)</f>
+        <v>99670</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" ref="AD16" si="128">ROUND(AC16*1.08,0)</f>
+        <v>107644</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" ref="AE16" si="129">ROUND(AD16*1.08,0)</f>
+        <v>116256</v>
+      </c>
+      <c r="AF16">
+        <f t="shared" ref="AF16" si="130">ROUND(AE16*1.08,0)</f>
+        <v>125556</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" ref="AG16" si="131">ROUND(AF16*1.08,0)</f>
+        <v>135600</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" ref="AH16" si="132">ROUND(AG16*1.08,0)</f>
+        <v>146448</v>
+      </c>
+      <c r="AI16">
+        <f t="shared" ref="AI16" si="133">ROUND(AH16*1.08,0)</f>
+        <v>158164</v>
+      </c>
+      <c r="AJ16">
+        <f t="shared" ref="AJ16" si="134">ROUND(AI16*1.08,0)</f>
+        <v>170817</v>
+      </c>
+      <c r="AK16">
+        <f t="shared" ref="AK16" si="135">ROUND(AJ16*1.08,0)</f>
+        <v>184482</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1405,7 +2237,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -1414,7 +2246,7 @@
         <v>63000</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:S18" si="38">(C15+C16)</f>
+        <f t="shared" ref="C18:S18" si="136">(C15+C16)</f>
         <v>87120</v>
       </c>
       <c r="D18">
@@ -1422,74 +2254,142 @@
         <v>98382</v>
       </c>
       <c r="E18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>94394</v>
       </c>
       <c r="F18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>98011</v>
       </c>
       <c r="G18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>101800</v>
       </c>
       <c r="H18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>105771</v>
       </c>
       <c r="I18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>109934</v>
       </c>
       <c r="J18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>113102</v>
       </c>
       <c r="K18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>117650</v>
       </c>
       <c r="L18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>122426</v>
       </c>
       <c r="M18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>127446</v>
       </c>
       <c r="N18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>132724</v>
       </c>
       <c r="O18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>138277</v>
       </c>
       <c r="P18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>129722</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>135446</v>
       </c>
       <c r="R18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>141488</v>
       </c>
       <c r="S18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="136"/>
         <v>147870</v>
       </c>
       <c r="T18">
-        <f t="shared" ref="T18" si="39">(T15+T16)</f>
+        <f t="shared" ref="T18" si="137">(T15+T16)</f>
         <v>154614</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <f t="shared" ref="U18:Z18" si="138">(U15+U16)</f>
+        <v>161746</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="138"/>
+        <v>169291</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="138"/>
+        <v>177277</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="138"/>
+        <v>185736</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="138"/>
+        <v>194700</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="138"/>
+        <v>204204</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" ref="AA18:AK18" si="139">(AA15+AA16)</f>
+        <v>214286</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="139"/>
+        <v>224987</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="139"/>
+        <v>236351</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="139"/>
+        <v>248425</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="139"/>
+        <v>261260</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="139"/>
+        <v>274910</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" si="139"/>
+        <v>289435</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="139"/>
+        <v>304898</v>
+      </c>
+      <c r="AI18">
+        <f t="shared" si="139"/>
+        <v>321368</v>
+      </c>
+      <c r="AJ18">
+        <f t="shared" si="139"/>
+        <v>338917</v>
+      </c>
+      <c r="AK18">
+        <f t="shared" si="139"/>
+        <v>357625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1512,64 +2412,132 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:T20" si="40">H10-H18</f>
+        <f t="shared" ref="H20:T20" si="140">H10-H18</f>
         <v>-55902</v>
       </c>
       <c r="I20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-59131</v>
       </c>
       <c r="J20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-61348</v>
       </c>
       <c r="K20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-49326</v>
       </c>
       <c r="L20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-52801</v>
       </c>
       <c r="M20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-56495</v>
       </c>
       <c r="N20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-60421</v>
       </c>
       <c r="O20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-28595</v>
       </c>
       <c r="P20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-17915</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-32476</v>
       </c>
       <c r="R20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-36530</v>
       </c>
       <c r="S20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-40883</v>
       </c>
       <c r="T20">
-        <f t="shared" si="40"/>
+        <f t="shared" si="140"/>
         <v>-45559</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <f t="shared" ref="U20:Z20" si="141">U10-U18</f>
+        <v>-50582</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="141"/>
+        <v>-55977</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="141"/>
+        <v>-61771</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="141"/>
+        <v>-67994</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="141"/>
+        <v>-74679</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="141"/>
+        <v>-81859</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" ref="AA20:AK20" si="142">AA10-AA18</f>
+        <v>-89572</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="142"/>
+        <v>-97856</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="142"/>
+        <v>-106755</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="142"/>
+        <v>-116317</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="142"/>
+        <v>-126591</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="142"/>
+        <v>-137630</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" si="142"/>
+        <v>-149492</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="142"/>
+        <v>-162239</v>
+      </c>
+      <c r="AI20">
+        <f t="shared" si="142"/>
+        <v>-175941</v>
+      </c>
+      <c r="AJ20">
+        <f t="shared" si="142"/>
+        <v>-190666</v>
+      </c>
+      <c r="AK20">
+        <f t="shared" si="142"/>
+        <v>-206496</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21">
-        <f>B10*C27-B13-B18</f>
+        <f>B10*C32-B13-B18</f>
         <v>-395</v>
       </c>
       <c r="C21">
@@ -1585,11 +2553,11 @@
         <v>23898</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:G21" si="41">F10-F13-F18</f>
+        <f t="shared" ref="F21:G21" si="143">F10-F13-F18</f>
         <v>-11697</v>
       </c>
       <c r="G21">
-        <f t="shared" si="41"/>
+        <f t="shared" si="143"/>
         <v>-12630</v>
       </c>
       <c r="H21">
@@ -1597,58 +2565,126 @@
         <v>-17568</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:T21" si="42">-I13</f>
+        <f t="shared" ref="I21:T21" si="144">-I13</f>
         <v>-18609</v>
       </c>
       <c r="J21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-19401</v>
       </c>
       <c r="K21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-20538</v>
       </c>
       <c r="L21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-21732</v>
       </c>
       <c r="M21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-22987</v>
       </c>
       <c r="N21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-24306</v>
       </c>
       <c r="O21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-25694</v>
       </c>
       <c r="P21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-23556</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-24987</v>
       </c>
       <c r="R21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-26497</v>
       </c>
       <c r="S21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-28093</v>
       </c>
       <c r="T21">
-        <f t="shared" si="42"/>
+        <f t="shared" si="144"/>
         <v>-29779</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <f t="shared" ref="U21:Z21" si="145">-U13</f>
+        <v>-31562</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="145"/>
+        <v>-33448</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="145"/>
+        <v>-35444</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="145"/>
+        <v>-37559</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="145"/>
+        <v>-39800</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="145"/>
+        <v>-42176</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" ref="AA21:AK21" si="146">-AA13</f>
+        <v>-44697</v>
+      </c>
+      <c r="AB21">
+        <f t="shared" si="146"/>
+        <v>-47372</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" si="146"/>
+        <v>-50213</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="146"/>
+        <v>-53231</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" si="146"/>
+        <v>-56440</v>
+      </c>
+      <c r="AF21">
+        <f t="shared" si="146"/>
+        <v>-59853</v>
+      </c>
+      <c r="AG21">
+        <f t="shared" si="146"/>
+        <v>-63484</v>
+      </c>
+      <c r="AH21">
+        <f t="shared" si="146"/>
+        <v>-67350</v>
+      </c>
+      <c r="AI21">
+        <f t="shared" si="146"/>
+        <v>-71467</v>
+      </c>
+      <c r="AJ21">
+        <f t="shared" si="146"/>
+        <v>-75854</v>
+      </c>
+      <c r="AK21">
+        <f t="shared" si="146"/>
+        <v>-80531</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1665,71 +2701,139 @@
         <v>646134</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:T23" si="43">ROUND((D23-$B$26+E20)*1.025,0)</f>
+        <f t="shared" ref="E23:T23" si="147">ROUND((D23-$B$31+E20)*1.025,0)</f>
         <v>647425</v>
       </c>
       <c r="F23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>648748</v>
       </c>
       <c r="G23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>650104</v>
       </c>
       <c r="H23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>594195</v>
       </c>
       <c r="I23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>533578</v>
       </c>
       <c r="J23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>469173</v>
       </c>
       <c r="K23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>415481</v>
       </c>
       <c r="L23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>356885</v>
       </c>
       <c r="M23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>293037</v>
       </c>
       <c r="N23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>223569</v>
       </c>
       <c r="O23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>184986</v>
       </c>
       <c r="P23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>156385</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>112144</v>
       </c>
       <c r="R23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>62642</v>
       </c>
       <c r="S23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>7440</v>
       </c>
       <c r="T23">
-        <f t="shared" si="43"/>
+        <f t="shared" si="147"/>
         <v>-53934</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <f t="shared" ref="U23" si="148">ROUND((T23-$B$31+U20)*1.025,0)</f>
+        <v>-121991</v>
+      </c>
+      <c r="V23">
+        <f t="shared" ref="V23" si="149">ROUND((U23-$B$31+V20)*1.025,0)</f>
+        <v>-197280</v>
+      </c>
+      <c r="W23">
+        <f t="shared" ref="W23" si="150">ROUND((V23-$B$31+W20)*1.025,0)</f>
+        <v>-280390</v>
+      </c>
+      <c r="X23">
+        <f t="shared" ref="X23" si="151">ROUND((W23-$B$31+X20)*1.025,0)</f>
+        <v>-371956</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" ref="Y23" si="152">ROUND((X23-$B$31+Y20)*1.025,0)</f>
+        <v>-472663</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" ref="Z23" si="153">ROUND((Y23-$B$31+Z20)*1.025,0)</f>
+        <v>-583248</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" ref="AA23" si="154">ROUND((Z23-$B$31+AA20)*1.025,0)</f>
+        <v>-704503</v>
+      </c>
+      <c r="AB23">
+        <f t="shared" ref="AB23" si="155">ROUND((AA23-$B$31+AB20)*1.025,0)</f>
+        <v>-837280</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" ref="AC23" si="156">ROUND((AB23-$B$31+AC20)*1.025,0)</f>
+        <v>-982498</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" ref="AD23" si="157">ROUND((AC23-$B$31+AD20)*1.025,0)</f>
+        <v>-1141148</v>
+      </c>
+      <c r="AE23">
+        <f t="shared" ref="AE23" si="158">ROUND((AD23-$B$31+AE20)*1.025,0)</f>
+        <v>-1314295</v>
+      </c>
+      <c r="AF23">
+        <f t="shared" ref="AF23" si="159">ROUND((AE23-$B$31+AF20)*1.025,0)</f>
+        <v>-1503086</v>
+      </c>
+      <c r="AG23">
+        <f t="shared" ref="AG23" si="160">ROUND((AF23-$B$31+AG20)*1.025,0)</f>
+        <v>-1708755</v>
+      </c>
+      <c r="AH23">
+        <f t="shared" ref="AH23" si="161">ROUND((AG23-$B$31+AH20)*1.025,0)</f>
+        <v>-1932631</v>
+      </c>
+      <c r="AI23">
+        <f t="shared" ref="AI23" si="162">ROUND((AH23-$B$31+AI20)*1.025,0)</f>
+        <v>-2176149</v>
+      </c>
+      <c r="AJ23">
+        <f t="shared" ref="AJ23" si="163">ROUND((AI23-$B$31+AJ20)*1.025,0)</f>
+        <v>-2440848</v>
+      </c>
+      <c r="AK23">
+        <f t="shared" ref="AK23" si="164">ROUND((AJ23-$B$31+AK20)*1.025,0)</f>
+        <v>-2728390</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1746,140 +2850,479 @@
         <v>44543</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:T24" si="44">ROUND((D24+E21 + $B$26)*1.025,0)</f>
+        <f t="shared" ref="E24:T24" si="165">ROUND((D24+E21 + $B$31)*1.025,0)</f>
         <v>85015</v>
       </c>
       <c r="F24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>90013</v>
       </c>
       <c r="G24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>94180</v>
       </c>
       <c r="H24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>93390</v>
       </c>
       <c r="I24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>91513</v>
       </c>
       <c r="J24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>88777</v>
       </c>
       <c r="K24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>84807</v>
       </c>
       <c r="L24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>79514</v>
       </c>
       <c r="M24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>72803</v>
       </c>
       <c r="N24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>64572</v>
       </c>
       <c r="O24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>54712</v>
       </c>
       <c r="P24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>46797</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>37218</v>
       </c>
       <c r="R24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>25852</v>
       </c>
       <c r="S24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>12565</v>
       </c>
       <c r="T24">
-        <f t="shared" si="44"/>
+        <f t="shared" si="165"/>
         <v>-2782</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <f t="shared" ref="U24" si="166">ROUND((T24+U21 + $B$31)*1.025,0)</f>
+        <v>-20340</v>
+      </c>
+      <c r="V24">
+        <f t="shared" ref="V24" si="167">ROUND((U24+V21 + $B$31)*1.025,0)</f>
+        <v>-40270</v>
+      </c>
+      <c r="W24">
+        <f t="shared" ref="W24" si="168">ROUND((V24+W21 + $B$31)*1.025,0)</f>
+        <v>-62744</v>
+      </c>
+      <c r="X24">
+        <f t="shared" ref="X24" si="169">ROUND((W24+X21 + $B$31)*1.025,0)</f>
+        <v>-87948</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" ref="Y24" si="170">ROUND((X24+Y21 + $B$31)*1.025,0)</f>
+        <v>-116079</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" ref="Z24" si="171">ROUND((Y24+Z21 + $B$31)*1.025,0)</f>
+        <v>-147349</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" ref="AA24" si="172">ROUND((Z24+AA21 + $B$31)*1.025,0)</f>
+        <v>-181985</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" ref="AB24" si="173">ROUND((AA24+AB21 + $B$31)*1.025,0)</f>
+        <v>-220228</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" ref="AC24" si="174">ROUND((AB24+AC21 + $B$31)*1.025,0)</f>
+        <v>-262340</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" ref="AD24" si="175">ROUND((AC24+AD21 + $B$31)*1.025,0)</f>
+        <v>-308598</v>
+      </c>
+      <c r="AE24">
+        <f t="shared" ref="AE24" si="176">ROUND((AD24+AE21 + $B$31)*1.025,0)</f>
+        <v>-359301</v>
+      </c>
+      <c r="AF24">
+        <f t="shared" ref="AF24" si="177">ROUND((AE24+AF21 + $B$31)*1.025,0)</f>
+        <v>-414770</v>
+      </c>
+      <c r="AG24">
+        <f t="shared" ref="AG24" si="178">ROUND((AF24+AG21 + $B$31)*1.025,0)</f>
+        <v>-475348</v>
+      </c>
+      <c r="AH24">
+        <f t="shared" ref="AH24" si="179">ROUND((AG24+AH21 + $B$31)*1.025,0)</f>
+        <v>-541403</v>
+      </c>
+      <c r="AI24">
+        <f t="shared" ref="AI24" si="180">ROUND((AH24+AI21 + $B$31)*1.025,0)</f>
+        <v>-613329</v>
+      </c>
+      <c r="AJ24">
+        <f t="shared" ref="AJ24" si="181">ROUND((AI24+AJ21 + $B$31)*1.025,0)</f>
+        <v>-691550</v>
+      </c>
+      <c r="AK24">
+        <f t="shared" ref="AK24" si="182">ROUND((AJ24+AK21 + $B$31)*1.025,0)</f>
+        <v>-776521</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P26">
+        <v>156384</v>
+      </c>
+      <c r="Q26">
+        <v>112141</v>
+      </c>
+      <c r="R26">
+        <v>62637</v>
+      </c>
+      <c r="S26">
+        <v>7432</v>
+      </c>
+      <c r="T26">
+        <v>-53945</v>
+      </c>
+      <c r="U26">
+        <v>-122005</v>
+      </c>
+      <c r="V26">
+        <v>-197296</v>
+      </c>
+      <c r="W26">
+        <v>-280406</v>
+      </c>
+      <c r="X26">
+        <v>-371975</v>
+      </c>
+      <c r="Y26">
+        <v>-472684</v>
+      </c>
+      <c r="Z26">
+        <v>-583270</v>
+      </c>
+      <c r="AK26">
+        <v>-2728454</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P27">
+        <v>46795</v>
+      </c>
+      <c r="Q27">
+        <v>37216</v>
+      </c>
+      <c r="R27">
+        <v>25849</v>
+      </c>
+      <c r="S27">
+        <v>12562</v>
+      </c>
+      <c r="T27">
+        <v>-2785</v>
+      </c>
+      <c r="U27">
+        <v>-20343</v>
+      </c>
+      <c r="V27">
+        <v>-40273</v>
+      </c>
+      <c r="W27">
+        <v>-62747</v>
+      </c>
+      <c r="X27">
+        <v>-87951</v>
+      </c>
+      <c r="Y27">
+        <v>-116082</v>
+      </c>
+      <c r="Z27">
+        <v>-147352</v>
+      </c>
+      <c r="AK27">
+        <v>-776525</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P28">
+        <f>P23-P26</f>
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" ref="Q28:Z28" si="183">Q23-Q26</f>
+        <v>3</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="183"/>
+        <v>5</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="183"/>
+        <v>8</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="183"/>
+        <v>11</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="183"/>
+        <v>14</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="183"/>
+        <v>16</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="183"/>
+        <v>16</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="183"/>
+        <v>19</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="183"/>
+        <v>21</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="183"/>
+        <v>22</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" ref="AA28:AK28" si="184">AA23-AA26</f>
+        <v>-704503</v>
+      </c>
+      <c r="AB28">
+        <f t="shared" si="184"/>
+        <v>-837280</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="184"/>
+        <v>-982498</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="184"/>
+        <v>-1141148</v>
+      </c>
+      <c r="AE28">
+        <f t="shared" si="184"/>
+        <v>-1314295</v>
+      </c>
+      <c r="AF28">
+        <f t="shared" si="184"/>
+        <v>-1503086</v>
+      </c>
+      <c r="AG28">
+        <f t="shared" si="184"/>
+        <v>-1708755</v>
+      </c>
+      <c r="AH28">
+        <f t="shared" si="184"/>
+        <v>-1932631</v>
+      </c>
+      <c r="AI28">
+        <f t="shared" si="184"/>
+        <v>-2176149</v>
+      </c>
+      <c r="AJ28">
+        <f t="shared" si="184"/>
+        <v>-2440848</v>
+      </c>
+      <c r="AK28">
+        <f t="shared" si="184"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P29">
+        <f>P24-P27</f>
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" ref="Q29:Z29" si="185">Q24-Q27</f>
+        <v>2</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="185"/>
+        <v>3</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" ref="AA29:AK29" si="186">AA24-AA27</f>
+        <v>-181985</v>
+      </c>
+      <c r="AB29">
+        <f t="shared" si="186"/>
+        <v>-220228</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="186"/>
+        <v>-262340</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="186"/>
+        <v>-308598</v>
+      </c>
+      <c r="AE29">
+        <f t="shared" si="186"/>
+        <v>-359301</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" si="186"/>
+        <v>-414770</v>
+      </c>
+      <c r="AG29">
+        <f t="shared" si="186"/>
+        <v>-475348</v>
+      </c>
+      <c r="AH29">
+        <f t="shared" si="186"/>
+        <v>-541403</v>
+      </c>
+      <c r="AI29">
+        <f t="shared" si="186"/>
+        <v>-613329</v>
+      </c>
+      <c r="AJ29">
+        <f t="shared" si="186"/>
+        <v>-691550</v>
+      </c>
+      <c r="AK29">
+        <f t="shared" si="186"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B31">
         <v>14500</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B32" t="s">
         <v>30</v>
       </c>
-      <c r="C27">
+      <c r="C32">
         <v>0.75</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Combined monthly non-medical expenses to single monthly amount
</commit_message>
<xml_diff>
--- a/test/TestCalculations.xlsx
+++ b/test/TestCalculations.xlsx
@@ -562,11 +562,11 @@
   <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2925" ySplit="690" topLeftCell="A2" activePane="bottomRight"/>
+      <pane xSplit="2925" ySplit="690" topLeftCell="Y2" activePane="bottomRight"/>
       <selection activeCell="A19" sqref="A19"/>
       <selection pane="topRight" sqref="A1:A1048576"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,7 +826,7 @@
         <v>84</v>
       </c>
       <c r="AA2" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="AB2" s="1">
         <v>86</v>
@@ -1934,7 +1934,7 @@
         <v>5165</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="B14:AH14" si="47">ROUND((1700 + 0.15*(C13- 36000)),0)</f>
+        <f t="shared" ref="C14:G14" si="47">ROUND((1700 + 0.15*(C13- 36000)),0)</f>
         <v>9059</v>
       </c>
       <c r="D14">

</xml_diff>

<commit_message>
Put tax brackets in yml file and updated to 2014. Added items to results.yml and annual expenses for property taxes, insurance and dues.
</commit_message>
<xml_diff>
--- a/test/TestCalculations.xlsx
+++ b/test/TestCalculations.xlsx
@@ -15,46 +15,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>richard.reed@improvingenterprises.com</author>
-  </authors>
-  <commentList>
-    <comment ref="H14" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Over $88k, 25% tax formula</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M27" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Year</t>
   </si>
@@ -129,18 +91,6 @@
   </si>
   <si>
     <t>Expenses (final_annual_expenses)</t>
-  </si>
-  <si>
-    <t>Calculated IRA Savings</t>
-  </si>
-  <si>
-    <t>Calculated non-IRA Savings</t>
-  </si>
-  <si>
-    <t>IRA Sav - Cal IRA Sav</t>
-  </si>
-  <si>
-    <t>non-IRA Sav - Calc non-IRA Sav</t>
   </si>
   <si>
     <t>Initial Values:</t>
@@ -204,7 +154,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,17 +174,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,15 +198,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -558,15 +508,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2925" ySplit="690" topLeftCell="Y2" activePane="bottomRight"/>
+      <pane xSplit="2925" ySplit="690" topLeftCell="O6" activePane="bottomLeft"/>
       <selection activeCell="A19" sqref="A19"/>
       <selection pane="topRight" sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="AA2" sqref="AA2"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:XFD30"/>
+      <selection pane="bottomRight" activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,10 +536,22 @@
     <col min="15" max="15" width="8.140625" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
     <col min="17" max="17" width="9.5703125" customWidth="1"/>
-    <col min="18" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="34" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="9" customWidth="1"/>
+    <col min="23" max="23" width="8.28515625" customWidth="1"/>
+    <col min="24" max="24" width="7.85546875" customWidth="1"/>
+    <col min="25" max="25" width="7.28515625" customWidth="1"/>
+    <col min="26" max="27" width="7.85546875" customWidth="1"/>
+    <col min="28" max="28" width="9" customWidth="1"/>
+    <col min="29" max="29" width="9.5703125" customWidth="1"/>
+    <col min="30" max="30" width="8.28515625" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" customWidth="1"/>
+    <col min="33" max="33" width="9.5703125" customWidth="1"/>
+    <col min="34" max="34" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -858,135 +820,135 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f>$N$33</f>
+        <f>$N$29</f>
         <v>39600</v>
       </c>
       <c r="C3">
-        <f>ROUND($N$33*$O$33,0)</f>
+        <f>ROUND($N$29*$O$29,0)</f>
         <v>40392</v>
       </c>
       <c r="D3">
-        <f>ROUND(C3*$O$33,0)</f>
+        <f>ROUND(C3*$O$29,0)</f>
         <v>41200</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:AH3" si="34">ROUND(D3*$O$33,0)</f>
+        <f>ROUND(D3*$O$29,0)</f>
         <v>42024</v>
       </c>
       <c r="F3">
-        <f t="shared" si="34"/>
+        <f>ROUND(E3*$O$29,0)</f>
         <v>42864</v>
       </c>
       <c r="G3">
-        <f t="shared" si="34"/>
+        <f>ROUND(F3*$O$29,0)</f>
         <v>43721</v>
       </c>
       <c r="H3">
-        <f t="shared" si="34"/>
+        <f>ROUND(G3*$O$29,0)</f>
         <v>44595</v>
       </c>
       <c r="I3">
-        <f t="shared" si="34"/>
+        <f>ROUND(H3*$O$29,0)</f>
         <v>45487</v>
       </c>
       <c r="J3">
-        <f t="shared" si="34"/>
+        <f>ROUND(I3*$O$29,0)</f>
         <v>46397</v>
       </c>
       <c r="K3">
-        <f t="shared" si="34"/>
+        <f>ROUND(J3*$O$29,0)</f>
         <v>47325</v>
       </c>
       <c r="L3">
-        <f t="shared" si="34"/>
+        <f>ROUND(K3*$O$29,0)</f>
         <v>48272</v>
       </c>
       <c r="M3">
-        <f t="shared" si="34"/>
+        <f>ROUND(L3*$O$29,0)</f>
         <v>49237</v>
       </c>
       <c r="N3">
-        <f t="shared" si="34"/>
+        <f>ROUND(M3*$O$29,0)</f>
         <v>50222</v>
       </c>
       <c r="O3">
-        <f t="shared" si="34"/>
+        <f>ROUND(N3*$O$29,0)</f>
         <v>51226</v>
       </c>
       <c r="P3">
-        <f t="shared" si="34"/>
+        <f>ROUND(O3*$O$29,0)</f>
         <v>52251</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="34"/>
+        <f>ROUND(P3*$O$29,0)</f>
         <v>53296</v>
       </c>
       <c r="R3">
-        <f t="shared" si="34"/>
+        <f>ROUND(Q3*$O$29,0)</f>
         <v>54362</v>
       </c>
       <c r="S3">
-        <f t="shared" si="34"/>
+        <f>ROUND(R3*$O$29,0)</f>
         <v>55449</v>
       </c>
       <c r="T3">
-        <f t="shared" si="34"/>
+        <f>ROUND(S3*$O$29,0)</f>
         <v>56558</v>
       </c>
       <c r="U3">
-        <f t="shared" si="34"/>
+        <f>ROUND(T3*$O$29,0)</f>
         <v>57689</v>
       </c>
       <c r="V3">
-        <f t="shared" si="34"/>
+        <f>ROUND(U3*$O$29,0)</f>
         <v>58843</v>
       </c>
       <c r="W3">
-        <f t="shared" si="34"/>
+        <f>ROUND(V3*$O$29,0)</f>
         <v>60020</v>
       </c>
       <c r="X3">
-        <f t="shared" si="34"/>
+        <f>ROUND(W3*$O$29,0)</f>
         <v>61220</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="34"/>
+        <f>ROUND(X3*$O$29,0)</f>
         <v>62444</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="34"/>
+        <f>ROUND(Y3*$O$29,0)</f>
         <v>63693</v>
       </c>
       <c r="AA3">
-        <f t="shared" si="34"/>
+        <f>ROUND(Z3*$O$29,0)</f>
         <v>64967</v>
       </c>
       <c r="AB3">
-        <f t="shared" si="34"/>
+        <f>ROUND(AA3*$O$29,0)</f>
         <v>66266</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="34"/>
+        <f>ROUND(AB3*$O$29,0)</f>
         <v>67591</v>
       </c>
       <c r="AD3">
-        <f t="shared" si="34"/>
+        <f>ROUND(AC3*$O$29,0)</f>
         <v>68943</v>
       </c>
       <c r="AE3">
-        <f t="shared" si="34"/>
+        <f>ROUND(AD3*$O$29,0)</f>
         <v>70322</v>
       </c>
       <c r="AF3">
-        <f t="shared" si="34"/>
+        <f>ROUND(AE3*$O$29,0)</f>
         <v>71728</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="34"/>
+        <f>ROUND(AF3*$O$29,0)</f>
         <v>73163</v>
       </c>
       <c r="AH3">
-        <f t="shared" si="34"/>
+        <f>ROUND(AG3*$O$29,0)</f>
         <v>74626</v>
       </c>
     </row>
@@ -995,184 +957,184 @@
         <v>4</v>
       </c>
       <c r="L4">
-        <f>$N$38</f>
+        <f>$N$34</f>
         <v>36000</v>
       </c>
       <c r="M4">
-        <f>ROUND($N$38*$O$38,0)</f>
+        <f>ROUND($N$34*$O$34,0)</f>
         <v>36720</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:AH4" si="35">ROUND(M4*$O$38,0)</f>
+        <f>ROUND(M4*$O$34,0)</f>
         <v>37454</v>
       </c>
       <c r="O4">
-        <f t="shared" si="35"/>
+        <f>ROUND(N4*$O$34,0)</f>
         <v>38203</v>
       </c>
       <c r="P4">
-        <f t="shared" si="35"/>
+        <f>ROUND(O4*$O$34,0)</f>
         <v>38967</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="35"/>
+        <f>ROUND(P4*$O$34,0)</f>
         <v>39746</v>
       </c>
       <c r="R4">
-        <f t="shared" si="35"/>
+        <f>ROUND(Q4*$O$34,0)</f>
         <v>40541</v>
       </c>
       <c r="S4">
-        <f t="shared" si="35"/>
+        <f>ROUND(R4*$O$34,0)</f>
         <v>41352</v>
       </c>
       <c r="T4">
-        <f t="shared" si="35"/>
+        <f>ROUND(S4*$O$34,0)</f>
         <v>42179</v>
       </c>
       <c r="U4">
-        <f t="shared" si="35"/>
+        <f>ROUND(T4*$O$34,0)</f>
         <v>43023</v>
       </c>
       <c r="V4">
-        <f t="shared" si="35"/>
+        <f>ROUND(U4*$O$34,0)</f>
         <v>43883</v>
       </c>
       <c r="W4">
-        <f t="shared" si="35"/>
+        <f>ROUND(V4*$O$34,0)</f>
         <v>44761</v>
       </c>
       <c r="X4">
-        <f t="shared" si="35"/>
+        <f>ROUND(W4*$O$34,0)</f>
         <v>45656</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="35"/>
+        <f>ROUND(X4*$O$34,0)</f>
         <v>46569</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="35"/>
+        <f>ROUND(Y4*$O$34,0)</f>
         <v>47500</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="35"/>
+        <f>ROUND(Z4*$O$34,0)</f>
         <v>48450</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="35"/>
+        <f>ROUND(AA4*$O$34,0)</f>
         <v>49419</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="35"/>
+        <f>ROUND(AB4*$O$34,0)</f>
         <v>50407</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="35"/>
+        <f>ROUND(AC4*$O$34,0)</f>
         <v>51415</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="35"/>
+        <f>ROUND(AD4*$O$34,0)</f>
         <v>52443</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="35"/>
+        <f>ROUND(AE4*$O$34,0)</f>
         <v>53492</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="35"/>
+        <f>ROUND(AF4*$O$34,0)</f>
         <v>54562</v>
       </c>
       <c r="AH4">
-        <f t="shared" si="35"/>
+        <f>ROUND(AG4*$O$34,0)</f>
         <v>55653</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="N5" s="2">
-        <f>N4*$P$38</f>
+        <f>N4*$P$34</f>
         <v>29963.200000000001</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" ref="O5:AH5" si="36">O4*$P$38</f>
+        <f>O4*$P$34</f>
         <v>30562.400000000001</v>
       </c>
       <c r="P5" s="2">
-        <f t="shared" si="36"/>
+        <f>P4*$P$34</f>
         <v>31173.600000000002</v>
       </c>
       <c r="Q5" s="2">
-        <f t="shared" si="36"/>
+        <f>Q4*$P$34</f>
         <v>31796.800000000003</v>
       </c>
       <c r="R5" s="2">
-        <f t="shared" si="36"/>
+        <f>R4*$P$34</f>
         <v>32432.800000000003</v>
       </c>
       <c r="S5" s="2">
-        <f t="shared" si="36"/>
+        <f>S4*$P$34</f>
         <v>33081.599999999999</v>
       </c>
       <c r="T5" s="2">
-        <f t="shared" si="36"/>
+        <f>T4*$P$34</f>
         <v>33743.200000000004</v>
       </c>
       <c r="U5" s="2">
-        <f t="shared" si="36"/>
+        <f>U4*$P$34</f>
         <v>34418.400000000001</v>
       </c>
       <c r="V5" s="2">
-        <f t="shared" si="36"/>
+        <f>V4*$P$34</f>
         <v>35106.400000000001</v>
       </c>
       <c r="W5" s="2">
-        <f t="shared" si="36"/>
+        <f>W4*$P$34</f>
         <v>35808.800000000003</v>
       </c>
       <c r="X5" s="2">
-        <f t="shared" si="36"/>
+        <f>X4*$P$34</f>
         <v>36524.800000000003</v>
       </c>
       <c r="Y5" s="2">
-        <f t="shared" si="36"/>
+        <f>Y4*$P$34</f>
         <v>37255.200000000004</v>
       </c>
       <c r="Z5" s="2">
-        <f t="shared" si="36"/>
+        <f>Z4*$P$34</f>
         <v>38000</v>
       </c>
       <c r="AA5" s="2">
-        <f t="shared" si="36"/>
+        <f>AA4*$P$34</f>
         <v>38760</v>
       </c>
       <c r="AB5" s="2">
-        <f t="shared" si="36"/>
+        <f>AB4*$P$34</f>
         <v>39535.200000000004</v>
       </c>
       <c r="AC5" s="2">
-        <f t="shared" si="36"/>
+        <f>AC4*$P$34</f>
         <v>40325.600000000006</v>
       </c>
       <c r="AD5" s="2">
-        <f t="shared" si="36"/>
+        <f>AD4*$P$34</f>
         <v>41132</v>
       </c>
       <c r="AE5" s="2">
-        <f t="shared" si="36"/>
+        <f>AE4*$P$34</f>
         <v>41954.400000000001</v>
       </c>
       <c r="AF5" s="2">
-        <f t="shared" si="36"/>
+        <f>AF4*$P$34</f>
         <v>42793.600000000006</v>
       </c>
       <c r="AG5" s="2">
-        <f t="shared" si="36"/>
+        <f>AG4*$P$34</f>
         <v>43649.600000000006</v>
       </c>
       <c r="AH5" s="2">
-        <f t="shared" si="36"/>
+        <f>AH4*$P$34</f>
         <v>44522.400000000001</v>
       </c>
     </row>
@@ -1181,200 +1143,200 @@
         <v>20</v>
       </c>
       <c r="H6">
-        <f>$N$39</f>
+        <f>$N$35</f>
         <v>15600</v>
       </c>
       <c r="I6">
-        <f>ROUND($N$39*$O$39,0)</f>
+        <f>ROUND($N$35*$O$35,0)</f>
         <v>15912</v>
       </c>
       <c r="J6">
-        <f>ROUND(I6*$O$39,0)</f>
+        <f>ROUND(I6*$O$35,0)</f>
         <v>16230</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:M6" si="37">ROUND(J6*$O$39,0)</f>
+        <f>ROUND(J6*$O$35,0)</f>
         <v>16555</v>
       </c>
       <c r="L6">
-        <f t="shared" si="37"/>
+        <f>ROUND(K6*$O$35,0)</f>
         <v>16886</v>
       </c>
       <c r="M6">
-        <f t="shared" si="37"/>
+        <f>ROUND(L6*$O$35,0)</f>
         <v>17224</v>
       </c>
       <c r="N6">
-        <f>ROUND(M6*$O$39,0)</f>
+        <f>ROUND(M6*$O$35,0)</f>
         <v>17568</v>
       </c>
       <c r="O6">
-        <f>ROUND(N6*$O$39,0)</f>
+        <f>ROUND(N6*$O$35,0)</f>
         <v>17919</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6:AH6" si="38">ROUND(O6*$O$39,0)</f>
+        <f>ROUND(O6*$O$35,0)</f>
         <v>18277</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="38"/>
+        <f>ROUND(P6*$O$35,0)</f>
         <v>18643</v>
       </c>
       <c r="R6">
-        <f t="shared" si="38"/>
+        <f>ROUND(Q6*$O$35,0)</f>
         <v>19016</v>
       </c>
       <c r="S6">
-        <f t="shared" si="38"/>
+        <f>ROUND(R6*$O$35,0)</f>
         <v>19396</v>
       </c>
       <c r="T6">
-        <f t="shared" si="38"/>
+        <f>ROUND(S6*$O$35,0)</f>
         <v>19784</v>
       </c>
       <c r="U6">
-        <f t="shared" si="38"/>
+        <f>ROUND(T6*$O$35,0)</f>
         <v>20180</v>
       </c>
       <c r="V6">
-        <f t="shared" si="38"/>
+        <f>ROUND(U6*$O$35,0)</f>
         <v>20584</v>
       </c>
       <c r="W6">
-        <f t="shared" si="38"/>
+        <f>ROUND(V6*$O$35,0)</f>
         <v>20996</v>
       </c>
       <c r="X6">
-        <f t="shared" si="38"/>
+        <f>ROUND(W6*$O$35,0)</f>
         <v>21416</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="38"/>
+        <f>ROUND(X6*$O$35,0)</f>
         <v>21844</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="38"/>
+        <f>ROUND(Y6*$O$35,0)</f>
         <v>22281</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="38"/>
+        <f>ROUND(Z6*$O$35,0)</f>
         <v>22727</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="38"/>
+        <f>ROUND(AA6*$O$35,0)</f>
         <v>23182</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="38"/>
+        <f>ROUND(AB6*$O$35,0)</f>
         <v>23646</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="38"/>
+        <f>ROUND(AC6*$O$35,0)</f>
         <v>24119</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="38"/>
+        <f>ROUND(AD6*$O$35,0)</f>
         <v>24601</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="38"/>
+        <f>ROUND(AE6*$O$35,0)</f>
         <v>25093</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="38"/>
+        <f>ROUND(AF6*$O$35,0)</f>
         <v>25595</v>
       </c>
       <c r="AH6">
-        <f t="shared" si="38"/>
+        <f>ROUND(AG6*$O$35,0)</f>
         <v>26107</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="N7" s="2">
-        <f>N6*$P$39</f>
+        <f>N6*$P$35</f>
         <v>14054.400000000001</v>
       </c>
       <c r="O7" s="2">
-        <f t="shared" ref="O7:AH7" si="39">O6*$P$39</f>
+        <f>O6*$P$35</f>
         <v>14335.2</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" si="39"/>
+        <f>P6*$P$35</f>
         <v>14621.6</v>
       </c>
       <c r="Q7" s="2">
-        <f t="shared" si="39"/>
+        <f>Q6*$P$35</f>
         <v>14914.400000000001</v>
       </c>
       <c r="R7" s="2">
-        <f t="shared" si="39"/>
+        <f>R6*$P$35</f>
         <v>15212.800000000001</v>
       </c>
       <c r="S7" s="2">
-        <f t="shared" si="39"/>
+        <f>S6*$P$35</f>
         <v>15516.800000000001</v>
       </c>
       <c r="T7" s="2">
-        <f t="shared" si="39"/>
+        <f>T6*$P$35</f>
         <v>15827.2</v>
       </c>
       <c r="U7" s="2">
-        <f t="shared" si="39"/>
+        <f>U6*$P$35</f>
         <v>16144</v>
       </c>
       <c r="V7" s="2">
-        <f t="shared" si="39"/>
+        <f>V6*$P$35</f>
         <v>16467.2</v>
       </c>
       <c r="W7" s="2">
-        <f t="shared" si="39"/>
+        <f>W6*$P$35</f>
         <v>16796.8</v>
       </c>
       <c r="X7" s="2">
-        <f t="shared" si="39"/>
+        <f>X6*$P$35</f>
         <v>17132.8</v>
       </c>
       <c r="Y7" s="2">
-        <f t="shared" si="39"/>
+        <f>Y6*$P$35</f>
         <v>17475.2</v>
       </c>
       <c r="Z7" s="2">
-        <f t="shared" si="39"/>
+        <f>Z6*$P$35</f>
         <v>17824.8</v>
       </c>
       <c r="AA7" s="2">
-        <f t="shared" si="39"/>
+        <f>AA6*$P$35</f>
         <v>18181.600000000002</v>
       </c>
       <c r="AB7" s="2">
-        <f t="shared" si="39"/>
+        <f>AB6*$P$35</f>
         <v>18545.600000000002</v>
       </c>
       <c r="AC7" s="2">
-        <f t="shared" si="39"/>
+        <f>AC6*$P$35</f>
         <v>18916.8</v>
       </c>
       <c r="AD7" s="2">
-        <f t="shared" si="39"/>
+        <f>AD6*$P$35</f>
         <v>19295.2</v>
       </c>
       <c r="AE7" s="2">
-        <f t="shared" si="39"/>
+        <f>AE6*$P$35</f>
         <v>19680.800000000003</v>
       </c>
       <c r="AF7" s="2">
-        <f t="shared" si="39"/>
+        <f>AF6*$P$35</f>
         <v>20074.400000000001</v>
       </c>
       <c r="AG7" s="2">
-        <f t="shared" si="39"/>
+        <f>AG6*$P$35</f>
         <v>20476</v>
       </c>
       <c r="AH7" s="2">
-        <f t="shared" si="39"/>
+        <f>AH6*$P$35</f>
         <v>20885.600000000002</v>
       </c>
     </row>
@@ -1383,135 +1345,135 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <f>$N$34</f>
+        <f>$N$30</f>
         <v>3000</v>
       </c>
       <c r="C8">
-        <f>$N$34*$O$34</f>
+        <f>$N$30*$O$30</f>
         <v>3044.9999999999995</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:E8" si="40">ROUND(C8*$O$34,0)</f>
+        <f>ROUND(C8*$O$30,0)</f>
         <v>3091</v>
       </c>
       <c r="E8">
-        <f t="shared" si="40"/>
+        <f>ROUND(D8*$O$30,0)</f>
         <v>3137</v>
       </c>
       <c r="F8">
-        <f>ROUND(E8*$O$34,0)</f>
+        <f>ROUND(E8*$O$30,0)</f>
         <v>3184</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:AH8" si="41">ROUND(F8*$O$34,0)</f>
+        <f>ROUND(F8*$O$30,0)</f>
         <v>3232</v>
       </c>
       <c r="H8">
-        <f t="shared" si="41"/>
+        <f>ROUND(G8*$O$30,0)</f>
         <v>3280</v>
       </c>
       <c r="I8">
-        <f t="shared" si="41"/>
+        <f>ROUND(H8*$O$30,0)</f>
         <v>3329</v>
       </c>
       <c r="J8">
-        <f t="shared" si="41"/>
+        <f>ROUND(I8*$O$30,0)</f>
         <v>3379</v>
       </c>
       <c r="K8">
-        <f t="shared" si="41"/>
+        <f>ROUND(J8*$O$30,0)</f>
         <v>3430</v>
       </c>
       <c r="L8">
-        <f t="shared" si="41"/>
+        <f>ROUND(K8*$O$30,0)</f>
         <v>3481</v>
       </c>
       <c r="M8">
-        <f t="shared" si="41"/>
+        <f>ROUND(L8*$O$30,0)</f>
         <v>3533</v>
       </c>
       <c r="N8">
-        <f t="shared" si="41"/>
+        <f>ROUND(M8*$O$30,0)</f>
         <v>3586</v>
       </c>
       <c r="O8">
-        <f t="shared" si="41"/>
+        <f>ROUND(N8*$O$30,0)</f>
         <v>3640</v>
       </c>
       <c r="P8">
-        <f t="shared" si="41"/>
+        <f>ROUND(O8*$O$30,0)</f>
         <v>3695</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="41"/>
+        <f>ROUND(P8*$O$30,0)</f>
         <v>3750</v>
       </c>
       <c r="R8">
-        <f t="shared" si="41"/>
+        <f>ROUND(Q8*$O$30,0)</f>
         <v>3806</v>
       </c>
       <c r="S8">
-        <f t="shared" si="41"/>
+        <f>ROUND(R8*$O$30,0)</f>
         <v>3863</v>
       </c>
       <c r="T8">
-        <f t="shared" si="41"/>
+        <f>ROUND(S8*$O$30,0)</f>
         <v>3921</v>
       </c>
       <c r="U8">
-        <f t="shared" si="41"/>
+        <f>ROUND(T8*$O$30,0)</f>
         <v>3980</v>
       </c>
       <c r="V8">
-        <f t="shared" si="41"/>
+        <f>ROUND(U8*$O$30,0)</f>
         <v>4040</v>
       </c>
       <c r="W8">
-        <f t="shared" si="41"/>
+        <f>ROUND(V8*$O$30,0)</f>
         <v>4101</v>
       </c>
       <c r="X8">
-        <f t="shared" si="41"/>
+        <f>ROUND(W8*$O$30,0)</f>
         <v>4163</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="41"/>
+        <f>ROUND(X8*$O$30,0)</f>
         <v>4225</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="41"/>
+        <f>ROUND(Y8*$O$30,0)</f>
         <v>4288</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="41"/>
+        <f>ROUND(Z8*$O$30,0)</f>
         <v>4352</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="41"/>
+        <f>ROUND(AA8*$O$30,0)</f>
         <v>4417</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="41"/>
+        <f>ROUND(AB8*$O$30,0)</f>
         <v>4483</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="41"/>
+        <f>ROUND(AC8*$O$30,0)</f>
         <v>4550</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="41"/>
+        <f>ROUND(AD8*$O$30,0)</f>
         <v>4618</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="41"/>
+        <f>ROUND(AE8*$O$30,0)</f>
         <v>4687</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="41"/>
+        <f>ROUND(AF8*$O$30,0)</f>
         <v>4757</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="41"/>
+        <f>ROUND(AG8*$O$30,0)</f>
         <v>4828</v>
       </c>
     </row>
@@ -1520,123 +1482,123 @@
         <v>10</v>
       </c>
       <c r="E9">
-        <f>$N$35</f>
+        <f>$N$31</f>
         <v>4800</v>
       </c>
       <c r="F9">
-        <f>ROUND($N$35*$O$35,0)</f>
+        <f>ROUND($N$31*$O$31,0)</f>
         <v>4848</v>
       </c>
       <c r="G9">
-        <f>ROUND(F9*$O$35,0)</f>
+        <f>ROUND(F9*$O$31,0)</f>
         <v>4896</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:AH9" si="42">ROUND(G9*$O$35,0)</f>
+        <f>ROUND(G9*$O$31,0)</f>
         <v>4945</v>
       </c>
       <c r="I9">
-        <f t="shared" si="42"/>
+        <f>ROUND(H9*$O$31,0)</f>
         <v>4994</v>
       </c>
       <c r="J9">
-        <f t="shared" si="42"/>
+        <f>ROUND(I9*$O$31,0)</f>
         <v>5044</v>
       </c>
       <c r="K9">
-        <f t="shared" si="42"/>
+        <f>ROUND(J9*$O$31,0)</f>
         <v>5094</v>
       </c>
       <c r="L9">
-        <f t="shared" si="42"/>
+        <f>ROUND(K9*$O$31,0)</f>
         <v>5145</v>
       </c>
       <c r="M9">
-        <f t="shared" si="42"/>
+        <f>ROUND(L9*$O$31,0)</f>
         <v>5196</v>
       </c>
       <c r="N9">
-        <f t="shared" si="42"/>
+        <f>ROUND(M9*$O$31,0)</f>
         <v>5248</v>
       </c>
       <c r="O9">
-        <f t="shared" si="42"/>
+        <f>ROUND(N9*$O$31,0)</f>
         <v>5300</v>
       </c>
       <c r="P9">
-        <f t="shared" si="42"/>
+        <f>ROUND(O9*$O$31,0)</f>
         <v>5353</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="42"/>
+        <f>ROUND(P9*$O$31,0)</f>
         <v>5407</v>
       </c>
       <c r="R9">
-        <f t="shared" si="42"/>
+        <f>ROUND(Q9*$O$31,0)</f>
         <v>5461</v>
       </c>
       <c r="S9">
-        <f t="shared" si="42"/>
+        <f>ROUND(R9*$O$31,0)</f>
         <v>5516</v>
       </c>
       <c r="T9">
-        <f t="shared" si="42"/>
+        <f>ROUND(S9*$O$31,0)</f>
         <v>5571</v>
       </c>
       <c r="U9">
-        <f t="shared" si="42"/>
+        <f>ROUND(T9*$O$31,0)</f>
         <v>5627</v>
       </c>
       <c r="V9">
-        <f t="shared" si="42"/>
+        <f>ROUND(U9*$O$31,0)</f>
         <v>5683</v>
       </c>
       <c r="W9">
-        <f t="shared" si="42"/>
+        <f>ROUND(V9*$O$31,0)</f>
         <v>5740</v>
       </c>
       <c r="X9">
-        <f t="shared" si="42"/>
+        <f>ROUND(W9*$O$31,0)</f>
         <v>5797</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="42"/>
+        <f>ROUND(X9*$O$31,0)</f>
         <v>5855</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="42"/>
+        <f>ROUND(Y9*$O$31,0)</f>
         <v>5914</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="42"/>
+        <f>ROUND(Z9*$O$31,0)</f>
         <v>5973</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="42"/>
+        <f>ROUND(AA9*$O$31,0)</f>
         <v>6033</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="42"/>
+        <f>ROUND(AB9*$O$31,0)</f>
         <v>6093</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="42"/>
+        <f>ROUND(AC9*$O$31,0)</f>
         <v>6154</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="42"/>
+        <f>ROUND(AD9*$O$31,0)</f>
         <v>6216</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="42"/>
+        <f>ROUND(AE9*$O$31,0)</f>
         <v>6278</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="42"/>
+        <f>ROUND(AF9*$O$31,0)</f>
         <v>6341</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="42"/>
+        <f>ROUND(AG9*$O$31,0)</f>
         <v>6404</v>
       </c>
     </row>
@@ -1653,19 +1615,19 @@
         <v>5</v>
       </c>
       <c r="B11" s="2">
-        <f>SUM(B3:B10)*$C$33</f>
+        <f>SUM(B3:B10)*$C$29</f>
         <v>31950</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:E11" si="43">SUM(C3:C10)</f>
+        <f t="shared" ref="C11:E11" si="34">SUM(C3:C10)</f>
         <v>43437</v>
       </c>
       <c r="D11">
-        <f t="shared" si="43"/>
+        <f t="shared" si="34"/>
         <v>44291</v>
       </c>
       <c r="E11">
-        <f t="shared" si="43"/>
+        <f t="shared" si="34"/>
         <v>49961</v>
       </c>
       <c r="F11">
@@ -1673,31 +1635,31 @@
         <v>59896</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:M11" si="44">SUM(G3:G10)</f>
+        <f t="shared" ref="G11:M11" si="35">SUM(G3:G10)</f>
         <v>51849</v>
       </c>
       <c r="H11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="35"/>
         <v>68420</v>
       </c>
       <c r="I11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="35"/>
         <v>69722</v>
       </c>
       <c r="J11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="35"/>
         <v>71050</v>
       </c>
       <c r="K11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="35"/>
         <v>72404</v>
       </c>
       <c r="L11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="35"/>
         <v>109784</v>
       </c>
       <c r="M11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="35"/>
         <v>111910</v>
       </c>
       <c r="N11" s="2">
@@ -1705,83 +1667,83 @@
         <v>103073.60000000001</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" ref="O11:AH11" si="45">O3+O5+SUM(O7:O10)</f>
+        <f t="shared" ref="O11:AH11" si="36">O3+O5+SUM(O7:O10)</f>
         <v>105063.59999999999</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>107094.20000000001</v>
       </c>
       <c r="Q11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>109164.20000000001</v>
       </c>
       <c r="R11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>111274.6</v>
       </c>
       <c r="S11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>113426.40000000001</v>
       </c>
       <c r="T11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>115620.40000000001</v>
       </c>
       <c r="U11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>117858.4</v>
       </c>
       <c r="V11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>120139.59999999999</v>
       </c>
       <c r="W11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>122466.6</v>
       </c>
       <c r="X11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>124837.6</v>
       </c>
       <c r="Y11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>127254.40000000001</v>
       </c>
       <c r="Z11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>129719.8</v>
       </c>
       <c r="AA11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>132233.60000000001</v>
       </c>
       <c r="AB11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>134796.80000000002</v>
       </c>
       <c r="AC11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>137409.4</v>
       </c>
       <c r="AD11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>140074.20000000001</v>
       </c>
       <c r="AE11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>142791.20000000001</v>
       </c>
       <c r="AF11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>145561</v>
       </c>
       <c r="AG11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>148386.6</v>
       </c>
       <c r="AH11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="36"/>
         <v>151266</v>
       </c>
     </row>
@@ -1790,276 +1752,276 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2">
-        <f>B11-B21+$B$32</f>
+        <f>B11-B21+$B$28</f>
         <v>59100</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" ref="C13:AH13" si="46">C11-C21+$B$32</f>
+        <f>C11-C21+$B$28</f>
         <v>85060</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="46"/>
+        <f>D11-D21+$B$28</f>
         <v>79642</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="46"/>
+        <f>E11-E21+$B$28</f>
         <v>82353</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="46"/>
+        <f>F11-F21+$B$28</f>
         <v>85201</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="46"/>
+        <f>G11-G21+$B$28</f>
         <v>86995</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="46"/>
+        <f>H11-H21+$B$28</f>
         <v>90109</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="46"/>
+        <f>I11-I21+$B$28</f>
         <v>93386</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="46"/>
+        <f>J11-J21+$B$28</f>
         <v>96838</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="46"/>
+        <f>K11-K21+$B$28</f>
         <v>100476</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="46"/>
+        <f>L11-L21+$B$28</f>
         <v>122384</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="46"/>
+        <f>M11-M21+$B$28</f>
         <v>124510</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="46"/>
+        <f>N11-N21+$B$28</f>
         <v>115673.60000000001</v>
       </c>
       <c r="O13" s="2">
-        <f t="shared" si="46"/>
+        <f>O11-O21+$B$28</f>
         <v>117663.59999999999</v>
       </c>
       <c r="P13" s="2">
-        <f t="shared" si="46"/>
+        <f>P11-P21+$B$28</f>
         <v>121909</v>
       </c>
       <c r="Q13" s="2">
-        <f t="shared" si="46"/>
+        <f>Q11-Q21+$B$28</f>
         <v>126951</v>
       </c>
       <c r="R13" s="2">
-        <f t="shared" si="46"/>
+        <f>R11-R21+$B$28</f>
         <v>132285</v>
       </c>
       <c r="S13" s="2">
-        <f t="shared" si="46"/>
+        <f>S11-S21+$B$28</f>
         <v>137931</v>
       </c>
       <c r="T13" s="2">
-        <f t="shared" si="46"/>
+        <f>T11-T21+$B$28</f>
         <v>143911</v>
       </c>
       <c r="U13" s="2">
-        <f t="shared" si="46"/>
+        <f>U11-U21+$B$28</f>
         <v>150248</v>
       </c>
       <c r="V13" s="2">
-        <f t="shared" si="46"/>
+        <f>V11-V21+$B$28</f>
         <v>156967</v>
       </c>
       <c r="W13" s="2">
-        <f t="shared" si="46"/>
+        <f>W11-W21+$B$28</f>
         <v>164094</v>
       </c>
       <c r="X13" s="2">
-        <f t="shared" si="46"/>
+        <f>X11-X21+$B$28</f>
         <v>171659</v>
       </c>
       <c r="Y13" s="2">
-        <f t="shared" si="46"/>
+        <f>Y11-Y21+$B$28</f>
         <v>179693</v>
       </c>
       <c r="Z13" s="2">
-        <f t="shared" si="46"/>
+        <f>Z11-Z21+$B$28</f>
         <v>188228</v>
       </c>
       <c r="AA13" s="2">
-        <f t="shared" si="46"/>
+        <f>AA11-AA21+$B$28</f>
         <v>197301</v>
       </c>
       <c r="AB13" s="2">
-        <f t="shared" si="46"/>
+        <f>AB11-AB21+$B$28</f>
         <v>206951</v>
       </c>
       <c r="AC13" s="2">
-        <f t="shared" si="46"/>
+        <f>AC11-AC21+$B$28</f>
         <v>217219</v>
       </c>
       <c r="AD13" s="2">
-        <f t="shared" si="46"/>
+        <f>AD11-AD21+$B$28</f>
         <v>228150</v>
       </c>
       <c r="AE13" s="2">
-        <f t="shared" si="46"/>
+        <f>AE11-AE21+$B$28</f>
         <v>239793</v>
       </c>
       <c r="AF13" s="2">
-        <f t="shared" si="46"/>
+        <f>AF11-AF21+$B$28</f>
         <v>252199</v>
       </c>
       <c r="AG13" s="2">
-        <f t="shared" si="46"/>
+        <f>AG11-AG21+$B$28</f>
         <v>265425</v>
       </c>
       <c r="AH13" s="2">
-        <f t="shared" si="46"/>
+        <f>AH11-AH21+$B$28</f>
         <v>279531</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B14">
-        <f>ROUND((1700 + 0.15*(B13- 36000)),0)</f>
-        <v>5165</v>
+        <f>ROUND((1815 + 0.15*(B13- 38250)),0)</f>
+        <v>4943</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:G14" si="47">ROUND((1700 + 0.15*(C13- 36000)),0)</f>
-        <v>9059</v>
+        <f t="shared" ref="C14:I14" si="37">ROUND((1815 + 0.15*(C13- 38250)),0)</f>
+        <v>8837</v>
       </c>
       <c r="D14">
-        <f t="shared" si="47"/>
-        <v>8246</v>
+        <f t="shared" si="37"/>
+        <v>8024</v>
       </c>
       <c r="E14">
-        <f t="shared" si="47"/>
-        <v>8653</v>
+        <f t="shared" si="37"/>
+        <v>8430</v>
       </c>
       <c r="F14">
-        <f t="shared" si="47"/>
-        <v>9080</v>
+        <f t="shared" si="37"/>
+        <v>8858</v>
       </c>
       <c r="G14">
-        <f t="shared" si="47"/>
-        <v>9349</v>
+        <f t="shared" si="37"/>
+        <v>9127</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14" si="48">ROUND((9500 + 0.25*(H13- 88000)),0)</f>
-        <v>10027</v>
+        <f t="shared" si="37"/>
+        <v>9594</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14" si="49">ROUND((9500 + 0.25*(I13- 88000)),0)</f>
-        <v>10847</v>
+        <f t="shared" si="37"/>
+        <v>10085</v>
       </c>
       <c r="J14">
-        <f t="shared" ref="J14" si="50">ROUND((9500 + 0.25*(J13- 88000)),0)</f>
-        <v>11710</v>
+        <f>ROUND((10163 + 0.25*(J13- 94100)),0)</f>
+        <v>10848</v>
       </c>
       <c r="K14">
-        <f t="shared" ref="K14" si="51">ROUND((9500 + 0.25*(K13- 88000)),0)</f>
-        <v>12619</v>
+        <f t="shared" ref="K14:AH14" si="38">ROUND((10163 + 0.25*(K13- 94100)),0)</f>
+        <v>11757</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14" si="52">ROUND((9500 + 0.25*(L13- 88000)),0)</f>
-        <v>18096</v>
+        <f t="shared" si="38"/>
+        <v>17234</v>
       </c>
       <c r="M14">
-        <f t="shared" ref="M14:AH14" si="53">ROUND((9500 + 0.25*(M13- 88000)),0)</f>
-        <v>18628</v>
+        <f t="shared" si="38"/>
+        <v>17766</v>
       </c>
       <c r="N14">
-        <f t="shared" si="53"/>
-        <v>16418</v>
+        <f t="shared" si="38"/>
+        <v>15556</v>
       </c>
       <c r="O14">
-        <f t="shared" si="53"/>
-        <v>16916</v>
+        <f t="shared" si="38"/>
+        <v>16054</v>
       </c>
       <c r="P14">
-        <f t="shared" si="53"/>
-        <v>17977</v>
+        <f t="shared" si="38"/>
+        <v>17115</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="53"/>
-        <v>19238</v>
+        <f t="shared" si="38"/>
+        <v>18376</v>
       </c>
       <c r="R14">
-        <f t="shared" si="53"/>
-        <v>20571</v>
+        <f t="shared" si="38"/>
+        <v>19709</v>
       </c>
       <c r="S14">
-        <f t="shared" si="53"/>
-        <v>21983</v>
+        <f t="shared" si="38"/>
+        <v>21121</v>
       </c>
       <c r="T14">
-        <f t="shared" si="53"/>
-        <v>23478</v>
+        <f t="shared" si="38"/>
+        <v>22616</v>
       </c>
       <c r="U14">
-        <f t="shared" si="53"/>
-        <v>25062</v>
+        <f t="shared" si="38"/>
+        <v>24200</v>
       </c>
       <c r="V14">
-        <f t="shared" si="53"/>
-        <v>26742</v>
+        <f t="shared" si="38"/>
+        <v>25880</v>
       </c>
       <c r="W14">
-        <f t="shared" si="53"/>
-        <v>28524</v>
+        <f t="shared" si="38"/>
+        <v>27662</v>
       </c>
       <c r="X14">
-        <f t="shared" si="53"/>
-        <v>30415</v>
+        <f t="shared" si="38"/>
+        <v>29553</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="53"/>
-        <v>32423</v>
+        <f t="shared" si="38"/>
+        <v>31561</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="53"/>
-        <v>34557</v>
+        <f t="shared" si="38"/>
+        <v>33695</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="53"/>
-        <v>36825</v>
+        <f t="shared" si="38"/>
+        <v>35963</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="53"/>
-        <v>39238</v>
+        <f t="shared" si="38"/>
+        <v>38376</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="53"/>
-        <v>41805</v>
+        <f t="shared" si="38"/>
+        <v>40943</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="53"/>
-        <v>44538</v>
+        <f t="shared" si="38"/>
+        <v>43676</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="53"/>
-        <v>47448</v>
+        <f t="shared" si="38"/>
+        <v>46586</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="53"/>
-        <v>50550</v>
+        <f t="shared" si="38"/>
+        <v>49688</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="53"/>
-        <v>53856</v>
+        <f t="shared" si="38"/>
+        <v>52994</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="53"/>
-        <v>57383</v>
+        <f t="shared" si="38"/>
+        <v>56521</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -2070,135 +2032,135 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <f>$N$36*$C$33</f>
+        <f>$N$32*$C$29</f>
         <v>37500</v>
       </c>
       <c r="C16">
-        <f>ROUND($N$36*$O$36,0)</f>
+        <f>ROUND($N$32*$O$32,0)</f>
         <v>51500</v>
       </c>
       <c r="D16">
-        <f>ROUND(C16*$O$36,0)</f>
+        <f>ROUND(C16*$O$32,0)</f>
         <v>53045</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16:F16" si="54">ROUND(D16*$O$36,0)</f>
+        <f>ROUND(D16*$O$32,0)</f>
         <v>54636</v>
       </c>
       <c r="F16">
-        <f t="shared" si="54"/>
+        <f>ROUND(E16*$O$32,0)</f>
         <v>56275</v>
       </c>
       <c r="G16">
-        <f>ROUND((F16*$O$36-1200),0)</f>
+        <f>ROUND((F16*$O$32-1200),0)</f>
         <v>56763</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:AH16" si="55">ROUND(G16*$O$36,0)</f>
+        <f>ROUND(G16*$O$32,0)</f>
         <v>58466</v>
       </c>
       <c r="I16">
-        <f t="shared" si="55"/>
+        <f>ROUND(H16*$O$32,0)</f>
         <v>60220</v>
       </c>
       <c r="J16">
-        <f t="shared" si="55"/>
+        <f>ROUND(I16*$O$32,0)</f>
         <v>62027</v>
       </c>
       <c r="K16">
-        <f t="shared" si="55"/>
+        <f>ROUND(J16*$O$32,0)</f>
         <v>63888</v>
       </c>
       <c r="L16">
-        <f t="shared" si="55"/>
+        <f>ROUND(K16*$O$32,0)</f>
         <v>65805</v>
       </c>
       <c r="M16">
-        <f t="shared" si="55"/>
+        <f>ROUND(L16*$O$32,0)</f>
         <v>67779</v>
       </c>
       <c r="N16">
-        <f t="shared" si="55"/>
+        <f>ROUND(M16*$O$32,0)</f>
         <v>69812</v>
       </c>
       <c r="O16">
-        <f t="shared" si="55"/>
+        <f>ROUND(N16*$O$32,0)</f>
         <v>71906</v>
       </c>
       <c r="P16">
-        <f t="shared" si="55"/>
+        <f>ROUND(O16*$O$32,0)</f>
         <v>74063</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="55"/>
+        <f>ROUND(P16*$O$32,0)</f>
         <v>76285</v>
       </c>
       <c r="R16">
-        <f t="shared" si="55"/>
+        <f>ROUND(Q16*$O$32,0)</f>
         <v>78574</v>
       </c>
       <c r="S16">
-        <f t="shared" si="55"/>
+        <f>ROUND(R16*$O$32,0)</f>
         <v>80931</v>
       </c>
       <c r="T16">
-        <f t="shared" si="55"/>
+        <f>ROUND(S16*$O$32,0)</f>
         <v>83359</v>
       </c>
       <c r="U16">
-        <f t="shared" si="55"/>
+        <f>ROUND(T16*$O$32,0)</f>
         <v>85860</v>
       </c>
       <c r="V16">
-        <f t="shared" si="55"/>
+        <f>ROUND(U16*$O$32,0)</f>
         <v>88436</v>
       </c>
       <c r="W16">
-        <f t="shared" si="55"/>
+        <f>ROUND(V16*$O$32,0)</f>
         <v>91089</v>
       </c>
       <c r="X16">
-        <f t="shared" si="55"/>
+        <f>ROUND(W16*$O$32,0)</f>
         <v>93822</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="55"/>
+        <f>ROUND(X16*$O$32,0)</f>
         <v>96637</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="55"/>
+        <f>ROUND(Y16*$O$32,0)</f>
         <v>99536</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="55"/>
+        <f>ROUND(Z16*$O$32,0)</f>
         <v>102522</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="55"/>
+        <f>ROUND(AA16*$O$32,0)</f>
         <v>105598</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="55"/>
+        <f>ROUND(AB16*$O$32,0)</f>
         <v>108766</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="55"/>
+        <f>ROUND(AC16*$O$32,0)</f>
         <v>112029</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="55"/>
+        <f>ROUND(AD16*$O$32,0)</f>
         <v>115390</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="55"/>
+        <f>ROUND(AE16*$O$32,0)</f>
         <v>118852</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="55"/>
+        <f>ROUND(AF16*$O$32,0)</f>
         <v>122418</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="55"/>
+        <f>ROUND(AG16*$O$32,0)</f>
         <v>126091</v>
       </c>
     </row>
@@ -2207,135 +2169,135 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <f>$N$37*$C$33</f>
+        <f>$N$33*$C$29</f>
         <v>9000</v>
       </c>
       <c r="C17">
-        <f>ROUND($N$37*$O$37,0)</f>
+        <f>ROUND($N$33*$O$33,0)</f>
         <v>12960</v>
       </c>
       <c r="D17">
-        <f>ROUND(C17*$O$37,0)</f>
+        <f>ROUND(C17*$O$33,0)</f>
         <v>13997</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:AH17" si="56">ROUND(D17*$O$37,0)</f>
+        <f>ROUND(D17*$O$33,0)</f>
         <v>15117</v>
       </c>
       <c r="F17">
-        <f t="shared" si="56"/>
+        <f>ROUND(E17*$O$33,0)</f>
         <v>16326</v>
       </c>
       <c r="G17">
-        <f t="shared" si="56"/>
+        <f>ROUND(F17*$O$33,0)</f>
         <v>17632</v>
       </c>
       <c r="H17">
-        <f t="shared" si="56"/>
+        <f>ROUND(G17*$O$33,0)</f>
         <v>19043</v>
       </c>
       <c r="I17">
-        <f t="shared" si="56"/>
+        <f>ROUND(H17*$O$33,0)</f>
         <v>20566</v>
       </c>
       <c r="J17">
-        <f t="shared" si="56"/>
+        <f>ROUND(I17*$O$33,0)</f>
         <v>22211</v>
       </c>
       <c r="K17">
-        <f t="shared" si="56"/>
+        <f>ROUND(J17*$O$33,0)</f>
         <v>23988</v>
       </c>
       <c r="L17">
-        <f t="shared" si="56"/>
+        <f>ROUND(K17*$O$33,0)</f>
         <v>25907</v>
       </c>
       <c r="M17">
-        <f t="shared" si="56"/>
+        <f>ROUND(L17*$O$33,0)</f>
         <v>27980</v>
       </c>
       <c r="N17">
-        <f t="shared" si="56"/>
+        <f>ROUND(M17*$O$33,0)</f>
         <v>30218</v>
       </c>
       <c r="O17">
-        <f t="shared" si="56"/>
+        <f>ROUND(N17*$O$33,0)</f>
         <v>32635</v>
       </c>
       <c r="P17">
-        <f t="shared" si="56"/>
+        <f>ROUND(O17*$O$33,0)</f>
         <v>35246</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="56"/>
+        <f>ROUND(P17*$O$33,0)</f>
         <v>38066</v>
       </c>
       <c r="R17">
-        <f t="shared" si="56"/>
+        <f>ROUND(Q17*$O$33,0)</f>
         <v>41111</v>
       </c>
       <c r="S17">
-        <f t="shared" si="56"/>
+        <f>ROUND(R17*$O$33,0)</f>
         <v>44400</v>
       </c>
       <c r="T17">
-        <f t="shared" si="56"/>
+        <f>ROUND(S17*$O$33,0)</f>
         <v>47952</v>
       </c>
       <c r="U17">
-        <f t="shared" si="56"/>
+        <f>ROUND(T17*$O$33,0)</f>
         <v>51788</v>
       </c>
       <c r="V17">
-        <f t="shared" si="56"/>
+        <f>ROUND(U17*$O$33,0)</f>
         <v>55931</v>
       </c>
       <c r="W17">
-        <f t="shared" si="56"/>
+        <f>ROUND(V17*$O$33,0)</f>
         <v>60405</v>
       </c>
       <c r="X17">
-        <f t="shared" si="56"/>
+        <f>ROUND(W17*$O$33,0)</f>
         <v>65237</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="56"/>
+        <f>ROUND(X17*$O$33,0)</f>
         <v>70456</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="56"/>
+        <f>ROUND(Y17*$O$33,0)</f>
         <v>76092</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="56"/>
+        <f>ROUND(Z17*$O$33,0)</f>
         <v>82179</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="56"/>
+        <f>ROUND(AA17*$O$33,0)</f>
         <v>88753</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="56"/>
+        <f>ROUND(AB17*$O$33,0)</f>
         <v>95853</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="56"/>
+        <f>ROUND(AC17*$O$33,0)</f>
         <v>103521</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="56"/>
+        <f>ROUND(AD17*$O$33,0)</f>
         <v>111803</v>
       </c>
       <c r="AF17">
-        <f t="shared" si="56"/>
+        <f>ROUND(AE17*$O$33,0)</f>
         <v>120747</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="56"/>
+        <f>ROUND(AF17*$O$33,0)</f>
         <v>130407</v>
       </c>
       <c r="AH17">
-        <f t="shared" si="56"/>
+        <f>ROUND(AG17*$O$33,0)</f>
         <v>140840</v>
       </c>
     </row>
@@ -2356,131 +2318,131 @@
         <v>46500</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:AH19" si="57">(C16+C17+C18)</f>
+        <f t="shared" ref="C19:AH19" si="39">(C16+C17+C18)</f>
         <v>72460</v>
       </c>
       <c r="D19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>67042</v>
       </c>
       <c r="E19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>69753</v>
       </c>
       <c r="F19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>72601</v>
       </c>
       <c r="G19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>74395</v>
       </c>
       <c r="H19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>77509</v>
       </c>
       <c r="I19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>80786</v>
       </c>
       <c r="J19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>84238</v>
       </c>
       <c r="K19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>87876</v>
       </c>
       <c r="L19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>91712</v>
       </c>
       <c r="M19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>95759</v>
       </c>
       <c r="N19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>100030</v>
       </c>
       <c r="O19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>104541</v>
       </c>
       <c r="P19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>109309</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>114351</v>
       </c>
       <c r="R19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>119685</v>
       </c>
       <c r="S19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>125331</v>
       </c>
       <c r="T19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>131311</v>
       </c>
       <c r="U19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>137648</v>
       </c>
       <c r="V19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>144367</v>
       </c>
       <c r="W19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>151494</v>
       </c>
       <c r="X19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>159059</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>167093</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>175628</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>184701</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>194351</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>204619</v>
       </c>
       <c r="AD19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>215550</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>227193</v>
       </c>
       <c r="AF19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>239599</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>252825</v>
       </c>
       <c r="AH19">
-        <f t="shared" si="57"/>
+        <f t="shared" si="39"/>
         <v>266931</v>
       </c>
     </row>
@@ -2491,60 +2453,60 @@
         <v>18072</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20:O20" si="58">M11-M19</f>
+        <f t="shared" ref="M20:O20" si="40">M11-M19</f>
         <v>16151</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" si="58"/>
+        <f t="shared" si="40"/>
         <v>3043.6000000000058</v>
       </c>
       <c r="O20">
-        <f t="shared" si="58"/>
+        <f t="shared" si="40"/>
         <v>522.59999999999127</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2">
         <f>B11-B19</f>
         <v>-14550</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" ref="C21:AH21" si="59">C11-C19</f>
+        <f t="shared" ref="C21:AH21" si="41">C11-C19</f>
         <v>-29023</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-22751</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-19792</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-12705</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-22546</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-9089</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-11064</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-13188</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-15472</v>
       </c>
       <c r="L21" s="2">
@@ -2560,79 +2522,79 @@
         <v>0</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-2214.7999999999884</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-5186.7999999999884</v>
       </c>
       <c r="R21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-8410.3999999999942</v>
       </c>
       <c r="S21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-11904.599999999991</v>
       </c>
       <c r="T21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-15690.599999999991</v>
       </c>
       <c r="U21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-19789.600000000006</v>
       </c>
       <c r="V21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-24227.400000000009</v>
       </c>
       <c r="W21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-29027.399999999994</v>
       </c>
       <c r="X21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-34221.399999999994</v>
       </c>
       <c r="Y21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-39838.599999999991</v>
       </c>
       <c r="Z21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-45908.2</v>
       </c>
       <c r="AA21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-52467.399999999994</v>
       </c>
       <c r="AB21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-59554.199999999983</v>
       </c>
       <c r="AC21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-67209.600000000006</v>
       </c>
       <c r="AD21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-75475.799999999988</v>
       </c>
       <c r="AE21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-84401.799999999988</v>
       </c>
       <c r="AF21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-94038</v>
       </c>
       <c r="AG21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-104438.39999999999</v>
       </c>
       <c r="AH21" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="41"/>
         <v>-115665</v>
       </c>
     </row>
@@ -2642,135 +2604,135 @@
       </c>
       <c r="B22">
         <f>-B14</f>
-        <v>-5165</v>
+        <v>-4943</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:D22" si="60">-C14</f>
-        <v>-9059</v>
+        <f t="shared" ref="C22:D22" si="42">-C14</f>
+        <v>-8837</v>
       </c>
       <c r="D22">
-        <f t="shared" si="60"/>
-        <v>-8246</v>
+        <f t="shared" si="42"/>
+        <v>-8024</v>
       </c>
       <c r="E22">
         <f>-E14</f>
-        <v>-8653</v>
+        <v>-8430</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:Q22" si="61">-F14</f>
-        <v>-9080</v>
+        <f t="shared" ref="F22:Q22" si="43">-F14</f>
+        <v>-8858</v>
       </c>
       <c r="G22">
-        <f t="shared" si="61"/>
-        <v>-9349</v>
+        <f t="shared" si="43"/>
+        <v>-9127</v>
       </c>
       <c r="H22">
-        <f t="shared" si="61"/>
-        <v>-10027</v>
+        <f t="shared" si="43"/>
+        <v>-9594</v>
       </c>
       <c r="I22">
-        <f t="shared" si="61"/>
-        <v>-10847</v>
+        <f t="shared" si="43"/>
+        <v>-10085</v>
       </c>
       <c r="J22">
-        <f t="shared" si="61"/>
-        <v>-11710</v>
+        <f t="shared" si="43"/>
+        <v>-10848</v>
       </c>
       <c r="K22">
-        <f t="shared" si="61"/>
-        <v>-12619</v>
+        <f t="shared" si="43"/>
+        <v>-11757</v>
       </c>
       <c r="L22">
         <f>L11-L19-L14</f>
-        <v>-24</v>
+        <v>838</v>
       </c>
       <c r="M22">
-        <f t="shared" ref="M22:O22" si="62">M11-M19-M14</f>
-        <v>-2477</v>
+        <f t="shared" ref="M22:O22" si="44">M11-M19-M14</f>
+        <v>-1615</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="62"/>
-        <v>-13374.399999999994</v>
+        <f t="shared" si="44"/>
+        <v>-12512.399999999994</v>
       </c>
       <c r="O22">
-        <f t="shared" si="62"/>
-        <v>-16393.400000000009</v>
+        <f t="shared" si="44"/>
+        <v>-15531.400000000009</v>
       </c>
       <c r="P22">
-        <f t="shared" si="61"/>
-        <v>-17977</v>
+        <f t="shared" si="43"/>
+        <v>-17115</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="61"/>
-        <v>-19238</v>
+        <f t="shared" si="43"/>
+        <v>-18376</v>
       </c>
       <c r="R22">
-        <f t="shared" ref="R22:W22" si="63">-R14</f>
-        <v>-20571</v>
+        <f t="shared" ref="R22:W22" si="45">-R14</f>
+        <v>-19709</v>
       </c>
       <c r="S22">
-        <f t="shared" si="63"/>
-        <v>-21983</v>
+        <f t="shared" si="45"/>
+        <v>-21121</v>
       </c>
       <c r="T22">
-        <f t="shared" si="63"/>
-        <v>-23478</v>
+        <f t="shared" si="45"/>
+        <v>-22616</v>
       </c>
       <c r="U22">
-        <f t="shared" si="63"/>
-        <v>-25062</v>
+        <f t="shared" si="45"/>
+        <v>-24200</v>
       </c>
       <c r="V22">
-        <f t="shared" si="63"/>
-        <v>-26742</v>
+        <f t="shared" si="45"/>
+        <v>-25880</v>
       </c>
       <c r="W22">
-        <f t="shared" si="63"/>
-        <v>-28524</v>
+        <f t="shared" si="45"/>
+        <v>-27662</v>
       </c>
       <c r="X22">
-        <f t="shared" ref="X22:AH22" si="64">-X14</f>
-        <v>-30415</v>
+        <f t="shared" ref="X22:AH22" si="46">-X14</f>
+        <v>-29553</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="64"/>
-        <v>-32423</v>
+        <f t="shared" si="46"/>
+        <v>-31561</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="64"/>
-        <v>-34557</v>
+        <f t="shared" si="46"/>
+        <v>-33695</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="64"/>
-        <v>-36825</v>
+        <f t="shared" si="46"/>
+        <v>-35963</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="64"/>
-        <v>-39238</v>
+        <f t="shared" si="46"/>
+        <v>-38376</v>
       </c>
       <c r="AC22">
-        <f t="shared" si="64"/>
-        <v>-41805</v>
+        <f t="shared" si="46"/>
+        <v>-40943</v>
       </c>
       <c r="AD22">
-        <f t="shared" si="64"/>
-        <v>-44538</v>
+        <f t="shared" si="46"/>
+        <v>-43676</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="64"/>
-        <v>-47448</v>
+        <f t="shared" si="46"/>
+        <v>-46586</v>
       </c>
       <c r="AF22">
-        <f t="shared" si="64"/>
-        <v>-50550</v>
+        <f t="shared" si="46"/>
+        <v>-49688</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="64"/>
-        <v>-53856</v>
+        <f t="shared" si="46"/>
+        <v>-52994</v>
       </c>
       <c r="AH22">
-        <f t="shared" si="64"/>
-        <v>-57383</v>
+        <f t="shared" si="46"/>
+        <v>-56521</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
@@ -2781,135 +2743,135 @@
         <v>19</v>
       </c>
       <c r="B24" s="2">
-        <f>ROUND(($H$32-$B$32+B21)*$H$34,0)</f>
+        <f>ROUND(($H$28-$B$28+B21)*$H$30,0)</f>
         <v>587171</v>
       </c>
       <c r="C24" s="2">
-        <f>ROUND((B24-$B$32+C21)*$H$34,0)</f>
+        <f>ROUND((B24-$B$28+C21)*$H$30,0)</f>
         <v>559187</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" ref="D24:AH24" si="65">ROUND((C24-$B$32+D21)*$H$34,0)</f>
+        <f>ROUND((C24-$B$28+D21)*$H$30,0)</f>
         <v>536932</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((D24-$B$28+E21)*$H$30,0)</f>
         <v>517154</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((E24-$B$28+F21)*$H$30,0)</f>
         <v>504145</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((F24-$B$28+G21)*$H$30,0)</f>
         <v>480724</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((G24-$B$28+H21)*$H$30,0)</f>
         <v>470511</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((H24-$B$28+I21)*$H$30,0)</f>
         <v>458018</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((I24-$B$28+J21)*$H$30,0)</f>
         <v>443036</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((J24-$B$28+K21)*$H$30,0)</f>
         <v>425338</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((K24-$B$28+L21)*$H$30,0)</f>
         <v>423056</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((L24-$B$28+M21)*$H$30,0)</f>
         <v>420717</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((M24-$B$28+N21)*$H$30,0)</f>
         <v>418320</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((N24-$B$28+O21)*$H$30,0)</f>
         <v>415863</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((O24-$B$28+P21)*$H$30,0)</f>
         <v>411074</v>
       </c>
       <c r="Q24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((P24-$B$28+Q21)*$H$30,0)</f>
         <v>403119</v>
       </c>
       <c r="R24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((Q24-$B$28+R21)*$H$30,0)</f>
         <v>391661</v>
       </c>
       <c r="S24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((R24-$B$28+S21)*$H$30,0)</f>
         <v>376335</v>
       </c>
       <c r="T24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((S24-$B$28+T21)*$H$30,0)</f>
         <v>356746</v>
       </c>
       <c r="U24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((T24-$B$28+U21)*$H$30,0)</f>
         <v>332465</v>
       </c>
       <c r="V24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((U24-$B$28+V21)*$H$30,0)</f>
         <v>303029</v>
       </c>
       <c r="W24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((V24-$B$28+W21)*$H$30,0)</f>
         <v>267937</v>
       </c>
       <c r="X24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((W24-$B$28+X21)*$H$30,0)</f>
         <v>226643</v>
       </c>
       <c r="Y24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((X24-$B$28+Y21)*$H$30,0)</f>
         <v>178560</v>
       </c>
       <c r="Z24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((Y24-$B$28+Z21)*$H$30,0)</f>
         <v>123053</v>
       </c>
       <c r="AA24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((Z24-$B$28+AA21)*$H$30,0)</f>
         <v>59435</v>
       </c>
       <c r="AB24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((AA24-$B$28+AB21)*$H$30,0)</f>
         <v>-13037</v>
       </c>
       <c r="AC24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((AB24-$B$28+AC21)*$H$30,0)</f>
         <v>-95168</v>
       </c>
       <c r="AD24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((AC24-$B$28+AD21)*$H$30,0)</f>
         <v>-187825</v>
       </c>
       <c r="AE24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((AD24-$B$28+AE21)*$H$30,0)</f>
         <v>-291947</v>
       </c>
       <c r="AF24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((AE24-$B$28+AF21)*$H$30,0)</f>
         <v>-408550</v>
       </c>
       <c r="AG24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((AF24-$B$28+AG21)*$H$30,0)</f>
         <v>-538728</v>
       </c>
       <c r="AH24" s="2">
-        <f t="shared" si="65"/>
+        <f>ROUND((AG24-$B$28+AH21)*$H$30,0)</f>
         <v>-683668</v>
       </c>
     </row>
@@ -2917,508 +2879,311 @@
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B25">
-        <f>ROUND(($H$33+B22 + $B$32)*$H$34,0)</f>
-        <v>69121</v>
-      </c>
-      <c r="C25">
-        <f>ROUND((B25+C22 + $B$32)*$H$34,0)</f>
-        <v>74479</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ref="D25:AH25" si="66">ROUND((C25+D22 + $B$32)*$H$34,0)</f>
-        <v>80804</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="66"/>
-        <v>86870</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="66"/>
-        <v>92650</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="66"/>
-        <v>98299</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="66"/>
-        <v>103394</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="66"/>
-        <v>107776</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="66"/>
-        <v>111383</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="66"/>
-        <v>114148</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="66"/>
-        <v>129892</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="66"/>
-        <v>143515</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="66"/>
-        <v>146309</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="66"/>
-        <v>146078</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="66"/>
-        <v>144219</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="66"/>
-        <v>141021</v>
-      </c>
-      <c r="R25">
-        <f t="shared" si="66"/>
-        <v>136376</v>
-      </c>
-      <c r="S25">
-        <f t="shared" si="66"/>
-        <v>130168</v>
-      </c>
-      <c r="T25">
-        <f t="shared" si="66"/>
-        <v>122272</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="66"/>
-        <v>112555</v>
-      </c>
-      <c r="V25">
-        <f t="shared" si="66"/>
-        <v>100873</v>
-      </c>
-      <c r="W25">
-        <f t="shared" si="66"/>
-        <v>87073</v>
-      </c>
-      <c r="X25">
-        <f t="shared" si="66"/>
-        <v>70989</v>
-      </c>
-      <c r="Y25">
-        <f t="shared" si="66"/>
-        <v>52445</v>
-      </c>
-      <c r="Z25">
-        <f t="shared" si="66"/>
-        <v>31250</v>
-      </c>
-      <c r="AA25">
-        <f t="shared" si="66"/>
-        <v>7201</v>
-      </c>
-      <c r="AB25">
-        <f t="shared" si="66"/>
-        <v>-19923</v>
-      </c>
-      <c r="AC25">
-        <f t="shared" si="66"/>
-        <v>-50356</v>
-      </c>
-      <c r="AD25">
-        <f t="shared" si="66"/>
-        <v>-84351</v>
-      </c>
-      <c r="AE25">
-        <f t="shared" si="66"/>
-        <v>-122179</v>
-      </c>
-      <c r="AF25">
-        <f t="shared" si="66"/>
-        <v>-164132</v>
-      </c>
-      <c r="AG25">
-        <f t="shared" si="66"/>
-        <v>-210523</v>
-      </c>
-      <c r="AH25">
-        <f t="shared" si="66"/>
-        <v>-261689</v>
+      <c r="B25" s="3">
+        <f>($H$29+B22 + $B$28)*$H$30</f>
+        <v>69348.424999999988</v>
+      </c>
+      <c r="C25" s="3">
+        <f>(B25+C22 + $B$28)*$H$30</f>
+        <v>74939.210624999978</v>
+      </c>
+      <c r="D25" s="3">
+        <f>(C25+D22 + $B$28)*$H$30</f>
+        <v>81503.090890624968</v>
+      </c>
+      <c r="E25" s="3">
+        <f>(D25+E22 + $B$28)*$H$30</f>
+        <v>87814.918162890579</v>
+      </c>
+      <c r="F25" s="3">
+        <f>(E25+F22 + $B$28)*$H$30</f>
+        <v>93845.841116962838</v>
+      </c>
+      <c r="G25" s="3">
+        <f>(F25+G22 + $B$28)*$H$30</f>
+        <v>99751.812144886906</v>
+      </c>
+      <c r="H25" s="3">
+        <f>(G25+H22 + $B$28)*$H$30</f>
+        <v>105326.75744850907</v>
+      </c>
+      <c r="I25" s="3">
+        <f>(H25+I22 + $B$28)*$H$30</f>
+        <v>110537.8013847218</v>
+      </c>
+      <c r="J25" s="3">
+        <f>(I25+J22 + $B$28)*$H$30</f>
+        <v>115097.04641933984</v>
+      </c>
+      <c r="K25" s="3">
+        <f>(J25+K22 + $B$28)*$H$30</f>
+        <v>118838.54757982332</v>
+      </c>
+      <c r="L25" s="3">
+        <f>(K25+L22 + $B$28)*$H$30</f>
+        <v>135583.46126931888</v>
+      </c>
+      <c r="M25" s="3">
+        <f>(L25+M22 + $B$28)*$H$30</f>
+        <v>150232.67280105184</v>
+      </c>
+      <c r="N25" s="3">
+        <f>(M25+N22 + $B$28)*$H$30</f>
+        <v>154078.27962107814</v>
+      </c>
+      <c r="O25" s="3">
+        <f>(N25+O22 + $B$28)*$H$30</f>
+        <v>154925.55161160507</v>
+      </c>
+      <c r="P25" s="3">
+        <f>(O25+P22 + $B$28)*$H$30</f>
+        <v>154170.81540189518</v>
+      </c>
+      <c r="Q25" s="3">
+        <f>(P25+Q22 + $B$28)*$H$30</f>
+        <v>152104.68578694254</v>
+      </c>
+      <c r="R25" s="3">
+        <f>(Q25+R22 + $B$28)*$H$30</f>
+        <v>148620.57793161611</v>
+      </c>
+      <c r="S25" s="3">
+        <f>(R25+S22 + $B$28)*$H$30</f>
+        <v>143602.06737990648</v>
+      </c>
+      <c r="T25" s="3">
+        <f>(S25+T22 + $B$28)*$H$30</f>
+        <v>136925.71906440414</v>
+      </c>
+      <c r="U25" s="3">
+        <f>(T25+U22 + $B$28)*$H$30</f>
+        <v>128458.86204101423</v>
+      </c>
+      <c r="V25" s="3">
+        <f>(U25+V22 + $B$28)*$H$30</f>
+        <v>118058.33359203958</v>
+      </c>
+      <c r="W25" s="3">
+        <f>(V25+W22 + $B$28)*$H$30</f>
+        <v>105571.24193184056</v>
+      </c>
+      <c r="X25" s="3">
+        <f>(W25+X22 + $B$28)*$H$30</f>
+        <v>90833.697980136567</v>
+      </c>
+      <c r="Y25" s="3">
+        <f>(X25+Y22 + $B$28)*$H$30</f>
+        <v>73669.515429639971</v>
+      </c>
+      <c r="Z25" s="3">
+        <f>(Y25+Z22 + $B$28)*$H$30</f>
+        <v>53888.878315380964</v>
+      </c>
+      <c r="AA25" s="3">
+        <f>(Z25+AA22 + $B$28)*$H$30</f>
+        <v>31289.025273265484</v>
+      </c>
+      <c r="AB25" s="3">
+        <f>(AA25+AB22 + $B$28)*$H$30</f>
+        <v>5650.8509050971206</v>
+      </c>
+      <c r="AC25" s="3">
+        <f>(AB25+AC22 + $B$28)*$H$30</f>
+        <v>-23259.452822275452</v>
+      </c>
+      <c r="AD25" s="3">
+        <f>(AC25+AD22 + $B$28)*$H$30</f>
+        <v>-55693.839142832345</v>
+      </c>
+      <c r="AE25" s="3">
+        <f>(AD25+AE22 + $B$28)*$H$30</f>
+        <v>-91921.835121403157</v>
+      </c>
+      <c r="AF25" s="3">
+        <f>(AE25+AF22 + $B$28)*$H$30</f>
+        <v>-132235.08099943821</v>
+      </c>
+      <c r="AG25" s="3">
+        <f>(AF25+AG22 + $B$28)*$H$30</f>
+        <v>-176944.80802442416</v>
+      </c>
+      <c r="AH25" s="3">
+        <f>(AG25+AH22 + $B$28)*$H$30</f>
+        <v>-226387.45322503475</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A27" s="1"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>12600</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28">
+        <v>600000</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="O28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M29">
-        <f>M24-M27</f>
-        <v>420717</v>
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>0.75</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29">
+        <v>60000</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="N29">
-        <f t="shared" ref="N29:W29" si="67">N24-N27</f>
-        <v>418320</v>
+        <v>39600</v>
       </c>
       <c r="O29">
-        <f t="shared" si="67"/>
-        <v>415863</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="67"/>
-        <v>411074</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="67"/>
-        <v>403119</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="67"/>
-        <v>391661</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="67"/>
-        <v>376335</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="67"/>
-        <v>356746</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="67"/>
-        <v>332465</v>
-      </c>
-      <c r="V29">
-        <f t="shared" si="67"/>
-        <v>303029</v>
-      </c>
-      <c r="W29">
-        <f t="shared" si="67"/>
-        <v>267937</v>
-      </c>
-      <c r="X29">
-        <f t="shared" ref="X29:AH29" si="68">X24-X27</f>
-        <v>226643</v>
-      </c>
-      <c r="Y29">
-        <f t="shared" si="68"/>
-        <v>178560</v>
-      </c>
-      <c r="Z29">
-        <f t="shared" si="68"/>
-        <v>123053</v>
-      </c>
-      <c r="AA29">
-        <f t="shared" si="68"/>
-        <v>59435</v>
-      </c>
-      <c r="AB29">
-        <f t="shared" si="68"/>
-        <v>-13037</v>
-      </c>
-      <c r="AC29">
-        <f t="shared" si="68"/>
-        <v>-95168</v>
-      </c>
-      <c r="AD29">
-        <f t="shared" si="68"/>
-        <v>-187825</v>
-      </c>
-      <c r="AE29">
-        <f t="shared" si="68"/>
-        <v>-291947</v>
-      </c>
-      <c r="AF29">
-        <f t="shared" si="68"/>
-        <v>-408550</v>
-      </c>
-      <c r="AG29">
-        <f t="shared" si="68"/>
-        <v>-538728</v>
-      </c>
-      <c r="AH29">
-        <f t="shared" si="68"/>
-        <v>-683668</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M30">
-        <f>M25-M28</f>
-        <v>143515</v>
+      <c r="A30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="N30">
-        <f t="shared" ref="N30:W30" si="69">N25-N28</f>
-        <v>146309</v>
+        <v>3000</v>
       </c>
       <c r="O30">
-        <f t="shared" si="69"/>
-        <v>146078</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="69"/>
-        <v>144219</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="69"/>
-        <v>141021</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="69"/>
-        <v>136376</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="69"/>
-        <v>130168</v>
-      </c>
-      <c r="T30">
-        <f t="shared" si="69"/>
-        <v>122272</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="69"/>
-        <v>112555</v>
-      </c>
-      <c r="V30">
-        <f t="shared" si="69"/>
-        <v>100873</v>
-      </c>
-      <c r="W30">
-        <f t="shared" si="69"/>
-        <v>87073</v>
-      </c>
-      <c r="X30">
-        <f t="shared" ref="X30:AH30" si="70">X25-X28</f>
-        <v>70989</v>
-      </c>
-      <c r="Y30">
-        <f t="shared" si="70"/>
-        <v>52445</v>
-      </c>
-      <c r="Z30">
-        <f t="shared" si="70"/>
-        <v>31250</v>
-      </c>
-      <c r="AA30">
-        <f t="shared" si="70"/>
-        <v>7201</v>
-      </c>
-      <c r="AB30">
-        <f t="shared" si="70"/>
-        <v>-19923</v>
-      </c>
-      <c r="AC30">
-        <f t="shared" si="70"/>
-        <v>-50356</v>
-      </c>
-      <c r="AD30">
-        <f t="shared" si="70"/>
-        <v>-84351</v>
-      </c>
-      <c r="AE30">
-        <f t="shared" si="70"/>
-        <v>-122179</v>
-      </c>
-      <c r="AF30">
-        <f t="shared" si="70"/>
-        <v>-164132</v>
-      </c>
-      <c r="AG30">
-        <f t="shared" si="70"/>
-        <v>-210523</v>
-      </c>
-      <c r="AH30">
-        <f t="shared" si="70"/>
-        <v>-261689</v>
+        <v>1.0149999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="K31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N31">
+        <v>4800</v>
+      </c>
+      <c r="O31">
+        <v>1.01</v>
+      </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32">
-        <v>12600</v>
-      </c>
-      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N32">
+        <v>50000</v>
+      </c>
+      <c r="O32">
+        <v>1.03</v>
+      </c>
+      <c r="Q32" t="s">
         <v>39</v>
       </c>
-      <c r="H32">
-        <v>600000</v>
-      </c>
-      <c r="J32" s="1" t="s">
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N33">
+        <v>12000</v>
+      </c>
+      <c r="O33">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="1"/>
-      <c r="O32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33">
-        <v>0.75</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H33">
-        <v>60000</v>
-      </c>
-      <c r="K33" s="1" t="s">
+      <c r="N34">
+        <v>36000</v>
+      </c>
+      <c r="O34">
+        <v>1.02</v>
+      </c>
+      <c r="P34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N33">
-        <v>39600</v>
-      </c>
-      <c r="O33">
+      <c r="N35">
+        <v>15600</v>
+      </c>
+      <c r="O35">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N34">
-        <v>3000</v>
-      </c>
-      <c r="O34">
-        <v>1.0149999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="K35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N35">
-        <v>4800</v>
-      </c>
-      <c r="O35">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N36">
-        <v>50000</v>
-      </c>
-      <c r="O36">
-        <v>1.03</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N37">
-        <v>12000</v>
-      </c>
-      <c r="O37">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N38">
-        <v>36000</v>
-      </c>
-      <c r="O38">
-        <v>1.02</v>
-      </c>
-      <c r="P38">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>37</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N39">
-        <v>15600</v>
-      </c>
-      <c r="O39">
-        <v>1.02</v>
-      </c>
-      <c r="P39">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>42</v>
-      </c>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
         <v>15</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D37" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>